<commit_message>
add transport in excell and create setky
</commit_message>
<xml_diff>
--- a/sourse - копия.xlsx
+++ b/sourse - копия.xlsx
@@ -4,14 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="1080" windowWidth="24915" windowHeight="11625" tabRatio="892" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="1140" windowWidth="24915" windowHeight="11565" tabRatio="892" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Комбайн" sheetId="1" r:id="rId1"/>
     <sheet name="01.10" sheetId="71" r:id="rId2"/>
-    <sheet name="test" r:id="rId7" sheetId="72"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" refMode="R1C1"/>
 </workbook>
 </file>
 
@@ -2795,7 +2794,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="81">
   <si>
     <t>Держ №</t>
   </si>
@@ -3044,7 +3043,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3129,7 +3127,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3144,19 +3142,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442" rgb="4F81BD"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442" rgb="F79646"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" rgb="000000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3180,19 +3178,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442" rgb="EEECE1"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893" rgb="000000"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485" rgb="9BBB59"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3202,45 +3200,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill>
-        <fgColor rgb="FFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill>
-        <fgColor indexed="64"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="64"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill>
-        <fgColor rgb="BFBFBF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="BFBFBF"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="58">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -3566,273 +3527,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border/>
-    <border>
-      <top style="medium"/>
-    </border>
-    <border>
-      <top style="medium"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <top style="medium"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <top style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <top style="medium"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <top style="medium"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="medium"/>
-    </border>
-    <border>
-      <right style="medium"/>
-      <top style="medium"/>
-    </border>
-    <border>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <top style="medium"/>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium"/>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="medium"/>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium"/>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4011,6 +3711,18 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4023,49 +3735,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="57" xfId="0" applyFill="true" applyBorder="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="30" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="36" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="42" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="49" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="55" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4384,9 +4058,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="1" max="1" width="28" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -7092,18 +6766,18 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AH12" sqref="AH12"/>
-      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
+      <selection pane="bottomLeft" activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="32" width="14.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="32" width="23.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="32" width="11.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="32" width="25.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="32" width="22.140625" collapsed="true"/>
-    <col min="6" max="53" customWidth="true" style="32" width="3.28515625" collapsed="true"/>
-    <col min="54" max="16384" style="32" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.7109375" style="32" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.85546875" style="32" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.42578125" style="32" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.85546875" style="32" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.140625" style="32" customWidth="1" collapsed="1"/>
+    <col min="6" max="53" width="3.28515625" style="32" customWidth="1" collapsed="1"/>
+    <col min="54" max="16384" width="9.140625" style="32" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.25">
@@ -7115,63 +6789,63 @@
       </c>
     </row>
     <row r="2" spans="1:53" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="104" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="111"/>
+      <c r="B2" s="104"/>
       <c r="C2" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="112" t="s">
+      <c r="F2" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
-      <c r="J2" s="112"/>
-      <c r="K2" s="112"/>
-      <c r="L2" s="112"/>
-      <c r="M2" s="112"/>
-      <c r="N2" s="112"/>
-      <c r="O2" s="112"/>
-      <c r="P2" s="112"/>
-      <c r="Q2" s="112"/>
-      <c r="R2" s="112"/>
-      <c r="S2" s="112"/>
-      <c r="T2" s="112"/>
-      <c r="U2" s="112"/>
-      <c r="V2" s="112"/>
-      <c r="W2" s="112"/>
-      <c r="X2" s="112"/>
-      <c r="Y2" s="112"/>
-      <c r="Z2" s="112"/>
-      <c r="AA2" s="112"/>
-      <c r="AB2" s="112"/>
-      <c r="AC2" s="112"/>
-      <c r="AD2" s="112"/>
-      <c r="AE2" s="112"/>
-      <c r="AF2" s="112"/>
-      <c r="AG2" s="112"/>
-      <c r="AH2" s="112"/>
-      <c r="AI2" s="112"/>
-      <c r="AJ2" s="112"/>
-      <c r="AK2" s="112"/>
-      <c r="AL2" s="112"/>
-      <c r="AM2" s="112"/>
-      <c r="AN2" s="112"/>
-      <c r="AO2" s="112"/>
-      <c r="AP2" s="112"/>
-      <c r="AQ2" s="112"/>
-      <c r="AR2" s="112"/>
-      <c r="AS2" s="112"/>
-      <c r="AT2" s="112"/>
-      <c r="AU2" s="112"/>
-      <c r="AV2" s="112"/>
-      <c r="AW2" s="112"/>
-      <c r="AX2" s="112"/>
-      <c r="AY2" s="112"/>
-      <c r="AZ2" s="112"/>
-      <c r="BA2" s="112"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105"/>
+      <c r="P2" s="105"/>
+      <c r="Q2" s="105"/>
+      <c r="R2" s="105"/>
+      <c r="S2" s="105"/>
+      <c r="T2" s="105"/>
+      <c r="U2" s="105"/>
+      <c r="V2" s="105"/>
+      <c r="W2" s="105"/>
+      <c r="X2" s="105"/>
+      <c r="Y2" s="105"/>
+      <c r="Z2" s="105"/>
+      <c r="AA2" s="105"/>
+      <c r="AB2" s="105"/>
+      <c r="AC2" s="105"/>
+      <c r="AD2" s="105"/>
+      <c r="AE2" s="105"/>
+      <c r="AF2" s="105"/>
+      <c r="AG2" s="105"/>
+      <c r="AH2" s="105"/>
+      <c r="AI2" s="105"/>
+      <c r="AJ2" s="105"/>
+      <c r="AK2" s="105"/>
+      <c r="AL2" s="105"/>
+      <c r="AM2" s="105"/>
+      <c r="AN2" s="105"/>
+      <c r="AO2" s="105"/>
+      <c r="AP2" s="105"/>
+      <c r="AQ2" s="105"/>
+      <c r="AR2" s="105"/>
+      <c r="AS2" s="105"/>
+      <c r="AT2" s="105"/>
+      <c r="AU2" s="105"/>
+      <c r="AV2" s="105"/>
+      <c r="AW2" s="105"/>
+      <c r="AX2" s="105"/>
+      <c r="AY2" s="105"/>
+      <c r="AZ2" s="105"/>
+      <c r="BA2" s="105"/>
     </row>
     <row r="3" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
@@ -7189,102 +6863,102 @@
       <c r="E3" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="108">
+      <c r="F3" s="106">
         <v>7</v>
       </c>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108">
+      <c r="G3" s="106"/>
+      <c r="H3" s="106">
         <v>8</v>
       </c>
-      <c r="I3" s="108"/>
-      <c r="J3" s="108">
+      <c r="I3" s="106"/>
+      <c r="J3" s="106">
         <v>9</v>
       </c>
-      <c r="K3" s="108"/>
-      <c r="L3" s="108">
+      <c r="K3" s="106"/>
+      <c r="L3" s="106">
         <v>10</v>
       </c>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108">
+      <c r="M3" s="106"/>
+      <c r="N3" s="106">
         <v>11</v>
       </c>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108">
+      <c r="O3" s="106"/>
+      <c r="P3" s="106">
         <v>12</v>
       </c>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="108">
+      <c r="Q3" s="106"/>
+      <c r="R3" s="106">
         <v>13</v>
       </c>
-      <c r="S3" s="108"/>
-      <c r="T3" s="108">
+      <c r="S3" s="106"/>
+      <c r="T3" s="106">
         <v>14</v>
       </c>
-      <c r="U3" s="108"/>
-      <c r="V3" s="108">
+      <c r="U3" s="106"/>
+      <c r="V3" s="106">
         <v>15</v>
       </c>
-      <c r="W3" s="108"/>
-      <c r="X3" s="108">
+      <c r="W3" s="106"/>
+      <c r="X3" s="106">
         <v>16</v>
       </c>
-      <c r="Y3" s="108"/>
-      <c r="Z3" s="110">
+      <c r="Y3" s="106"/>
+      <c r="Z3" s="113">
         <v>17</v>
       </c>
-      <c r="AA3" s="110"/>
-      <c r="AB3" s="110">
+      <c r="AA3" s="113"/>
+      <c r="AB3" s="113">
         <v>18</v>
       </c>
-      <c r="AC3" s="110"/>
-      <c r="AD3" s="108">
+      <c r="AC3" s="113"/>
+      <c r="AD3" s="106">
         <v>19</v>
       </c>
-      <c r="AE3" s="108"/>
-      <c r="AF3" s="108">
+      <c r="AE3" s="106"/>
+      <c r="AF3" s="106">
         <v>20</v>
       </c>
-      <c r="AG3" s="108"/>
-      <c r="AH3" s="108">
+      <c r="AG3" s="106"/>
+      <c r="AH3" s="106">
         <v>21</v>
       </c>
-      <c r="AI3" s="108"/>
-      <c r="AJ3" s="108">
+      <c r="AI3" s="106"/>
+      <c r="AJ3" s="106">
         <v>22</v>
       </c>
-      <c r="AK3" s="108"/>
-      <c r="AL3" s="108">
+      <c r="AK3" s="106"/>
+      <c r="AL3" s="106">
         <v>23</v>
       </c>
-      <c r="AM3" s="108"/>
-      <c r="AN3" s="108">
+      <c r="AM3" s="106"/>
+      <c r="AN3" s="106">
         <v>24</v>
       </c>
-      <c r="AO3" s="108"/>
-      <c r="AP3" s="108">
+      <c r="AO3" s="106"/>
+      <c r="AP3" s="106">
         <v>1</v>
       </c>
-      <c r="AQ3" s="108"/>
-      <c r="AR3" s="108">
+      <c r="AQ3" s="106"/>
+      <c r="AR3" s="106">
         <v>2</v>
       </c>
-      <c r="AS3" s="108"/>
-      <c r="AT3" s="108">
+      <c r="AS3" s="106"/>
+      <c r="AT3" s="106">
         <v>3</v>
       </c>
-      <c r="AU3" s="108"/>
-      <c r="AV3" s="108">
+      <c r="AU3" s="106"/>
+      <c r="AV3" s="106">
         <v>4</v>
       </c>
-      <c r="AW3" s="108"/>
-      <c r="AX3" s="108">
+      <c r="AW3" s="106"/>
+      <c r="AX3" s="106">
         <v>5</v>
       </c>
-      <c r="AY3" s="108"/>
-      <c r="AZ3" s="108">
+      <c r="AY3" s="106"/>
+      <c r="AZ3" s="106">
         <v>6</v>
       </c>
-      <c r="BA3" s="113"/>
+      <c r="BA3" s="107"/>
     </row>
     <row r="4" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="94" t="s">
@@ -7344,7 +7018,7 @@
       <c r="BA4" s="97"/>
     </row>
     <row r="5" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="104" t="s">
+      <c r="A5" s="108" t="s">
         <v>72</v>
       </c>
       <c r="B5" s="59" t="s">
@@ -7411,7 +7085,7 @@
       <c r="BA5" s="50"/>
     </row>
     <row r="6" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="107"/>
+      <c r="A6" s="111"/>
       <c r="B6" s="34" t="s">
         <v>62</v>
       </c>
@@ -7478,7 +7152,7 @@
       <c r="BA6" s="51"/>
     </row>
     <row r="7" spans="1:53" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="105"/>
+      <c r="A7" s="109"/>
       <c r="B7" s="40" t="s">
         <v>62</v>
       </c>
@@ -7543,7 +7217,7 @@
       <c r="BA7" s="57"/>
     </row>
     <row r="8" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="106" t="s">
+      <c r="A8" s="110" t="s">
         <v>67</v>
       </c>
       <c r="B8" s="38" t="s">
@@ -7610,7 +7284,7 @@
       <c r="BA8" s="74"/>
     </row>
     <row r="9" spans="1:53" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="109"/>
+      <c r="A9" s="112"/>
       <c r="B9" s="87" t="s">
         <v>32</v>
       </c>
@@ -7673,7 +7347,7 @@
       <c r="BA9" s="70"/>
     </row>
     <row r="10" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="104" t="s">
+      <c r="A10" s="108" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="59" t="s">
@@ -7738,7 +7412,7 @@
       <c r="BA10" s="50"/>
     </row>
     <row r="11" spans="1:53" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="105"/>
+      <c r="A11" s="109"/>
       <c r="B11" s="40" t="s">
         <v>69</v>
       </c>
@@ -7797,7 +7471,7 @@
       <c r="BA11" s="57"/>
     </row>
     <row r="12" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="106" t="s">
+      <c r="A12" s="110" t="s">
         <v>70</v>
       </c>
       <c r="B12" s="58" t="s">
@@ -7866,7 +7540,7 @@
       <c r="BA12" s="71"/>
     </row>
     <row r="13" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="107"/>
+      <c r="A13" s="111"/>
       <c r="B13" s="34" t="s">
         <v>24</v>
       </c>
@@ -7933,7 +7607,7 @@
       <c r="BA13" s="51"/>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A14" s="107"/>
+      <c r="A14" s="111"/>
       <c r="B14" s="34" t="s">
         <v>24</v>
       </c>
@@ -7998,7 +7672,7 @@
       <c r="BA14" s="51"/>
     </row>
     <row r="15" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A15" s="107"/>
+      <c r="A15" s="111"/>
       <c r="B15" s="34" t="s">
         <v>24</v>
       </c>
@@ -8061,7 +7735,7 @@
       <c r="BA15" s="51"/>
     </row>
     <row r="16" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="107"/>
+      <c r="A16" s="111"/>
       <c r="B16" s="34" t="s">
         <v>45</v>
       </c>
@@ -8122,7 +7796,7 @@
       <c r="BA16" s="51"/>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A17" s="107"/>
+      <c r="A17" s="111"/>
       <c r="B17" s="34" t="s">
         <v>24</v>
       </c>
@@ -8187,7 +7861,7 @@
       <c r="BA17" s="51"/>
     </row>
     <row r="18" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="105"/>
+      <c r="A18" s="109"/>
       <c r="B18" s="40" t="s">
         <v>24</v>
       </c>
@@ -8252,7 +7926,7 @@
       <c r="BA18" s="57"/>
     </row>
     <row r="19" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="106" t="s">
+      <c r="A19" s="110" t="s">
         <v>71</v>
       </c>
       <c r="B19" s="38" t="s">
@@ -8319,7 +7993,7 @@
       <c r="BA19" s="71"/>
     </row>
     <row r="20" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A20" s="107"/>
+      <c r="A20" s="111"/>
       <c r="B20" s="41" t="s">
         <v>32</v>
       </c>
@@ -8382,7 +8056,7 @@
       <c r="BA20" s="51"/>
     </row>
     <row r="21" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="105"/>
+      <c r="A21" s="109"/>
       <c r="B21" s="60" t="s">
         <v>32</v>
       </c>
@@ -8905,21 +8579,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:BA2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="AX3:AY3"/>
-    <mergeCell ref="AZ3:BA3"/>
-    <mergeCell ref="AN3:AO3"/>
-    <mergeCell ref="AP3:AQ3"/>
-    <mergeCell ref="AR3:AS3"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A18"/>
     <mergeCell ref="A19:A21"/>
@@ -8936,197 +8595,8 @@
     <mergeCell ref="AB3:AC3"/>
     <mergeCell ref="AD3:AE3"/>
     <mergeCell ref="AF3:AG3"/>
-  </mergeCells>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="true"/>
-    <col min="2" max="2" width="23.85546875" customWidth="true"/>
-    <col min="3" max="3" width="11.42578125" customWidth="true"/>
-    <col min="4" max="4" width="25.85546875" customWidth="true"/>
-    <col min="5" max="5" width="22.140625" customWidth="true"/>
-    <col min="6" max="6" width="3.28515625" customWidth="true"/>
-    <col min="7" max="7" width="3.28515625" customWidth="true"/>
-    <col min="8" max="8" width="3.28515625" customWidth="true"/>
-    <col min="9" max="9" width="3.28515625" customWidth="true"/>
-    <col min="10" max="10" width="3.28515625" customWidth="true"/>
-    <col min="11" max="11" width="3.28515625" customWidth="true"/>
-    <col min="12" max="12" width="3.28515625" customWidth="true"/>
-    <col min="13" max="13" width="3.28515625" customWidth="true"/>
-    <col min="14" max="14" width="3.28515625" customWidth="true"/>
-    <col min="15" max="15" width="3.28515625" customWidth="true"/>
-    <col min="16" max="16" width="3.28515625" customWidth="true"/>
-    <col min="17" max="17" width="3.28515625" customWidth="true"/>
-    <col min="18" max="18" width="3.28515625" customWidth="true"/>
-    <col min="19" max="19" width="3.28515625" customWidth="true"/>
-    <col min="20" max="20" width="3.28515625" customWidth="true"/>
-    <col min="21" max="21" width="3.28515625" customWidth="true"/>
-    <col min="22" max="22" width="3.28515625" customWidth="true"/>
-    <col min="23" max="23" width="3.28515625" customWidth="true"/>
-    <col min="24" max="24" width="3.28515625" customWidth="true"/>
-    <col min="25" max="25" width="3.28515625" customWidth="true"/>
-    <col min="26" max="26" width="3.28515625" customWidth="true"/>
-    <col min="27" max="27" width="3.28515625" customWidth="true"/>
-    <col min="28" max="28" width="3.28515625" customWidth="true"/>
-    <col min="29" max="29" width="3.28515625" customWidth="true"/>
-    <col min="30" max="30" width="3.28515625" customWidth="true"/>
-    <col min="31" max="31" width="3.28515625" customWidth="true"/>
-    <col min="32" max="32" width="3.28515625" customWidth="true"/>
-    <col min="33" max="33" width="3.28515625" customWidth="true"/>
-    <col min="34" max="34" width="3.28515625" customWidth="true"/>
-    <col min="35" max="35" width="3.28515625" customWidth="true"/>
-    <col min="36" max="36" width="3.28515625" customWidth="true"/>
-    <col min="37" max="37" width="3.28515625" customWidth="true"/>
-    <col min="38" max="38" width="3.28515625" customWidth="true"/>
-    <col min="39" max="39" width="3.28515625" customWidth="true"/>
-    <col min="40" max="40" width="3.28515625" customWidth="true"/>
-    <col min="41" max="41" width="3.28515625" customWidth="true"/>
-    <col min="42" max="42" width="3.28515625" customWidth="true"/>
-    <col min="43" max="43" width="3.28515625" customWidth="true"/>
-    <col min="44" max="44" width="3.28515625" customWidth="true"/>
-    <col min="45" max="45" width="3.28515625" customWidth="true"/>
-    <col min="46" max="46" width="3.28515625" customWidth="true"/>
-    <col min="47" max="47" width="3.28515625" customWidth="true"/>
-    <col min="48" max="48" width="3.28515625" customWidth="true"/>
-    <col min="49" max="49" width="3.28515625" customWidth="true"/>
-    <col min="50" max="50" width="3.28515625" customWidth="true"/>
-    <col min="51" max="51" width="3.28515625" customWidth="true"/>
-    <col min="52" max="52" width="3.28515625" customWidth="true"/>
-    <col min="53" max="53" width="3.28515625" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="2">
-      <c r="A2" t="s" s="114">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="115">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s" s="115">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s" s="115">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s" s="115">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s" s="115">
-        <v>20</v>
-      </c>
-      <c r="F3" t="n" s="115">
-        <v>7.0</v>
-      </c>
-      <c r="G3" s="120"/>
-      <c r="H3" t="n" s="115">
-        <v>8.0</v>
-      </c>
-      <c r="I3" s="120"/>
-      <c r="J3" t="n" s="115">
-        <v>9.0</v>
-      </c>
-      <c r="K3" s="120"/>
-      <c r="L3" t="n" s="115">
-        <v>10.0</v>
-      </c>
-      <c r="M3" s="120"/>
-      <c r="N3" t="n" s="115">
-        <v>11.0</v>
-      </c>
-      <c r="O3" s="120"/>
-      <c r="P3" t="n" s="115">
-        <v>12.0</v>
-      </c>
-      <c r="Q3" s="120"/>
-      <c r="R3" t="n" s="115">
-        <v>13.0</v>
-      </c>
-      <c r="S3" s="120"/>
-      <c r="T3" t="n" s="115">
-        <v>14.0</v>
-      </c>
-      <c r="U3" s="120"/>
-      <c r="V3" t="n" s="115">
-        <v>15.0</v>
-      </c>
-      <c r="W3" s="120"/>
-      <c r="X3" t="n" s="115">
-        <v>16.0</v>
-      </c>
-      <c r="Y3" s="120"/>
-      <c r="Z3" t="n" s="115">
-        <v>17.0</v>
-      </c>
-      <c r="AA3" s="120"/>
-      <c r="AB3" t="n" s="115">
-        <v>18.0</v>
-      </c>
-      <c r="AC3" s="120"/>
-      <c r="AD3" t="n" s="115">
-        <v>19.0</v>
-      </c>
-      <c r="AE3" s="120"/>
-      <c r="AF3" t="n" s="115">
-        <v>20.0</v>
-      </c>
-      <c r="AG3" s="120"/>
-      <c r="AH3" t="n" s="115">
-        <v>21.0</v>
-      </c>
-      <c r="AI3" s="120"/>
-      <c r="AJ3" t="n" s="115">
-        <v>22.0</v>
-      </c>
-      <c r="AK3" s="120"/>
-      <c r="AL3" t="n" s="115">
-        <v>23.0</v>
-      </c>
-      <c r="AM3" s="120"/>
-      <c r="AN3" t="n" s="115">
-        <v>24.0</v>
-      </c>
-      <c r="AO3" s="120"/>
-      <c r="AP3" t="n" s="115">
-        <v>1.0</v>
-      </c>
-      <c r="AQ3" s="120"/>
-      <c r="AR3" t="n" s="115">
-        <v>2.0</v>
-      </c>
-      <c r="AS3" s="120"/>
-      <c r="AT3" t="n" s="115">
-        <v>3.0</v>
-      </c>
-      <c r="AU3" s="120"/>
-      <c r="AV3" t="n" s="115">
-        <v>4.0</v>
-      </c>
-      <c r="AW3" s="120"/>
-      <c r="AX3" t="n" s="115">
-        <v>5.0</v>
-      </c>
-      <c r="AY3" s="120"/>
-      <c r="AZ3" t="n" s="115">
-        <v>6.0</v>
-      </c>
-      <c r="BA3" s="120"/>
-    </row>
-  </sheetData>
-  <mergeCells>
     <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:BA2"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
@@ -9135,23 +8605,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="R3:S3"/>
     <mergeCell ref="T3:U3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AJ3:AK3"/>
-    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="AX3:AY3"/>
+    <mergeCell ref="AZ3:BA3"/>
     <mergeCell ref="AN3:AO3"/>
     <mergeCell ref="AP3:AQ3"/>
     <mergeCell ref="AR3:AS3"/>
-    <mergeCell ref="AT3:AU3"/>
-    <mergeCell ref="AV3:AW3"/>
-    <mergeCell ref="AX3:AY3"/>
-    <mergeCell ref="AZ3:BA3"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
I must debug NullPointerException in StartTime/EndTime reports
</commit_message>
<xml_diff>
--- a/sourse - копия.xlsx
+++ b/sourse - копия.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet name="Комбайн" sheetId="1" r:id="rId1"/>
     <sheet name="01.10" sheetId="71" r:id="rId2"/>
-    <sheet name="test" r:id="rId7" sheetId="72"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -2795,7 +2794,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="81">
   <si>
     <t>Держ №</t>
   </si>
@@ -3039,84 +3038,11 @@
   <si>
     <t>test version</t>
   </si>
-  <si>
-    <t>John Deere-S6901_09039BI</t>
-  </si>
-  <si>
-    <t>Хмільниця_Тест</t>
-  </si>
-  <si>
-    <t>Збирання кукурудзи_Тест</t>
-  </si>
-  <si>
-    <t>Півень В.М.</t>
-  </si>
-  <si>
-    <t>John Deere-S9880_11270CB</t>
-  </si>
-  <si>
-    <t>Коробко В.М.</t>
-  </si>
-  <si>
-    <t>John Deere-S9880_11271CB</t>
-  </si>
-  <si>
-    <t>John Deere-S9880_11273CB</t>
-  </si>
-  <si>
-    <t>Василенко А.П.</t>
-  </si>
-  <si>
-    <t>John Deere-S9880_11269CB</t>
-  </si>
-  <si>
-    <t>Скляров О.В.</t>
-  </si>
-  <si>
-    <t>John Deere-S9880_11272CB</t>
-  </si>
-  <si>
-    <t>Скляров М.В</t>
-  </si>
-  <si>
-    <t>Палессе 16318СВ</t>
-  </si>
-  <si>
-    <t>16318</t>
-  </si>
-  <si>
-    <t xml:space="preserve">най-н Clas 22491АС </t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Нью-Холонд Новий </t>
-  </si>
-  <si>
-    <t>б/н</t>
-  </si>
-  <si>
-    <t>Иллюшко С.Л</t>
-  </si>
-  <si>
-    <t>най-й Джон Дір 18143 2105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">най-н CLAS 2249АС (міні) </t>
-  </si>
-  <si>
-    <t>най Case 07156 Данилов Ю.М. 2102</t>
-  </si>
-  <si>
-    <t>най Сase 07157 Косенко О.І. 1750</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3201,7 +3127,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3216,19 +3142,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442" rgb="4F81BD"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442" rgb="F79646"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" rgb="000000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3252,19 +3178,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442" rgb="EEECE1"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893" rgb="000000"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485" rgb="9BBB59"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3274,45 +3200,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill>
-        <fgColor rgb="FFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill>
-        <fgColor indexed="64"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="64"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill>
-        <fgColor rgb="BFBFBF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="BFBFBF"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="83">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -3638,481 +3527,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border/>
-    <border>
-      <top style="medium"/>
-    </border>
-    <border>
-      <top style="medium"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <top style="medium"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <top style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <top style="medium"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <top style="medium"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="medium"/>
-    </border>
-    <border>
-      <right style="medium"/>
-      <top style="medium"/>
-    </border>
-    <border>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <top style="medium"/>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium"/>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="8"/>
-      </left>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="medium"/>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium"/>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right style="medium">
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <top style="thin"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="thin"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <top style="thin"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="thin"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin"/>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin"/>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4320,48 +3740,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="57" xfId="0" applyFill="true" applyBorder="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="30" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="36" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="42" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="49" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="55" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="62" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="68" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="74" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="82" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4680,9 +4058,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -7393,13 +6771,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="32" width="14.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="32" width="23.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="32" width="11.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="32" width="25.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="32" width="22.140625" collapsed="true"/>
-    <col min="6" max="53" customWidth="true" style="32" width="3.28515625" collapsed="true"/>
-    <col min="54" max="16384" style="32" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.7109375" style="32" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="32" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="32" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="32" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="32" customWidth="1"/>
+    <col min="6" max="53" width="3.28515625" style="32" customWidth="1"/>
+    <col min="54" max="16384" width="9.140625" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.25">
@@ -9237,1117 +8615,4 @@
   <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="true"/>
-    <col min="2" max="2" width="23.85546875" customWidth="true"/>
-    <col min="3" max="3" width="11.42578125" customWidth="true"/>
-    <col min="4" max="4" width="25.85546875" customWidth="true"/>
-    <col min="5" max="5" width="22.140625" customWidth="true"/>
-    <col min="6" max="6" width="3.28515625" customWidth="true"/>
-    <col min="7" max="7" width="3.28515625" customWidth="true"/>
-    <col min="8" max="8" width="3.28515625" customWidth="true"/>
-    <col min="9" max="9" width="3.28515625" customWidth="true"/>
-    <col min="10" max="10" width="3.28515625" customWidth="true"/>
-    <col min="11" max="11" width="3.28515625" customWidth="true"/>
-    <col min="12" max="12" width="3.28515625" customWidth="true"/>
-    <col min="13" max="13" width="3.28515625" customWidth="true"/>
-    <col min="14" max="14" width="3.28515625" customWidth="true"/>
-    <col min="15" max="15" width="3.28515625" customWidth="true"/>
-    <col min="16" max="16" width="3.28515625" customWidth="true"/>
-    <col min="17" max="17" width="3.28515625" customWidth="true"/>
-    <col min="18" max="18" width="3.28515625" customWidth="true"/>
-    <col min="19" max="19" width="3.28515625" customWidth="true"/>
-    <col min="20" max="20" width="3.28515625" customWidth="true"/>
-    <col min="21" max="21" width="3.28515625" customWidth="true"/>
-    <col min="22" max="22" width="3.28515625" customWidth="true"/>
-    <col min="23" max="23" width="3.28515625" customWidth="true"/>
-    <col min="24" max="24" width="3.28515625" customWidth="true"/>
-    <col min="25" max="25" width="3.28515625" customWidth="true"/>
-    <col min="26" max="26" width="3.28515625" customWidth="true"/>
-    <col min="27" max="27" width="3.28515625" customWidth="true"/>
-    <col min="28" max="28" width="3.28515625" customWidth="true"/>
-    <col min="29" max="29" width="3.28515625" customWidth="true"/>
-    <col min="30" max="30" width="3.28515625" customWidth="true"/>
-    <col min="31" max="31" width="3.28515625" customWidth="true"/>
-    <col min="32" max="32" width="3.28515625" customWidth="true"/>
-    <col min="33" max="33" width="3.28515625" customWidth="true"/>
-    <col min="34" max="34" width="3.28515625" customWidth="true"/>
-    <col min="35" max="35" width="3.28515625" customWidth="true"/>
-    <col min="36" max="36" width="3.28515625" customWidth="true"/>
-    <col min="37" max="37" width="3.28515625" customWidth="true"/>
-    <col min="38" max="38" width="3.28515625" customWidth="true"/>
-    <col min="39" max="39" width="3.28515625" customWidth="true"/>
-    <col min="40" max="40" width="3.28515625" customWidth="true"/>
-    <col min="41" max="41" width="3.28515625" customWidth="true"/>
-    <col min="42" max="42" width="3.28515625" customWidth="true"/>
-    <col min="43" max="43" width="3.28515625" customWidth="true"/>
-    <col min="44" max="44" width="3.28515625" customWidth="true"/>
-    <col min="45" max="45" width="3.28515625" customWidth="true"/>
-    <col min="46" max="46" width="3.28515625" customWidth="true"/>
-    <col min="47" max="47" width="3.28515625" customWidth="true"/>
-    <col min="48" max="48" width="3.28515625" customWidth="true"/>
-    <col min="49" max="49" width="3.28515625" customWidth="true"/>
-    <col min="50" max="50" width="3.28515625" customWidth="true"/>
-    <col min="51" max="51" width="3.28515625" customWidth="true"/>
-    <col min="52" max="52" width="3.28515625" customWidth="true"/>
-    <col min="53" max="53" width="3.28515625" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="2">
-      <c r="A2" t="s" s="114">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="115">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s" s="115">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s" s="115">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s" s="115">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s" s="115">
-        <v>20</v>
-      </c>
-      <c r="F3" t="n" s="115">
-        <v>7.0</v>
-      </c>
-      <c r="G3" s="120"/>
-      <c r="H3" t="n" s="115">
-        <v>8.0</v>
-      </c>
-      <c r="I3" s="120"/>
-      <c r="J3" t="n" s="115">
-        <v>9.0</v>
-      </c>
-      <c r="K3" s="120"/>
-      <c r="L3" t="n" s="115">
-        <v>10.0</v>
-      </c>
-      <c r="M3" s="120"/>
-      <c r="N3" t="n" s="115">
-        <v>11.0</v>
-      </c>
-      <c r="O3" s="120"/>
-      <c r="P3" t="n" s="115">
-        <v>12.0</v>
-      </c>
-      <c r="Q3" s="120"/>
-      <c r="R3" t="n" s="115">
-        <v>13.0</v>
-      </c>
-      <c r="S3" s="120"/>
-      <c r="T3" t="n" s="115">
-        <v>14.0</v>
-      </c>
-      <c r="U3" s="120"/>
-      <c r="V3" t="n" s="115">
-        <v>15.0</v>
-      </c>
-      <c r="W3" s="120"/>
-      <c r="X3" t="n" s="115">
-        <v>16.0</v>
-      </c>
-      <c r="Y3" s="120"/>
-      <c r="Z3" t="n" s="115">
-        <v>17.0</v>
-      </c>
-      <c r="AA3" s="120"/>
-      <c r="AB3" t="n" s="115">
-        <v>18.0</v>
-      </c>
-      <c r="AC3" s="120"/>
-      <c r="AD3" t="n" s="115">
-        <v>19.0</v>
-      </c>
-      <c r="AE3" s="120"/>
-      <c r="AF3" t="n" s="115">
-        <v>20.0</v>
-      </c>
-      <c r="AG3" s="120"/>
-      <c r="AH3" t="n" s="115">
-        <v>21.0</v>
-      </c>
-      <c r="AI3" s="120"/>
-      <c r="AJ3" t="n" s="115">
-        <v>22.0</v>
-      </c>
-      <c r="AK3" s="120"/>
-      <c r="AL3" t="n" s="115">
-        <v>23.0</v>
-      </c>
-      <c r="AM3" s="120"/>
-      <c r="AN3" t="n" s="115">
-        <v>24.0</v>
-      </c>
-      <c r="AO3" s="120"/>
-      <c r="AP3" t="n" s="115">
-        <v>1.0</v>
-      </c>
-      <c r="AQ3" s="120"/>
-      <c r="AR3" t="n" s="115">
-        <v>2.0</v>
-      </c>
-      <c r="AS3" s="120"/>
-      <c r="AT3" t="n" s="115">
-        <v>3.0</v>
-      </c>
-      <c r="AU3" s="120"/>
-      <c r="AV3" t="n" s="115">
-        <v>4.0</v>
-      </c>
-      <c r="AW3" s="120"/>
-      <c r="AX3" t="n" s="115">
-        <v>5.0</v>
-      </c>
-      <c r="AY3" s="120"/>
-      <c r="AZ3" t="n" s="115">
-        <v>6.0</v>
-      </c>
-      <c r="BA3" s="120"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="124"/>
-      <c r="B4" s="124"/>
-      <c r="C4" s="124"/>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="124"/>
-      <c r="H4" s="124"/>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
-      <c r="K4" s="124"/>
-      <c r="L4" s="124"/>
-      <c r="M4" s="124"/>
-      <c r="N4" s="124"/>
-      <c r="O4" s="124"/>
-      <c r="P4" s="124"/>
-      <c r="Q4" s="124"/>
-      <c r="R4" s="124"/>
-      <c r="S4" s="124"/>
-      <c r="T4" s="124"/>
-      <c r="U4"/>
-      <c r="V4" s="124"/>
-      <c r="W4" s="124"/>
-      <c r="X4" s="124"/>
-      <c r="Y4" s="124"/>
-      <c r="Z4" s="124"/>
-      <c r="AA4" s="124"/>
-      <c r="AB4" s="124"/>
-      <c r="AC4" s="124"/>
-      <c r="AD4" s="124"/>
-      <c r="AE4" s="124"/>
-      <c r="AF4" s="124"/>
-      <c r="AG4" s="124"/>
-      <c r="AH4" s="124"/>
-      <c r="AI4" s="124"/>
-      <c r="AJ4" s="124"/>
-      <c r="AK4" s="124"/>
-      <c r="AL4" s="124"/>
-      <c r="AM4" s="124"/>
-      <c r="AN4" s="124"/>
-      <c r="AO4" s="124"/>
-      <c r="AP4" s="124"/>
-      <c r="AQ4" s="124"/>
-      <c r="AR4" s="124"/>
-      <c r="AS4" s="124"/>
-      <c r="AT4" s="124"/>
-      <c r="AU4" s="124"/>
-      <c r="AV4" s="124"/>
-      <c r="AW4" s="124"/>
-      <c r="AX4" s="124"/>
-      <c r="AY4" s="124"/>
-      <c r="AZ4" s="124"/>
-      <c r="BA4" s="124"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="124">
-        <v>82</v>
-      </c>
-      <c r="B5" t="s" s="124">
-        <v>81</v>
-      </c>
-      <c r="C5" t="s" s="124">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s" s="124">
-        <v>83</v>
-      </c>
-      <c r="E5" t="s" s="124">
-        <v>84</v>
-      </c>
-      <c r="F5" s="124"/>
-      <c r="G5" s="124"/>
-      <c r="H5" s="124"/>
-      <c r="I5" s="124"/>
-      <c r="J5" s="124"/>
-      <c r="K5" s="124"/>
-      <c r="L5" s="124"/>
-      <c r="M5" s="124"/>
-      <c r="N5" s="124"/>
-      <c r="O5" s="124"/>
-      <c r="P5" s="124"/>
-      <c r="Q5" s="124"/>
-      <c r="R5" s="124"/>
-      <c r="S5" s="124"/>
-      <c r="T5" s="124"/>
-      <c r="U5" s="124"/>
-      <c r="V5" s="124"/>
-      <c r="W5" s="124"/>
-      <c r="X5" s="124"/>
-      <c r="Y5" s="124"/>
-      <c r="Z5" s="124"/>
-      <c r="AA5" s="124"/>
-      <c r="AB5" s="124"/>
-      <c r="AC5" s="124"/>
-      <c r="AD5" s="124"/>
-      <c r="AE5" s="124"/>
-      <c r="AF5" s="124"/>
-      <c r="AG5" s="124"/>
-      <c r="AH5" s="124"/>
-      <c r="AI5" s="124"/>
-      <c r="AJ5" s="124"/>
-      <c r="AK5" s="124"/>
-      <c r="AL5" s="124"/>
-      <c r="AM5" s="124"/>
-      <c r="AN5" s="124"/>
-      <c r="AO5" s="124"/>
-      <c r="AP5" s="124"/>
-      <c r="AQ5" s="124"/>
-      <c r="AR5" s="124"/>
-      <c r="AS5" s="124"/>
-      <c r="AT5" s="124"/>
-      <c r="AU5" s="124"/>
-      <c r="AV5" s="124"/>
-      <c r="AW5" s="124"/>
-      <c r="AX5" s="124"/>
-      <c r="AY5" s="124"/>
-      <c r="AZ5" s="124"/>
-      <c r="BA5" s="124"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="124">
-        <v>82</v>
-      </c>
-      <c r="B6" t="s" s="124">
-        <v>85</v>
-      </c>
-      <c r="C6" t="s" s="124">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s" s="124">
-        <v>83</v>
-      </c>
-      <c r="E6" t="s" s="124">
-        <v>86</v>
-      </c>
-      <c r="F6" s="124"/>
-      <c r="G6" s="124"/>
-      <c r="H6" s="124"/>
-      <c r="I6" s="124"/>
-      <c r="J6" s="124"/>
-      <c r="K6" s="124"/>
-      <c r="L6" s="124"/>
-      <c r="M6" s="124"/>
-      <c r="N6" s="124"/>
-      <c r="O6" s="124"/>
-      <c r="P6" s="124"/>
-      <c r="Q6" s="124"/>
-      <c r="R6" s="124"/>
-      <c r="S6" s="124"/>
-      <c r="T6" s="124"/>
-      <c r="U6" s="124"/>
-      <c r="V6" s="124"/>
-      <c r="W6" s="124"/>
-      <c r="X6" s="124"/>
-      <c r="Y6" s="124"/>
-      <c r="Z6" s="124"/>
-      <c r="AA6" s="124"/>
-      <c r="AB6" s="124"/>
-      <c r="AC6" s="124"/>
-      <c r="AD6" s="124"/>
-      <c r="AE6" s="124"/>
-      <c r="AF6" s="124"/>
-      <c r="AG6" s="124"/>
-      <c r="AH6" s="124"/>
-      <c r="AI6" s="124"/>
-      <c r="AJ6" s="124"/>
-      <c r="AK6" s="124"/>
-      <c r="AL6" s="124"/>
-      <c r="AM6" s="124"/>
-      <c r="AN6" s="124"/>
-      <c r="AO6" s="124"/>
-      <c r="AP6" s="124"/>
-      <c r="AQ6" s="124"/>
-      <c r="AR6" s="124"/>
-      <c r="AS6" s="124"/>
-      <c r="AT6" s="124"/>
-      <c r="AU6" s="124"/>
-      <c r="AV6" s="124"/>
-      <c r="AW6" s="124"/>
-      <c r="AX6" s="124"/>
-      <c r="AY6" s="124"/>
-      <c r="AZ6" s="124"/>
-      <c r="BA6" s="124"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="124">
-        <v>82</v>
-      </c>
-      <c r="B7" t="s" s="124">
-        <v>87</v>
-      </c>
-      <c r="C7" t="s" s="124">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s" s="124">
-        <v>83</v>
-      </c>
-      <c r="E7" t="s" s="124">
-        <v>51</v>
-      </c>
-      <c r="F7" s="124"/>
-      <c r="G7" s="124"/>
-      <c r="H7" s="124"/>
-      <c r="I7" s="124"/>
-      <c r="J7" s="124"/>
-      <c r="K7" s="124"/>
-      <c r="L7" s="124"/>
-      <c r="M7" s="124"/>
-      <c r="N7" s="124"/>
-      <c r="O7" s="124"/>
-      <c r="P7" s="124"/>
-      <c r="Q7" s="124"/>
-      <c r="R7" s="124"/>
-      <c r="S7" s="124"/>
-      <c r="T7" s="124"/>
-      <c r="U7" s="124"/>
-      <c r="V7" s="124"/>
-      <c r="W7" s="124"/>
-      <c r="X7" s="124"/>
-      <c r="Y7" s="124"/>
-      <c r="Z7" s="124"/>
-      <c r="AA7" s="124"/>
-      <c r="AB7" s="124"/>
-      <c r="AC7" s="124"/>
-      <c r="AD7" s="124"/>
-      <c r="AE7" s="124"/>
-      <c r="AF7" s="124"/>
-      <c r="AG7" s="124"/>
-      <c r="AH7" s="124"/>
-      <c r="AI7" s="124"/>
-      <c r="AJ7" s="124"/>
-      <c r="AK7" s="124"/>
-      <c r="AL7" s="124"/>
-      <c r="AM7" s="124"/>
-      <c r="AN7" s="124"/>
-      <c r="AO7" s="124"/>
-      <c r="AP7" s="124"/>
-      <c r="AQ7" s="124"/>
-      <c r="AR7" s="124"/>
-      <c r="AS7" s="124"/>
-      <c r="AT7" s="124"/>
-      <c r="AU7" s="124"/>
-      <c r="AV7" s="124"/>
-      <c r="AW7" s="124"/>
-      <c r="AX7" s="124"/>
-      <c r="AY7" s="124"/>
-      <c r="AZ7" s="124"/>
-      <c r="BA7" s="124"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="124">
-        <v>82</v>
-      </c>
-      <c r="B8" t="s" s="124">
-        <v>88</v>
-      </c>
-      <c r="C8" t="s" s="124">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s" s="124">
-        <v>83</v>
-      </c>
-      <c r="E8" t="s" s="124">
-        <v>89</v>
-      </c>
-      <c r="F8" s="124"/>
-      <c r="G8" s="124"/>
-      <c r="H8" s="124"/>
-      <c r="I8" s="124"/>
-      <c r="J8" s="124"/>
-      <c r="K8" s="124"/>
-      <c r="L8" s="124"/>
-      <c r="M8" s="124"/>
-      <c r="N8" s="124"/>
-      <c r="O8" s="124"/>
-      <c r="P8" s="124"/>
-      <c r="Q8" s="124"/>
-      <c r="R8" s="124"/>
-      <c r="S8" s="124"/>
-      <c r="T8" s="124"/>
-      <c r="U8" s="124"/>
-      <c r="V8" s="124"/>
-      <c r="W8" s="124"/>
-      <c r="X8" s="124"/>
-      <c r="Y8" s="124"/>
-      <c r="Z8" s="124"/>
-      <c r="AA8" s="124"/>
-      <c r="AB8" s="124"/>
-      <c r="AC8" s="124"/>
-      <c r="AD8" s="124"/>
-      <c r="AE8" s="124"/>
-      <c r="AF8" s="124"/>
-      <c r="AG8" s="124"/>
-      <c r="AH8" s="124"/>
-      <c r="AI8" s="124"/>
-      <c r="AJ8" s="124"/>
-      <c r="AK8" s="124"/>
-      <c r="AL8" s="124"/>
-      <c r="AM8" s="124"/>
-      <c r="AN8" s="124"/>
-      <c r="AO8" s="124"/>
-      <c r="AP8" s="124"/>
-      <c r="AQ8" s="124"/>
-      <c r="AR8" s="124"/>
-      <c r="AS8" s="124"/>
-      <c r="AT8" s="124"/>
-      <c r="AU8" s="124"/>
-      <c r="AV8" s="124"/>
-      <c r="AW8" s="124"/>
-      <c r="AX8" s="124"/>
-      <c r="AY8" s="124"/>
-      <c r="AZ8" s="124"/>
-      <c r="BA8" s="124"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="124">
-        <v>82</v>
-      </c>
-      <c r="B9" t="s" s="124">
-        <v>90</v>
-      </c>
-      <c r="C9" t="s" s="124">
-        <v>30</v>
-      </c>
-      <c r="D9" t="s" s="124">
-        <v>83</v>
-      </c>
-      <c r="E9" t="s" s="124">
-        <v>91</v>
-      </c>
-      <c r="F9" s="124"/>
-      <c r="G9" s="124"/>
-      <c r="H9" s="124"/>
-      <c r="I9" s="124"/>
-      <c r="J9" s="124"/>
-      <c r="K9" s="124"/>
-      <c r="L9" s="124"/>
-      <c r="M9" s="124"/>
-      <c r="N9" s="124"/>
-      <c r="O9" s="124"/>
-      <c r="P9" s="124"/>
-      <c r="Q9" s="124"/>
-      <c r="R9" s="124"/>
-      <c r="S9" s="124"/>
-      <c r="T9" s="124"/>
-      <c r="U9" s="124"/>
-      <c r="V9" s="124"/>
-      <c r="W9" s="124"/>
-      <c r="X9" s="124"/>
-      <c r="Y9" s="124"/>
-      <c r="Z9" s="124"/>
-      <c r="AA9" s="124"/>
-      <c r="AB9" s="124"/>
-      <c r="AC9" s="124"/>
-      <c r="AD9" s="124"/>
-      <c r="AE9" s="124"/>
-      <c r="AF9" s="124"/>
-      <c r="AG9" s="124"/>
-      <c r="AH9" s="124"/>
-      <c r="AI9" s="124"/>
-      <c r="AJ9" s="124"/>
-      <c r="AK9" s="124"/>
-      <c r="AL9" s="124"/>
-      <c r="AM9" s="124"/>
-      <c r="AN9" s="124"/>
-      <c r="AO9" s="124"/>
-      <c r="AP9" s="124"/>
-      <c r="AQ9" s="124"/>
-      <c r="AR9" s="124"/>
-      <c r="AS9" s="124"/>
-      <c r="AT9" s="124"/>
-      <c r="AU9" s="124"/>
-      <c r="AV9" s="124"/>
-      <c r="AW9" s="124"/>
-      <c r="AX9" s="124"/>
-      <c r="AY9" s="124"/>
-      <c r="AZ9" s="124"/>
-      <c r="BA9" s="124"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="124">
-        <v>82</v>
-      </c>
-      <c r="B10" t="s" s="124">
-        <v>92</v>
-      </c>
-      <c r="C10" t="s" s="124">
-        <v>31</v>
-      </c>
-      <c r="D10" t="s" s="124">
-        <v>83</v>
-      </c>
-      <c r="E10" t="s" s="124">
-        <v>93</v>
-      </c>
-      <c r="F10" s="124"/>
-      <c r="G10" s="124"/>
-      <c r="H10" s="124"/>
-      <c r="I10" s="124"/>
-      <c r="J10" s="124"/>
-      <c r="K10" s="124"/>
-      <c r="L10" s="124"/>
-      <c r="M10" s="124"/>
-      <c r="N10" s="124"/>
-      <c r="O10" s="124"/>
-      <c r="P10" s="124"/>
-      <c r="Q10" s="124"/>
-      <c r="R10" s="124"/>
-      <c r="S10" s="124"/>
-      <c r="T10" s="124"/>
-      <c r="U10" s="124"/>
-      <c r="V10" s="124"/>
-      <c r="W10" s="124"/>
-      <c r="X10" s="124"/>
-      <c r="Y10" s="124"/>
-      <c r="Z10" s="124"/>
-      <c r="AA10" s="124"/>
-      <c r="AB10" s="124"/>
-      <c r="AC10" s="124"/>
-      <c r="AD10" s="124"/>
-      <c r="AE10" s="124"/>
-      <c r="AF10" s="124"/>
-      <c r="AG10" s="124"/>
-      <c r="AH10" s="124"/>
-      <c r="AI10" s="124"/>
-      <c r="AJ10" s="124"/>
-      <c r="AK10" s="124"/>
-      <c r="AL10" s="124"/>
-      <c r="AM10" s="124"/>
-      <c r="AN10" s="124"/>
-      <c r="AO10" s="124"/>
-      <c r="AP10" s="124"/>
-      <c r="AQ10" s="124"/>
-      <c r="AR10" s="124"/>
-      <c r="AS10" s="124"/>
-      <c r="AT10" s="124"/>
-      <c r="AU10" s="124"/>
-      <c r="AV10" s="124"/>
-      <c r="AW10" s="124"/>
-      <c r="AX10" s="124"/>
-      <c r="AY10" s="124"/>
-      <c r="AZ10" s="124"/>
-      <c r="BA10" s="124"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="s" s="124">
-        <v>82</v>
-      </c>
-      <c r="B11" t="s" s="124">
-        <v>94</v>
-      </c>
-      <c r="C11" t="s" s="124">
-        <v>95</v>
-      </c>
-      <c r="D11" t="s" s="124">
-        <v>83</v>
-      </c>
-      <c r="E11" t="s" s="124">
-        <v>55</v>
-      </c>
-      <c r="F11" s="124"/>
-      <c r="G11" s="124"/>
-      <c r="H11" s="124"/>
-      <c r="I11" s="124"/>
-      <c r="J11" s="124"/>
-      <c r="K11" s="124"/>
-      <c r="L11" s="124"/>
-      <c r="M11" s="124"/>
-      <c r="N11" s="124"/>
-      <c r="O11" s="124"/>
-      <c r="P11" s="124"/>
-      <c r="Q11" s="124"/>
-      <c r="R11" s="124"/>
-      <c r="S11" s="124"/>
-      <c r="T11" s="124"/>
-      <c r="U11" s="124"/>
-      <c r="V11" s="124"/>
-      <c r="W11" s="124"/>
-      <c r="X11" s="124"/>
-      <c r="Y11" s="124"/>
-      <c r="Z11" s="124"/>
-      <c r="AA11" s="124"/>
-      <c r="AB11" s="124"/>
-      <c r="AC11" s="124"/>
-      <c r="AD11" s="124"/>
-      <c r="AE11" s="124"/>
-      <c r="AF11" s="124"/>
-      <c r="AG11" s="124"/>
-      <c r="AH11" s="124"/>
-      <c r="AI11" s="124"/>
-      <c r="AJ11" s="124"/>
-      <c r="AK11" s="124"/>
-      <c r="AL11" s="124"/>
-      <c r="AM11" s="124"/>
-      <c r="AN11" s="124"/>
-      <c r="AO11" s="124"/>
-      <c r="AP11" s="124"/>
-      <c r="AQ11" s="124"/>
-      <c r="AR11" s="124"/>
-      <c r="AS11" s="124"/>
-      <c r="AT11" s="124"/>
-      <c r="AU11" s="124"/>
-      <c r="AV11" s="124"/>
-      <c r="AW11" s="124"/>
-      <c r="AX11" s="124"/>
-      <c r="AY11" s="124"/>
-      <c r="AZ11" s="124"/>
-      <c r="BA11" s="124"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="124">
-        <v>82</v>
-      </c>
-      <c r="B12" t="s" s="124">
-        <v>96</v>
-      </c>
-      <c r="C12" t="s" s="124">
-        <v>97</v>
-      </c>
-      <c r="D12" t="s" s="124">
-        <v>83</v>
-      </c>
-      <c r="E12" t="s" s="124">
-        <v>97</v>
-      </c>
-      <c r="F12" s="124"/>
-      <c r="G12" s="124"/>
-      <c r="H12" s="124"/>
-      <c r="I12" s="124"/>
-      <c r="J12" s="124"/>
-      <c r="K12" s="124"/>
-      <c r="L12" s="124"/>
-      <c r="M12" s="124"/>
-      <c r="N12" s="124"/>
-      <c r="O12" s="124"/>
-      <c r="P12" s="124"/>
-      <c r="Q12" s="124"/>
-      <c r="R12" s="124"/>
-      <c r="S12" s="124"/>
-      <c r="T12" s="124"/>
-      <c r="U12" s="124"/>
-      <c r="V12" s="124"/>
-      <c r="W12" s="124"/>
-      <c r="X12" s="124"/>
-      <c r="Y12" s="124"/>
-      <c r="Z12" s="124"/>
-      <c r="AA12" s="124"/>
-      <c r="AB12" s="124"/>
-      <c r="AC12" s="124"/>
-      <c r="AD12" s="124"/>
-      <c r="AE12" s="124"/>
-      <c r="AF12" s="124"/>
-      <c r="AG12" s="124"/>
-      <c r="AH12" s="124"/>
-      <c r="AI12" s="124"/>
-      <c r="AJ12" s="124"/>
-      <c r="AK12" s="124"/>
-      <c r="AL12" s="124"/>
-      <c r="AM12" s="124"/>
-      <c r="AN12" s="124"/>
-      <c r="AO12" s="124"/>
-      <c r="AP12" s="124"/>
-      <c r="AQ12" s="124"/>
-      <c r="AR12" s="124"/>
-      <c r="AS12" s="124"/>
-      <c r="AT12" s="124"/>
-      <c r="AU12" s="124"/>
-      <c r="AV12" s="124"/>
-      <c r="AW12" s="124"/>
-      <c r="AX12" s="124"/>
-      <c r="AY12" s="124"/>
-      <c r="AZ12" s="124"/>
-      <c r="BA12" s="124"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="124">
-        <v>82</v>
-      </c>
-      <c r="B13" t="s" s="124">
-        <v>98</v>
-      </c>
-      <c r="C13" t="s" s="124">
-        <v>99</v>
-      </c>
-      <c r="D13" t="s" s="124">
-        <v>83</v>
-      </c>
-      <c r="E13" t="s" s="124">
-        <v>100</v>
-      </c>
-      <c r="F13" s="124"/>
-      <c r="G13" s="124"/>
-      <c r="H13" s="124"/>
-      <c r="I13" s="124"/>
-      <c r="J13" s="124"/>
-      <c r="K13" s="124"/>
-      <c r="L13" s="124"/>
-      <c r="M13" s="124"/>
-      <c r="N13" s="124"/>
-      <c r="O13" s="124"/>
-      <c r="P13" s="124"/>
-      <c r="Q13" s="124"/>
-      <c r="R13" s="124"/>
-      <c r="S13" s="124"/>
-      <c r="T13" s="124"/>
-      <c r="U13" s="124"/>
-      <c r="V13" s="124"/>
-      <c r="W13" s="124"/>
-      <c r="X13" s="124"/>
-      <c r="Y13" s="124"/>
-      <c r="Z13" s="124"/>
-      <c r="AA13" s="124"/>
-      <c r="AB13" s="124"/>
-      <c r="AC13" s="124"/>
-      <c r="AD13" s="124"/>
-      <c r="AE13" s="124"/>
-      <c r="AF13" s="124"/>
-      <c r="AG13" s="124"/>
-      <c r="AH13" s="124"/>
-      <c r="AI13" s="124"/>
-      <c r="AJ13" s="124"/>
-      <c r="AK13" s="124"/>
-      <c r="AL13" s="124"/>
-      <c r="AM13" s="124"/>
-      <c r="AN13" s="124"/>
-      <c r="AO13" s="124"/>
-      <c r="AP13" s="124"/>
-      <c r="AQ13" s="124"/>
-      <c r="AR13" s="124"/>
-      <c r="AS13" s="124"/>
-      <c r="AT13" s="124"/>
-      <c r="AU13" s="124"/>
-      <c r="AV13" s="124"/>
-      <c r="AW13" s="124"/>
-      <c r="AX13" s="124"/>
-      <c r="AY13" s="124"/>
-      <c r="AZ13" s="124"/>
-      <c r="BA13" s="124"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="s" s="124">
-        <v>82</v>
-      </c>
-      <c r="B14" t="s" s="124">
-        <v>101</v>
-      </c>
-      <c r="C14" t="s" s="124">
-        <v>97</v>
-      </c>
-      <c r="D14" t="s" s="124">
-        <v>83</v>
-      </c>
-      <c r="E14" t="s" s="124">
-        <v>97</v>
-      </c>
-      <c r="F14" s="124"/>
-      <c r="G14" s="124"/>
-      <c r="H14" s="124"/>
-      <c r="I14" s="124"/>
-      <c r="J14" s="124"/>
-      <c r="K14" s="124"/>
-      <c r="L14" s="124"/>
-      <c r="M14" s="124"/>
-      <c r="N14" s="124"/>
-      <c r="O14" s="124"/>
-      <c r="P14" s="124"/>
-      <c r="Q14" s="124"/>
-      <c r="R14" s="124"/>
-      <c r="S14" s="124"/>
-      <c r="T14" s="124"/>
-      <c r="U14" s="124"/>
-      <c r="V14" s="124"/>
-      <c r="W14" s="124"/>
-      <c r="X14" s="124"/>
-      <c r="Y14" s="124"/>
-      <c r="Z14" s="124"/>
-      <c r="AA14" s="124"/>
-      <c r="AB14" s="124"/>
-      <c r="AC14" s="124"/>
-      <c r="AD14" s="124"/>
-      <c r="AE14" s="124"/>
-      <c r="AF14" s="124"/>
-      <c r="AG14" s="124"/>
-      <c r="AH14" s="124"/>
-      <c r="AI14" s="124"/>
-      <c r="AJ14" s="124"/>
-      <c r="AK14" s="124"/>
-      <c r="AL14" s="124"/>
-      <c r="AM14" s="124"/>
-      <c r="AN14" s="124"/>
-      <c r="AO14" s="124"/>
-      <c r="AP14" s="124"/>
-      <c r="AQ14" s="124"/>
-      <c r="AR14" s="124"/>
-      <c r="AS14" s="124"/>
-      <c r="AT14" s="124"/>
-      <c r="AU14" s="124"/>
-      <c r="AV14" s="124"/>
-      <c r="AW14" s="124"/>
-      <c r="AX14" s="124"/>
-      <c r="AY14" s="124"/>
-      <c r="AZ14" s="124"/>
-      <c r="BA14" s="124"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="s" s="124">
-        <v>82</v>
-      </c>
-      <c r="B15" t="s" s="124">
-        <v>102</v>
-      </c>
-      <c r="C15" t="s" s="124">
-        <v>97</v>
-      </c>
-      <c r="D15" t="s" s="124">
-        <v>83</v>
-      </c>
-      <c r="E15" t="s" s="124">
-        <v>97</v>
-      </c>
-      <c r="F15" s="124"/>
-      <c r="G15" s="124"/>
-      <c r="H15" s="124"/>
-      <c r="I15" s="124"/>
-      <c r="J15" s="124"/>
-      <c r="K15" s="124"/>
-      <c r="L15" s="124"/>
-      <c r="M15" s="124"/>
-      <c r="N15" s="124"/>
-      <c r="O15" s="124"/>
-      <c r="P15" s="124"/>
-      <c r="Q15" s="124"/>
-      <c r="R15" s="124"/>
-      <c r="S15" s="124"/>
-      <c r="T15" s="124"/>
-      <c r="U15" s="124"/>
-      <c r="V15" s="124"/>
-      <c r="W15" s="124"/>
-      <c r="X15" s="124"/>
-      <c r="Y15" s="124"/>
-      <c r="Z15" s="124"/>
-      <c r="AA15" s="124"/>
-      <c r="AB15" s="124"/>
-      <c r="AC15" s="124"/>
-      <c r="AD15" s="124"/>
-      <c r="AE15" s="124"/>
-      <c r="AF15" s="124"/>
-      <c r="AG15" s="124"/>
-      <c r="AH15" s="124"/>
-      <c r="AI15" s="124"/>
-      <c r="AJ15" s="124"/>
-      <c r="AK15" s="124"/>
-      <c r="AL15" s="124"/>
-      <c r="AM15" s="124"/>
-      <c r="AN15" s="124"/>
-      <c r="AO15" s="124"/>
-      <c r="AP15" s="124"/>
-      <c r="AQ15" s="124"/>
-      <c r="AR15" s="124"/>
-      <c r="AS15" s="124"/>
-      <c r="AT15" s="124"/>
-      <c r="AU15" s="124"/>
-      <c r="AV15" s="124"/>
-      <c r="AW15" s="124"/>
-      <c r="AX15" s="124"/>
-      <c r="AY15" s="124"/>
-      <c r="AZ15" s="124"/>
-      <c r="BA15" s="124"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="s" s="124">
-        <v>82</v>
-      </c>
-      <c r="B16" t="s" s="124">
-        <v>103</v>
-      </c>
-      <c r="C16" t="s" s="124">
-        <v>97</v>
-      </c>
-      <c r="D16" t="s" s="124">
-        <v>83</v>
-      </c>
-      <c r="E16" t="s" s="124">
-        <v>97</v>
-      </c>
-      <c r="F16" s="124"/>
-      <c r="G16" s="124"/>
-      <c r="H16" s="124"/>
-      <c r="I16" s="124"/>
-      <c r="J16" s="124"/>
-      <c r="K16" s="124"/>
-      <c r="L16" s="124"/>
-      <c r="M16" s="124"/>
-      <c r="N16" s="124"/>
-      <c r="O16" s="124"/>
-      <c r="P16" s="124"/>
-      <c r="Q16" s="124"/>
-      <c r="R16" s="124"/>
-      <c r="S16" s="124"/>
-      <c r="T16" s="124"/>
-      <c r="U16" s="124"/>
-      <c r="V16" s="124"/>
-      <c r="W16" s="124"/>
-      <c r="X16" s="124"/>
-      <c r="Y16" s="124"/>
-      <c r="Z16" s="124"/>
-      <c r="AA16" s="124"/>
-      <c r="AB16" s="124"/>
-      <c r="AC16" s="124"/>
-      <c r="AD16" s="124"/>
-      <c r="AE16" s="124"/>
-      <c r="AF16" s="124"/>
-      <c r="AG16" s="124"/>
-      <c r="AH16" s="124"/>
-      <c r="AI16" s="124"/>
-      <c r="AJ16" s="124"/>
-      <c r="AK16" s="124"/>
-      <c r="AL16" s="124"/>
-      <c r="AM16" s="124"/>
-      <c r="AN16" s="124"/>
-      <c r="AO16" s="124"/>
-      <c r="AP16" s="124"/>
-      <c r="AQ16" s="124"/>
-      <c r="AR16" s="124"/>
-      <c r="AS16" s="124"/>
-      <c r="AT16" s="124"/>
-      <c r="AU16" s="124"/>
-      <c r="AV16" s="124"/>
-      <c r="AW16" s="124"/>
-      <c r="AX16" s="124"/>
-      <c r="AY16" s="124"/>
-      <c r="AZ16" s="124"/>
-      <c r="BA16" s="124"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="s" s="124">
-        <v>82</v>
-      </c>
-      <c r="B17" t="s" s="124">
-        <v>104</v>
-      </c>
-      <c r="C17" t="s" s="124">
-        <v>97</v>
-      </c>
-      <c r="D17" t="s" s="124">
-        <v>83</v>
-      </c>
-      <c r="E17" t="s" s="124">
-        <v>97</v>
-      </c>
-      <c r="F17" s="124"/>
-      <c r="G17" s="124"/>
-      <c r="H17" s="124"/>
-      <c r="I17" s="124"/>
-      <c r="J17" s="124"/>
-      <c r="K17" s="124"/>
-      <c r="L17" s="124"/>
-      <c r="M17" s="124"/>
-      <c r="N17" s="124"/>
-      <c r="O17" s="124"/>
-      <c r="P17" s="124"/>
-      <c r="Q17" s="124"/>
-      <c r="R17" s="124"/>
-      <c r="S17" s="124"/>
-      <c r="T17" s="124"/>
-      <c r="U17" s="124"/>
-      <c r="V17" s="124"/>
-      <c r="W17" s="124"/>
-      <c r="X17" s="124"/>
-      <c r="Y17" s="124"/>
-      <c r="Z17" s="124"/>
-      <c r="AA17" s="124"/>
-      <c r="AB17" s="124"/>
-      <c r="AC17" s="124"/>
-      <c r="AD17" s="124"/>
-      <c r="AE17" s="124"/>
-      <c r="AF17" s="124"/>
-      <c r="AG17" s="124"/>
-      <c r="AH17" s="124"/>
-      <c r="AI17" s="124"/>
-      <c r="AJ17" s="124"/>
-      <c r="AK17" s="124"/>
-      <c r="AL17" s="124"/>
-      <c r="AM17" s="124"/>
-      <c r="AN17" s="124"/>
-      <c r="AO17" s="124"/>
-      <c r="AP17" s="124"/>
-      <c r="AQ17" s="124"/>
-      <c r="AR17" s="124"/>
-      <c r="AS17" s="124"/>
-      <c r="AT17" s="124"/>
-      <c r="AU17" s="124"/>
-      <c r="AV17" s="124"/>
-      <c r="AW17" s="124"/>
-      <c r="AX17" s="124"/>
-      <c r="AY17" s="124"/>
-      <c r="AZ17" s="124"/>
-      <c r="BA17" s="124"/>
-    </row>
-  </sheetData>
-  <mergeCells>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AJ3:AK3"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="AN3:AO3"/>
-    <mergeCell ref="AP3:AQ3"/>
-    <mergeCell ref="AR3:AS3"/>
-    <mergeCell ref="AT3:AU3"/>
-    <mergeCell ref="AV3:AW3"/>
-    <mergeCell ref="AX3:AY3"/>
-    <mergeCell ref="AZ3:BA3"/>
-  </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
delete bugs whith null.well done driwing
</commit_message>
<xml_diff>
--- a/sourse - копия.xlsx
+++ b/sourse - копия.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Комбайн" sheetId="1" r:id="rId1"/>
     <sheet name="01.10" sheetId="71" r:id="rId2"/>
+    <sheet name="test" r:id="rId7" sheetId="72"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -2794,7 +2795,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="99">
   <si>
     <t>Держ №</t>
   </si>
@@ -3038,11 +3039,74 @@
   <si>
     <t>test version</t>
   </si>
+  <si>
+    <t xml:space="preserve">John Deere-S6901_09039BI"
+</t>
+  </si>
+  <si>
+    <t>Хмільниця_Тест</t>
+  </si>
+  <si>
+    <t>Збирання кукурудзи_Тест</t>
+  </si>
+  <si>
+    <t>Півень В.М.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John Deere-S9880_11270CB"
+</t>
+  </si>
+  <si>
+    <t>Коробко В.М.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John Deere-S9880_11271CB"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John Deere-S9880_11273CB"
+</t>
+  </si>
+  <si>
+    <t>Василенко А.П.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John Deere-S9880_11269CB"
+</t>
+  </si>
+  <si>
+    <t>Скляров О.В.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John Deere-S9880_11272CB"
+</t>
+  </si>
+  <si>
+    <t>Скляров М.В</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Палессе 16318СВ"
+</t>
+  </si>
+  <si>
+    <t>16318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нью-Холонд Новий "
+</t>
+  </si>
+  <si>
+    <t>б/н</t>
+  </si>
+  <si>
+    <t>Иллюшко С.Л</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3127,7 +3191,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3142,19 +3206,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.79998168889431442" rgb="4F81BD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.79998168889431442" rgb="F79646"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="0" rgb="000000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3178,19 +3242,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor theme="3" tint="0.79998168889431442" rgb="EEECE1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
+        <fgColor theme="0" tint="-0.249977111117893" rgb="000000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.59999389629810485" rgb="9BBB59"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3200,8 +3264,55 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill>
+        <fgColor rgb="FFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="64"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor rgb="BFBFBF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="BFBFBF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor rgb="00B050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B050"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="85">
     <border>
       <left/>
       <right/>
@@ -3527,12 +3638,488 @@
       </bottom>
       <diagonal/>
     </border>
+    <border/>
+    <border>
+      <top style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <top style="medium"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <top style="medium"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="medium"/>
+    </border>
+    <border>
+      <right style="medium"/>
+      <top style="medium"/>
+    </border>
+    <border>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <top style="medium"/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium"/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium"/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <top style="thin"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="thin"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <top style="thin"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="thin"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin"/>
+    </border>
+    <border>
+      <right style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="286">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3741,6 +4328,209 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="57" xfId="0" applyFill="true" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="30" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="36" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="42" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="49" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="55" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="62" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="68" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="74" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="82" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -4058,9 +4848,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -6771,13 +7561,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="32" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="32" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="32" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" style="32" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" style="32" customWidth="1"/>
-    <col min="6" max="53" width="3.28515625" style="32" customWidth="1"/>
-    <col min="54" max="16384" width="9.140625" style="32"/>
+    <col min="1" max="1" customWidth="true" style="32" width="14.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="32" width="23.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="32" width="11.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="32" width="25.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="32" width="22.140625" collapsed="true"/>
+    <col min="6" max="53" customWidth="true" style="32" width="3.28515625" collapsed="true"/>
+    <col min="54" max="16384" style="32" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.25">
@@ -8615,4 +9405,792 @@
   <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="true"/>
+    <col min="2" max="2" width="23.85546875" customWidth="true"/>
+    <col min="3" max="3" width="11.42578125" customWidth="true"/>
+    <col min="4" max="4" width="25.85546875" customWidth="true"/>
+    <col min="5" max="5" width="22.140625" customWidth="true"/>
+    <col min="6" max="6" width="3.28515625" customWidth="true"/>
+    <col min="7" max="7" width="3.28515625" customWidth="true"/>
+    <col min="8" max="8" width="3.28515625" customWidth="true"/>
+    <col min="9" max="9" width="3.28515625" customWidth="true"/>
+    <col min="10" max="10" width="3.28515625" customWidth="true"/>
+    <col min="11" max="11" width="3.28515625" customWidth="true"/>
+    <col min="12" max="12" width="3.28515625" customWidth="true"/>
+    <col min="13" max="13" width="3.28515625" customWidth="true"/>
+    <col min="14" max="14" width="3.28515625" customWidth="true"/>
+    <col min="15" max="15" width="3.28515625" customWidth="true"/>
+    <col min="16" max="16" width="3.28515625" customWidth="true"/>
+    <col min="17" max="17" width="3.28515625" customWidth="true"/>
+    <col min="18" max="18" width="3.28515625" customWidth="true"/>
+    <col min="19" max="19" width="3.28515625" customWidth="true"/>
+    <col min="20" max="20" width="3.28515625" customWidth="true"/>
+    <col min="21" max="21" width="3.28515625" customWidth="true"/>
+    <col min="22" max="22" width="3.28515625" customWidth="true"/>
+    <col min="23" max="23" width="3.28515625" customWidth="true"/>
+    <col min="24" max="24" width="3.28515625" customWidth="true"/>
+    <col min="25" max="25" width="3.28515625" customWidth="true"/>
+    <col min="26" max="26" width="3.28515625" customWidth="true"/>
+    <col min="27" max="27" width="3.28515625" customWidth="true"/>
+    <col min="28" max="28" width="3.28515625" customWidth="true"/>
+    <col min="29" max="29" width="3.28515625" customWidth="true"/>
+    <col min="30" max="30" width="3.28515625" customWidth="true"/>
+    <col min="31" max="31" width="3.28515625" customWidth="true"/>
+    <col min="32" max="32" width="3.28515625" customWidth="true"/>
+    <col min="33" max="33" width="3.28515625" customWidth="true"/>
+    <col min="34" max="34" width="3.28515625" customWidth="true"/>
+    <col min="35" max="35" width="3.28515625" customWidth="true"/>
+    <col min="36" max="36" width="3.28515625" customWidth="true"/>
+    <col min="37" max="37" width="3.28515625" customWidth="true"/>
+    <col min="38" max="38" width="3.28515625" customWidth="true"/>
+    <col min="39" max="39" width="3.28515625" customWidth="true"/>
+    <col min="40" max="40" width="3.28515625" customWidth="true"/>
+    <col min="41" max="41" width="3.28515625" customWidth="true"/>
+    <col min="42" max="42" width="3.28515625" customWidth="true"/>
+    <col min="43" max="43" width="3.28515625" customWidth="true"/>
+    <col min="44" max="44" width="3.28515625" customWidth="true"/>
+    <col min="45" max="45" width="3.28515625" customWidth="true"/>
+    <col min="46" max="46" width="3.28515625" customWidth="true"/>
+    <col min="47" max="47" width="3.28515625" customWidth="true"/>
+    <col min="48" max="48" width="3.28515625" customWidth="true"/>
+    <col min="49" max="49" width="3.28515625" customWidth="true"/>
+    <col min="50" max="50" width="3.28515625" customWidth="true"/>
+    <col min="51" max="51" width="3.28515625" customWidth="true"/>
+    <col min="52" max="52" width="3.28515625" customWidth="true"/>
+    <col min="53" max="53" width="3.28515625" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="s" s="114">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="115">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s" s="115">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s" s="115">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s" s="115">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s" s="115">
+        <v>20</v>
+      </c>
+      <c r="F3" t="n" s="115">
+        <v>7.0</v>
+      </c>
+      <c r="G3" s="120"/>
+      <c r="H3" t="n" s="115">
+        <v>8.0</v>
+      </c>
+      <c r="I3" s="120"/>
+      <c r="J3" t="n" s="115">
+        <v>9.0</v>
+      </c>
+      <c r="K3" s="120"/>
+      <c r="L3" t="n" s="115">
+        <v>10.0</v>
+      </c>
+      <c r="M3" s="120"/>
+      <c r="N3" t="n" s="115">
+        <v>11.0</v>
+      </c>
+      <c r="O3" s="120"/>
+      <c r="P3" t="n" s="115">
+        <v>12.0</v>
+      </c>
+      <c r="Q3" s="120"/>
+      <c r="R3" t="n" s="115">
+        <v>13.0</v>
+      </c>
+      <c r="S3" s="120"/>
+      <c r="T3" t="n" s="115">
+        <v>14.0</v>
+      </c>
+      <c r="U3" s="120"/>
+      <c r="V3" t="n" s="115">
+        <v>15.0</v>
+      </c>
+      <c r="W3" s="120"/>
+      <c r="X3" t="n" s="115">
+        <v>16.0</v>
+      </c>
+      <c r="Y3" s="120"/>
+      <c r="Z3" t="n" s="115">
+        <v>17.0</v>
+      </c>
+      <c r="AA3" s="120"/>
+      <c r="AB3" t="n" s="115">
+        <v>18.0</v>
+      </c>
+      <c r="AC3" s="120"/>
+      <c r="AD3" t="n" s="115">
+        <v>19.0</v>
+      </c>
+      <c r="AE3" s="120"/>
+      <c r="AF3" t="n" s="115">
+        <v>20.0</v>
+      </c>
+      <c r="AG3" s="120"/>
+      <c r="AH3" t="n" s="115">
+        <v>21.0</v>
+      </c>
+      <c r="AI3" s="120"/>
+      <c r="AJ3" t="n" s="115">
+        <v>22.0</v>
+      </c>
+      <c r="AK3" s="120"/>
+      <c r="AL3" t="n" s="115">
+        <v>23.0</v>
+      </c>
+      <c r="AM3" s="120"/>
+      <c r="AN3" t="n" s="115">
+        <v>24.0</v>
+      </c>
+      <c r="AO3" s="120"/>
+      <c r="AP3" t="n" s="115">
+        <v>1.0</v>
+      </c>
+      <c r="AQ3" s="120"/>
+      <c r="AR3" t="n" s="115">
+        <v>2.0</v>
+      </c>
+      <c r="AS3" s="120"/>
+      <c r="AT3" t="n" s="115">
+        <v>3.0</v>
+      </c>
+      <c r="AU3" s="120"/>
+      <c r="AV3" t="n" s="115">
+        <v>4.0</v>
+      </c>
+      <c r="AW3" s="120"/>
+      <c r="AX3" t="n" s="115">
+        <v>5.0</v>
+      </c>
+      <c r="AY3" s="120"/>
+      <c r="AZ3" t="n" s="115">
+        <v>6.0</v>
+      </c>
+      <c r="BA3" s="120"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="124"/>
+      <c r="B4" s="124"/>
+      <c r="C4" s="124"/>
+      <c r="D4" s="124"/>
+      <c r="E4" s="124"/>
+      <c r="F4" s="124"/>
+      <c r="G4" s="124"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
+      <c r="K4" s="124"/>
+      <c r="L4" s="124"/>
+      <c r="M4" s="124"/>
+      <c r="N4" s="124"/>
+      <c r="O4" s="124"/>
+      <c r="P4" s="124"/>
+      <c r="Q4" s="124"/>
+      <c r="R4" s="124"/>
+      <c r="S4" s="124"/>
+      <c r="T4" s="124"/>
+      <c r="U4" s="124"/>
+      <c r="V4" s="124"/>
+      <c r="W4" s="124"/>
+      <c r="X4" s="124"/>
+      <c r="Y4" s="124"/>
+      <c r="Z4" s="124"/>
+      <c r="AA4" s="124"/>
+      <c r="AB4" s="124"/>
+      <c r="AC4" s="124"/>
+      <c r="AD4" s="124"/>
+      <c r="AE4" s="124"/>
+      <c r="AF4" s="124"/>
+      <c r="AG4" s="124"/>
+      <c r="AH4" s="124"/>
+      <c r="AI4" s="124"/>
+      <c r="AJ4" s="124"/>
+      <c r="AK4" s="124"/>
+      <c r="AL4" s="124"/>
+      <c r="AM4" s="124"/>
+      <c r="AN4" s="124"/>
+      <c r="AO4" s="124"/>
+      <c r="AP4" s="124"/>
+      <c r="AQ4" s="124"/>
+      <c r="AR4" s="124"/>
+      <c r="AS4" s="124"/>
+      <c r="AT4" s="124"/>
+      <c r="AU4" s="124"/>
+      <c r="AV4" s="124"/>
+      <c r="AW4" s="124"/>
+      <c r="AX4" s="124"/>
+      <c r="AY4" s="124"/>
+      <c r="AZ4" s="124"/>
+      <c r="BA4" s="124"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="124">
+        <v>82</v>
+      </c>
+      <c r="B5" t="s" s="124">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s" s="124">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s" s="124">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s" s="124">
+        <v>84</v>
+      </c>
+      <c r="F5" s="124"/>
+      <c r="G5" s="124"/>
+      <c r="H5" s="124"/>
+      <c r="I5" s="124"/>
+      <c r="J5" s="124"/>
+      <c r="K5" s="125"/>
+      <c r="L5" s="126"/>
+      <c r="M5" s="127"/>
+      <c r="N5" s="128"/>
+      <c r="O5" s="129"/>
+      <c r="P5" s="130"/>
+      <c r="Q5" s="131"/>
+      <c r="R5" s="132"/>
+      <c r="S5" s="133"/>
+      <c r="T5" s="134"/>
+      <c r="U5" s="135"/>
+      <c r="V5" s="136"/>
+      <c r="W5" s="137"/>
+      <c r="X5" s="138"/>
+      <c r="Y5" s="139"/>
+      <c r="Z5" s="140"/>
+      <c r="AA5" s="141"/>
+      <c r="AB5" s="142"/>
+      <c r="AC5" s="143"/>
+      <c r="AD5" s="144"/>
+      <c r="AE5" s="145"/>
+      <c r="AF5" s="146"/>
+      <c r="AG5" s="147"/>
+      <c r="AH5" s="148"/>
+      <c r="AI5" s="149"/>
+      <c r="AJ5" s="124"/>
+      <c r="AK5" s="124"/>
+      <c r="AL5" s="124"/>
+      <c r="AM5" s="124"/>
+      <c r="AN5" s="124"/>
+      <c r="AO5" s="124"/>
+      <c r="AP5" s="124"/>
+      <c r="AQ5" s="124"/>
+      <c r="AR5" s="124"/>
+      <c r="AS5" s="124"/>
+      <c r="AT5" s="124"/>
+      <c r="AU5" s="124"/>
+      <c r="AV5" s="124"/>
+      <c r="AW5" s="124"/>
+      <c r="AX5" s="124"/>
+      <c r="AY5" s="124"/>
+      <c r="AZ5" s="124"/>
+      <c r="BA5" s="124"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="124">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s" s="124">
+        <v>85</v>
+      </c>
+      <c r="C6" t="s" s="124">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s" s="124">
+        <v>83</v>
+      </c>
+      <c r="E6" t="s" s="124">
+        <v>86</v>
+      </c>
+      <c r="F6" s="124"/>
+      <c r="G6" s="124"/>
+      <c r="H6" s="124"/>
+      <c r="I6" s="150"/>
+      <c r="J6" s="151"/>
+      <c r="K6" s="152"/>
+      <c r="L6" s="153"/>
+      <c r="M6" s="154"/>
+      <c r="N6" s="155"/>
+      <c r="O6" s="156"/>
+      <c r="P6" s="157"/>
+      <c r="Q6" s="158"/>
+      <c r="R6" s="159"/>
+      <c r="S6" s="160"/>
+      <c r="T6" s="161"/>
+      <c r="U6" s="162"/>
+      <c r="V6" s="163"/>
+      <c r="W6" s="164"/>
+      <c r="X6" s="165"/>
+      <c r="Y6" s="166"/>
+      <c r="Z6" s="167"/>
+      <c r="AA6" s="168"/>
+      <c r="AB6" s="169"/>
+      <c r="AC6" s="170"/>
+      <c r="AD6" s="171"/>
+      <c r="AE6" s="172"/>
+      <c r="AF6" s="173"/>
+      <c r="AG6" s="174"/>
+      <c r="AH6" s="175"/>
+      <c r="AI6" s="176"/>
+      <c r="AJ6" s="124"/>
+      <c r="AK6" s="124"/>
+      <c r="AL6" s="124"/>
+      <c r="AM6" s="124"/>
+      <c r="AN6" s="124"/>
+      <c r="AO6" s="124"/>
+      <c r="AP6" s="124"/>
+      <c r="AQ6" s="124"/>
+      <c r="AR6" s="124"/>
+      <c r="AS6" s="124"/>
+      <c r="AT6" s="124"/>
+      <c r="AU6" s="124"/>
+      <c r="AV6" s="124"/>
+      <c r="AW6" s="124"/>
+      <c r="AX6" s="124"/>
+      <c r="AY6" s="124"/>
+      <c r="AZ6" s="124"/>
+      <c r="BA6" s="124"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="124">
+        <v>82</v>
+      </c>
+      <c r="B7" t="s" s="124">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s" s="124">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s" s="124">
+        <v>83</v>
+      </c>
+      <c r="E7" t="s" s="124">
+        <v>51</v>
+      </c>
+      <c r="F7" s="124"/>
+      <c r="G7" s="124"/>
+      <c r="H7" s="124"/>
+      <c r="I7" s="124"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="177"/>
+      <c r="L7" s="178"/>
+      <c r="M7" s="179"/>
+      <c r="N7" s="180"/>
+      <c r="O7" s="181"/>
+      <c r="P7" s="182"/>
+      <c r="Q7" s="183"/>
+      <c r="R7" s="184"/>
+      <c r="S7" s="185"/>
+      <c r="T7" s="186"/>
+      <c r="U7" s="187"/>
+      <c r="V7" s="188"/>
+      <c r="W7" s="189"/>
+      <c r="X7" s="124"/>
+      <c r="Y7" s="124"/>
+      <c r="Z7" s="124"/>
+      <c r="AA7" s="124"/>
+      <c r="AB7" s="124"/>
+      <c r="AC7" s="124"/>
+      <c r="AD7" s="124"/>
+      <c r="AE7" s="124"/>
+      <c r="AF7" s="124"/>
+      <c r="AG7" s="124"/>
+      <c r="AH7" s="124"/>
+      <c r="AI7" s="124"/>
+      <c r="AJ7" s="124"/>
+      <c r="AK7" s="124"/>
+      <c r="AL7" s="124"/>
+      <c r="AM7" s="124"/>
+      <c r="AN7" s="124"/>
+      <c r="AO7" s="124"/>
+      <c r="AP7" s="124"/>
+      <c r="AQ7" s="124"/>
+      <c r="AR7" s="124"/>
+      <c r="AS7" s="124"/>
+      <c r="AT7" s="124"/>
+      <c r="AU7" s="124"/>
+      <c r="AV7" s="124"/>
+      <c r="AW7" s="124"/>
+      <c r="AX7" s="124"/>
+      <c r="AY7" s="124"/>
+      <c r="AZ7" s="124"/>
+      <c r="BA7" s="124"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="124">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s" s="124">
+        <v>88</v>
+      </c>
+      <c r="C8" t="s" s="124">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s" s="124">
+        <v>83</v>
+      </c>
+      <c r="E8" t="s" s="124">
+        <v>89</v>
+      </c>
+      <c r="F8" s="124"/>
+      <c r="G8" s="124"/>
+      <c r="H8" s="124"/>
+      <c r="I8" s="124"/>
+      <c r="J8" s="124"/>
+      <c r="K8" s="124"/>
+      <c r="L8" s="190"/>
+      <c r="M8" s="191"/>
+      <c r="N8" s="192"/>
+      <c r="O8" s="193"/>
+      <c r="P8" s="194"/>
+      <c r="Q8" s="195"/>
+      <c r="R8" s="196"/>
+      <c r="S8" s="197"/>
+      <c r="T8" s="198"/>
+      <c r="U8" s="199"/>
+      <c r="V8" s="200"/>
+      <c r="W8" s="201"/>
+      <c r="X8" s="202"/>
+      <c r="Y8" s="203"/>
+      <c r="Z8" s="204"/>
+      <c r="AA8" s="205"/>
+      <c r="AB8" s="206"/>
+      <c r="AC8" s="207"/>
+      <c r="AD8" s="208"/>
+      <c r="AE8" s="209"/>
+      <c r="AF8" s="210"/>
+      <c r="AG8" s="211"/>
+      <c r="AH8" s="212"/>
+      <c r="AI8" s="124"/>
+      <c r="AJ8" s="124"/>
+      <c r="AK8" s="124"/>
+      <c r="AL8" s="124"/>
+      <c r="AM8" s="124"/>
+      <c r="AN8" s="124"/>
+      <c r="AO8" s="124"/>
+      <c r="AP8" s="124"/>
+      <c r="AQ8" s="124"/>
+      <c r="AR8" s="124"/>
+      <c r="AS8" s="124"/>
+      <c r="AT8" s="124"/>
+      <c r="AU8" s="124"/>
+      <c r="AV8" s="124"/>
+      <c r="AW8" s="124"/>
+      <c r="AX8" s="124"/>
+      <c r="AY8" s="124"/>
+      <c r="AZ8" s="124"/>
+      <c r="BA8" s="124"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="124">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s" s="124">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s" s="124">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s" s="124">
+        <v>83</v>
+      </c>
+      <c r="E9" t="s" s="124">
+        <v>91</v>
+      </c>
+      <c r="F9" s="124"/>
+      <c r="G9" s="124"/>
+      <c r="H9" s="124"/>
+      <c r="I9" s="124"/>
+      <c r="J9" s="124"/>
+      <c r="K9" s="124"/>
+      <c r="L9" s="213"/>
+      <c r="M9" s="214"/>
+      <c r="N9" s="215"/>
+      <c r="O9" s="216"/>
+      <c r="P9" s="217"/>
+      <c r="Q9" s="218"/>
+      <c r="R9" s="219"/>
+      <c r="S9" s="220"/>
+      <c r="T9" s="221"/>
+      <c r="U9" s="222"/>
+      <c r="V9" s="223"/>
+      <c r="W9" s="224"/>
+      <c r="X9" s="225"/>
+      <c r="Y9" s="226"/>
+      <c r="Z9" s="227"/>
+      <c r="AA9" s="228"/>
+      <c r="AB9" s="229"/>
+      <c r="AC9" s="230"/>
+      <c r="AD9" s="231"/>
+      <c r="AE9" s="232"/>
+      <c r="AF9" s="233"/>
+      <c r="AG9" s="234"/>
+      <c r="AH9" s="235"/>
+      <c r="AI9" s="236"/>
+      <c r="AJ9" s="124"/>
+      <c r="AK9" s="124"/>
+      <c r="AL9" s="124"/>
+      <c r="AM9" s="124"/>
+      <c r="AN9" s="124"/>
+      <c r="AO9" s="124"/>
+      <c r="AP9" s="124"/>
+      <c r="AQ9" s="124"/>
+      <c r="AR9" s="124"/>
+      <c r="AS9" s="124"/>
+      <c r="AT9" s="124"/>
+      <c r="AU9" s="124"/>
+      <c r="AV9" s="124"/>
+      <c r="AW9" s="124"/>
+      <c r="AX9" s="124"/>
+      <c r="AY9" s="124"/>
+      <c r="AZ9" s="124"/>
+      <c r="BA9" s="124"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="124">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s" s="124">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s" s="124">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s" s="124">
+        <v>83</v>
+      </c>
+      <c r="E10" t="s" s="124">
+        <v>93</v>
+      </c>
+      <c r="F10" s="124"/>
+      <c r="G10" s="124"/>
+      <c r="H10" s="124"/>
+      <c r="I10" s="124"/>
+      <c r="J10" s="124"/>
+      <c r="K10" s="124"/>
+      <c r="L10" s="237"/>
+      <c r="M10" s="238"/>
+      <c r="N10" s="239"/>
+      <c r="O10" s="240"/>
+      <c r="P10" s="241"/>
+      <c r="Q10" s="242"/>
+      <c r="R10" s="243"/>
+      <c r="S10" s="244"/>
+      <c r="T10" s="245"/>
+      <c r="U10" s="246"/>
+      <c r="V10" s="247"/>
+      <c r="W10" s="248"/>
+      <c r="X10" s="249"/>
+      <c r="Y10" s="250"/>
+      <c r="Z10" s="251"/>
+      <c r="AA10" s="252"/>
+      <c r="AB10" s="253"/>
+      <c r="AC10" s="254"/>
+      <c r="AD10" s="255"/>
+      <c r="AE10" s="256"/>
+      <c r="AF10" s="257"/>
+      <c r="AG10" s="258"/>
+      <c r="AH10" s="259"/>
+      <c r="AI10" s="260"/>
+      <c r="AJ10" s="124"/>
+      <c r="AK10" s="124"/>
+      <c r="AL10" s="124"/>
+      <c r="AM10" s="124"/>
+      <c r="AN10" s="124"/>
+      <c r="AO10" s="124"/>
+      <c r="AP10" s="124"/>
+      <c r="AQ10" s="124"/>
+      <c r="AR10" s="124"/>
+      <c r="AS10" s="124"/>
+      <c r="AT10" s="124"/>
+      <c r="AU10" s="124"/>
+      <c r="AV10" s="124"/>
+      <c r="AW10" s="124"/>
+      <c r="AX10" s="124"/>
+      <c r="AY10" s="124"/>
+      <c r="AZ10" s="124"/>
+      <c r="BA10" s="124"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="124">
+        <v>82</v>
+      </c>
+      <c r="B11" t="s" s="124">
+        <v>94</v>
+      </c>
+      <c r="C11" t="s" s="124">
+        <v>95</v>
+      </c>
+      <c r="D11" t="s" s="124">
+        <v>83</v>
+      </c>
+      <c r="E11" t="s" s="124">
+        <v>55</v>
+      </c>
+      <c r="F11" s="124"/>
+      <c r="G11" s="124"/>
+      <c r="H11" s="124"/>
+      <c r="I11" s="124"/>
+      <c r="J11" s="124"/>
+      <c r="K11" s="124"/>
+      <c r="L11" s="124"/>
+      <c r="M11" s="124"/>
+      <c r="N11" s="124"/>
+      <c r="O11" s="124"/>
+      <c r="P11" s="124"/>
+      <c r="Q11" s="124"/>
+      <c r="R11" s="124"/>
+      <c r="S11" s="124"/>
+      <c r="T11" s="124"/>
+      <c r="U11" s="124"/>
+      <c r="V11" s="124"/>
+      <c r="W11" s="124"/>
+      <c r="X11" s="124"/>
+      <c r="Y11" s="124"/>
+      <c r="Z11" s="124"/>
+      <c r="AA11" s="124"/>
+      <c r="AB11" s="124"/>
+      <c r="AC11" s="124"/>
+      <c r="AD11" s="124"/>
+      <c r="AE11" s="124"/>
+      <c r="AF11" s="124"/>
+      <c r="AG11" s="124"/>
+      <c r="AH11" s="124"/>
+      <c r="AI11" s="124"/>
+      <c r="AJ11" s="124"/>
+      <c r="AK11" s="124"/>
+      <c r="AL11" s="124"/>
+      <c r="AM11" s="124"/>
+      <c r="AN11" s="124"/>
+      <c r="AO11" s="261"/>
+      <c r="AP11" s="124"/>
+      <c r="AQ11" s="124"/>
+      <c r="AR11" s="124"/>
+      <c r="AS11" s="124"/>
+      <c r="AT11" s="124"/>
+      <c r="AU11" s="124"/>
+      <c r="AV11" s="124"/>
+      <c r="AW11" s="124"/>
+      <c r="AX11" s="124"/>
+      <c r="AY11" s="124"/>
+      <c r="AZ11" s="124"/>
+      <c r="BA11" s="124"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="124">
+        <v>82</v>
+      </c>
+      <c r="B12" t="s" s="124">
+        <v>96</v>
+      </c>
+      <c r="C12" t="s" s="124">
+        <v>97</v>
+      </c>
+      <c r="D12" t="s" s="124">
+        <v>83</v>
+      </c>
+      <c r="E12" t="s" s="124">
+        <v>98</v>
+      </c>
+      <c r="F12" s="124"/>
+      <c r="G12" s="124"/>
+      <c r="H12" s="124"/>
+      <c r="I12" s="124"/>
+      <c r="J12" s="124"/>
+      <c r="K12" s="262"/>
+      <c r="L12" s="263"/>
+      <c r="M12" s="264"/>
+      <c r="N12" s="265"/>
+      <c r="O12" s="266"/>
+      <c r="P12" s="267"/>
+      <c r="Q12" s="268"/>
+      <c r="R12" s="269"/>
+      <c r="S12" s="270"/>
+      <c r="T12" s="271"/>
+      <c r="U12" s="272"/>
+      <c r="V12" s="273"/>
+      <c r="W12" s="274"/>
+      <c r="X12" s="275"/>
+      <c r="Y12" s="276"/>
+      <c r="Z12" s="277"/>
+      <c r="AA12" s="278"/>
+      <c r="AB12" s="279"/>
+      <c r="AC12" s="280"/>
+      <c r="AD12" s="281"/>
+      <c r="AE12" s="282"/>
+      <c r="AF12" s="283"/>
+      <c r="AG12" s="284"/>
+      <c r="AH12" s="285"/>
+      <c r="AI12" s="124"/>
+      <c r="AJ12" s="124"/>
+      <c r="AK12" s="124"/>
+      <c r="AL12" s="124"/>
+      <c r="AM12" s="124"/>
+      <c r="AN12" s="124"/>
+      <c r="AO12" s="124"/>
+      <c r="AP12" s="124"/>
+      <c r="AQ12" s="124"/>
+      <c r="AR12" s="124"/>
+      <c r="AS12" s="124"/>
+      <c r="AT12" s="124"/>
+      <c r="AU12" s="124"/>
+      <c r="AV12" s="124"/>
+      <c r="AW12" s="124"/>
+      <c r="AX12" s="124"/>
+      <c r="AY12" s="124"/>
+      <c r="AZ12" s="124"/>
+      <c r="BA12" s="124"/>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="AD3:AE3"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AJ3:AK3"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="AN3:AO3"/>
+    <mergeCell ref="AP3:AQ3"/>
+    <mergeCell ref="AR3:AS3"/>
+    <mergeCell ref="AT3:AU3"/>
+    <mergeCell ref="AV3:AW3"/>
+    <mergeCell ref="AX3:AY3"/>
+    <mergeCell ref="AZ3:BA3"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
revrite heat of excell and data_rounding method
</commit_message>
<xml_diff>
--- a/sourse - копия.xlsx
+++ b/sourse - копия.xlsx
@@ -11,7 +11,7 @@
     <sheet name="01.10" sheetId="71" r:id="rId2"/>
     <sheet name="test" r:id="rId7" sheetId="72"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" refMode="R1C1"/>
 </workbook>
 </file>
 
@@ -3312,7 +3312,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="85">
+  <borders count="88">
     <border>
       <left/>
       <right/>
@@ -3837,6 +3837,51 @@
       </bottom>
     </border>
     <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <top style="medium"/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium"/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
       <right style="medium"/>
       <bottom style="medium"/>
     </border>
@@ -3944,42 +3989,41 @@
       </bottom>
     </border>
     <border>
-      <left style="thin"/>
+      <bottom style="thin"/>
     </border>
     <border>
-      <left style="thin"/>
       <top style="thin"/>
+      <bottom style="thin"/>
     </border>
     <border>
-      <left style="thin"/>
       <top style="thin"/>
-      <bottom>
+      <bottom style="thin">
         <color indexed="8"/>
       </bottom>
     </border>
     <border>
-      <left style="thin">
+      <left>
         <color indexed="8"/>
       </left>
       <top style="thin"/>
-      <bottom>
+      <bottom style="thin">
         <color indexed="8"/>
       </bottom>
     </border>
     <border>
-      <left style="thin">
+      <left>
         <color indexed="8"/>
       </left>
       <right>
         <color indexed="8"/>
       </right>
       <top style="thin"/>
-      <bottom>
+      <bottom style="thin">
         <color indexed="8"/>
       </bottom>
     </border>
     <border>
-      <left style="thin">
+      <left>
         <color indexed="8"/>
       </left>
       <right>
@@ -3988,51 +4032,50 @@
       <top style="thin">
         <color indexed="8"/>
       </top>
-      <bottom>
+      <bottom style="thin">
         <color indexed="8"/>
       </bottom>
     </border>
     <border>
-      <left style="thin"/>
       <right style="thin"/>
+      <bottom style="thin"/>
     </border>
     <border>
-      <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
+      <bottom style="thin"/>
     </border>
     <border>
-      <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
-      <bottom>
+      <bottom style="thin">
         <color indexed="8"/>
       </bottom>
     </border>
     <border>
-      <left style="thin">
+      <left>
         <color indexed="8"/>
       </left>
       <right style="thin"/>
       <top style="thin"/>
-      <bottom>
+      <bottom style="thin">
         <color indexed="8"/>
       </bottom>
     </border>
     <border>
-      <left style="thin">
+      <left>
         <color indexed="8"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="thin"/>
-      <bottom>
+      <bottom style="thin">
         <color indexed="8"/>
       </bottom>
     </border>
     <border>
-      <left style="thin">
+      <left>
         <color indexed="8"/>
       </left>
       <right style="thin">
@@ -4041,12 +4084,9 @@
       <top style="thin">
         <color indexed="8"/>
       </top>
-      <bottom>
+      <bottom style="thin">
         <color indexed="8"/>
       </bottom>
-    </border>
-    <border>
-      <bottom style="thin"/>
     </border>
     <border>
       <left style="thin"/>
@@ -4110,16 +4150,12 @@
     <border>
       <right style="thin"/>
     </border>
-    <border>
-      <right style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="286">
+  <cellXfs count="287">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4298,6 +4334,18 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4310,28 +4358,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="57" xfId="0" applyFill="true" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="62" xfId="0" applyFill="true" applyBorder="true">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="30" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
@@ -4350,187 +4386,191 @@
       <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="55" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="54" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="62" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="60" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="68" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="67" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="74" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="73" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="82" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="79" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="84" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="86" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" indent="0" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="74" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -7556,7 +7596,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AH12" sqref="AH12"/>
-      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
+      <selection pane="bottomLeft" activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7579,63 +7619,63 @@
       </c>
     </row>
     <row r="2" spans="1:53" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="104" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="111"/>
+      <c r="B2" s="104"/>
       <c r="C2" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="112" t="s">
+      <c r="F2" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
-      <c r="J2" s="112"/>
-      <c r="K2" s="112"/>
-      <c r="L2" s="112"/>
-      <c r="M2" s="112"/>
-      <c r="N2" s="112"/>
-      <c r="O2" s="112"/>
-      <c r="P2" s="112"/>
-      <c r="Q2" s="112"/>
-      <c r="R2" s="112"/>
-      <c r="S2" s="112"/>
-      <c r="T2" s="112"/>
-      <c r="U2" s="112"/>
-      <c r="V2" s="112"/>
-      <c r="W2" s="112"/>
-      <c r="X2" s="112"/>
-      <c r="Y2" s="112"/>
-      <c r="Z2" s="112"/>
-      <c r="AA2" s="112"/>
-      <c r="AB2" s="112"/>
-      <c r="AC2" s="112"/>
-      <c r="AD2" s="112"/>
-      <c r="AE2" s="112"/>
-      <c r="AF2" s="112"/>
-      <c r="AG2" s="112"/>
-      <c r="AH2" s="112"/>
-      <c r="AI2" s="112"/>
-      <c r="AJ2" s="112"/>
-      <c r="AK2" s="112"/>
-      <c r="AL2" s="112"/>
-      <c r="AM2" s="112"/>
-      <c r="AN2" s="112"/>
-      <c r="AO2" s="112"/>
-      <c r="AP2" s="112"/>
-      <c r="AQ2" s="112"/>
-      <c r="AR2" s="112"/>
-      <c r="AS2" s="112"/>
-      <c r="AT2" s="112"/>
-      <c r="AU2" s="112"/>
-      <c r="AV2" s="112"/>
-      <c r="AW2" s="112"/>
-      <c r="AX2" s="112"/>
-      <c r="AY2" s="112"/>
-      <c r="AZ2" s="112"/>
-      <c r="BA2" s="112"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105"/>
+      <c r="P2" s="105"/>
+      <c r="Q2" s="105"/>
+      <c r="R2" s="105"/>
+      <c r="S2" s="105"/>
+      <c r="T2" s="105"/>
+      <c r="U2" s="105"/>
+      <c r="V2" s="105"/>
+      <c r="W2" s="105"/>
+      <c r="X2" s="105"/>
+      <c r="Y2" s="105"/>
+      <c r="Z2" s="105"/>
+      <c r="AA2" s="105"/>
+      <c r="AB2" s="105"/>
+      <c r="AC2" s="105"/>
+      <c r="AD2" s="105"/>
+      <c r="AE2" s="105"/>
+      <c r="AF2" s="105"/>
+      <c r="AG2" s="105"/>
+      <c r="AH2" s="105"/>
+      <c r="AI2" s="105"/>
+      <c r="AJ2" s="105"/>
+      <c r="AK2" s="105"/>
+      <c r="AL2" s="105"/>
+      <c r="AM2" s="105"/>
+      <c r="AN2" s="105"/>
+      <c r="AO2" s="105"/>
+      <c r="AP2" s="105"/>
+      <c r="AQ2" s="105"/>
+      <c r="AR2" s="105"/>
+      <c r="AS2" s="105"/>
+      <c r="AT2" s="105"/>
+      <c r="AU2" s="105"/>
+      <c r="AV2" s="105"/>
+      <c r="AW2" s="105"/>
+      <c r="AX2" s="105"/>
+      <c r="AY2" s="105"/>
+      <c r="AZ2" s="105"/>
+      <c r="BA2" s="105"/>
     </row>
     <row r="3" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
@@ -7653,102 +7693,102 @@
       <c r="E3" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="108">
+      <c r="F3" s="106">
         <v>7</v>
       </c>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108">
+      <c r="G3" s="106"/>
+      <c r="H3" s="106">
         <v>8</v>
       </c>
-      <c r="I3" s="108"/>
-      <c r="J3" s="108">
+      <c r="I3" s="106"/>
+      <c r="J3" s="106">
         <v>9</v>
       </c>
-      <c r="K3" s="108"/>
-      <c r="L3" s="108">
+      <c r="K3" s="106"/>
+      <c r="L3" s="106">
         <v>10</v>
       </c>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108">
+      <c r="M3" s="106"/>
+      <c r="N3" s="106">
         <v>11</v>
       </c>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108">
+      <c r="O3" s="106"/>
+      <c r="P3" s="106">
         <v>12</v>
       </c>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="108">
+      <c r="Q3" s="106"/>
+      <c r="R3" s="106">
         <v>13</v>
       </c>
-      <c r="S3" s="108"/>
-      <c r="T3" s="108">
+      <c r="S3" s="106"/>
+      <c r="T3" s="106">
         <v>14</v>
       </c>
-      <c r="U3" s="108"/>
-      <c r="V3" s="108">
+      <c r="U3" s="106"/>
+      <c r="V3" s="106">
         <v>15</v>
       </c>
-      <c r="W3" s="108"/>
-      <c r="X3" s="108">
+      <c r="W3" s="106"/>
+      <c r="X3" s="106">
         <v>16</v>
       </c>
-      <c r="Y3" s="108"/>
-      <c r="Z3" s="110">
+      <c r="Y3" s="106"/>
+      <c r="Z3" s="113">
         <v>17</v>
       </c>
-      <c r="AA3" s="110"/>
-      <c r="AB3" s="110">
+      <c r="AA3" s="113"/>
+      <c r="AB3" s="113">
         <v>18</v>
       </c>
-      <c r="AC3" s="110"/>
-      <c r="AD3" s="108">
+      <c r="AC3" s="113"/>
+      <c r="AD3" s="106">
         <v>19</v>
       </c>
-      <c r="AE3" s="108"/>
-      <c r="AF3" s="108">
+      <c r="AE3" s="106"/>
+      <c r="AF3" s="106">
         <v>20</v>
       </c>
-      <c r="AG3" s="108"/>
-      <c r="AH3" s="108">
+      <c r="AG3" s="106"/>
+      <c r="AH3" s="106">
         <v>21</v>
       </c>
-      <c r="AI3" s="108"/>
-      <c r="AJ3" s="108">
+      <c r="AI3" s="106"/>
+      <c r="AJ3" s="106">
         <v>22</v>
       </c>
-      <c r="AK3" s="108"/>
-      <c r="AL3" s="108">
+      <c r="AK3" s="106"/>
+      <c r="AL3" s="106">
         <v>23</v>
       </c>
-      <c r="AM3" s="108"/>
-      <c r="AN3" s="108">
+      <c r="AM3" s="106"/>
+      <c r="AN3" s="106">
         <v>24</v>
       </c>
-      <c r="AO3" s="108"/>
-      <c r="AP3" s="108">
+      <c r="AO3" s="106"/>
+      <c r="AP3" s="106">
         <v>1</v>
       </c>
-      <c r="AQ3" s="108"/>
-      <c r="AR3" s="108">
+      <c r="AQ3" s="106"/>
+      <c r="AR3" s="106">
         <v>2</v>
       </c>
-      <c r="AS3" s="108"/>
-      <c r="AT3" s="108">
+      <c r="AS3" s="106"/>
+      <c r="AT3" s="106">
         <v>3</v>
       </c>
-      <c r="AU3" s="108"/>
-      <c r="AV3" s="108">
+      <c r="AU3" s="106"/>
+      <c r="AV3" s="106">
         <v>4</v>
       </c>
-      <c r="AW3" s="108"/>
-      <c r="AX3" s="108">
+      <c r="AW3" s="106"/>
+      <c r="AX3" s="106">
         <v>5</v>
       </c>
-      <c r="AY3" s="108"/>
-      <c r="AZ3" s="108">
+      <c r="AY3" s="106"/>
+      <c r="AZ3" s="106">
         <v>6</v>
       </c>
-      <c r="BA3" s="113"/>
+      <c r="BA3" s="107"/>
     </row>
     <row r="4" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="94" t="s">
@@ -7808,7 +7848,7 @@
       <c r="BA4" s="97"/>
     </row>
     <row r="5" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="104" t="s">
+      <c r="A5" s="108" t="s">
         <v>72</v>
       </c>
       <c r="B5" s="59" t="s">
@@ -7875,7 +7915,7 @@
       <c r="BA5" s="50"/>
     </row>
     <row r="6" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="107"/>
+      <c r="A6" s="111"/>
       <c r="B6" s="34" t="s">
         <v>62</v>
       </c>
@@ -7942,7 +7982,7 @@
       <c r="BA6" s="51"/>
     </row>
     <row r="7" spans="1:53" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="105"/>
+      <c r="A7" s="109"/>
       <c r="B7" s="40" t="s">
         <v>62</v>
       </c>
@@ -8007,7 +8047,7 @@
       <c r="BA7" s="57"/>
     </row>
     <row r="8" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="106" t="s">
+      <c r="A8" s="110" t="s">
         <v>67</v>
       </c>
       <c r="B8" s="38" t="s">
@@ -8074,7 +8114,7 @@
       <c r="BA8" s="74"/>
     </row>
     <row r="9" spans="1:53" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="109"/>
+      <c r="A9" s="112"/>
       <c r="B9" s="87" t="s">
         <v>32</v>
       </c>
@@ -8137,7 +8177,7 @@
       <c r="BA9" s="70"/>
     </row>
     <row r="10" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="104" t="s">
+      <c r="A10" s="108" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="59" t="s">
@@ -8202,7 +8242,7 @@
       <c r="BA10" s="50"/>
     </row>
     <row r="11" spans="1:53" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="105"/>
+      <c r="A11" s="109"/>
       <c r="B11" s="40" t="s">
         <v>69</v>
       </c>
@@ -8261,7 +8301,7 @@
       <c r="BA11" s="57"/>
     </row>
     <row r="12" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="106" t="s">
+      <c r="A12" s="110" t="s">
         <v>70</v>
       </c>
       <c r="B12" s="58" t="s">
@@ -8330,7 +8370,7 @@
       <c r="BA12" s="71"/>
     </row>
     <row r="13" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="107"/>
+      <c r="A13" s="111"/>
       <c r="B13" s="34" t="s">
         <v>24</v>
       </c>
@@ -8397,7 +8437,7 @@
       <c r="BA13" s="51"/>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A14" s="107"/>
+      <c r="A14" s="111"/>
       <c r="B14" s="34" t="s">
         <v>24</v>
       </c>
@@ -8462,7 +8502,7 @@
       <c r="BA14" s="51"/>
     </row>
     <row r="15" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A15" s="107"/>
+      <c r="A15" s="111"/>
       <c r="B15" s="34" t="s">
         <v>24</v>
       </c>
@@ -8525,7 +8565,7 @@
       <c r="BA15" s="51"/>
     </row>
     <row r="16" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="107"/>
+      <c r="A16" s="111"/>
       <c r="B16" s="34" t="s">
         <v>45</v>
       </c>
@@ -8586,7 +8626,7 @@
       <c r="BA16" s="51"/>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A17" s="107"/>
+      <c r="A17" s="111"/>
       <c r="B17" s="34" t="s">
         <v>24</v>
       </c>
@@ -8651,7 +8691,7 @@
       <c r="BA17" s="51"/>
     </row>
     <row r="18" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="105"/>
+      <c r="A18" s="109"/>
       <c r="B18" s="40" t="s">
         <v>24</v>
       </c>
@@ -8716,7 +8756,7 @@
       <c r="BA18" s="57"/>
     </row>
     <row r="19" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="106" t="s">
+      <c r="A19" s="110" t="s">
         <v>71</v>
       </c>
       <c r="B19" s="38" t="s">
@@ -8783,7 +8823,7 @@
       <c r="BA19" s="71"/>
     </row>
     <row r="20" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A20" s="107"/>
+      <c r="A20" s="111"/>
       <c r="B20" s="41" t="s">
         <v>32</v>
       </c>
@@ -8846,7 +8886,7 @@
       <c r="BA20" s="51"/>
     </row>
     <row r="21" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="105"/>
+      <c r="A21" s="109"/>
       <c r="B21" s="60" t="s">
         <v>32</v>
       </c>
@@ -9369,21 +9409,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:BA2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="AX3:AY3"/>
-    <mergeCell ref="AZ3:BA3"/>
-    <mergeCell ref="AN3:AO3"/>
-    <mergeCell ref="AP3:AQ3"/>
-    <mergeCell ref="AR3:AS3"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A18"/>
     <mergeCell ref="A19:A21"/>
@@ -9400,6 +9425,21 @@
     <mergeCell ref="AB3:AC3"/>
     <mergeCell ref="AD3:AE3"/>
     <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:BA2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="AX3:AY3"/>
+    <mergeCell ref="AZ3:BA3"/>
+    <mergeCell ref="AN3:AO3"/>
+    <mergeCell ref="AP3:AQ3"/>
+    <mergeCell ref="AR3:AS3"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>
@@ -9420,54 +9460,102 @@
     <col min="3" max="3" width="11.42578125" customWidth="true"/>
     <col min="4" max="4" width="25.85546875" customWidth="true"/>
     <col min="5" max="5" width="22.140625" customWidth="true"/>
-    <col min="6" max="6" width="3.28515625" customWidth="true"/>
-    <col min="7" max="7" width="3.28515625" customWidth="true"/>
-    <col min="8" max="8" width="3.28515625" customWidth="true"/>
-    <col min="9" max="9" width="3.28515625" customWidth="true"/>
-    <col min="10" max="10" width="3.28515625" customWidth="true"/>
-    <col min="11" max="11" width="3.28515625" customWidth="true"/>
-    <col min="12" max="12" width="3.28515625" customWidth="true"/>
-    <col min="13" max="13" width="3.28515625" customWidth="true"/>
-    <col min="14" max="14" width="3.28515625" customWidth="true"/>
-    <col min="15" max="15" width="3.28515625" customWidth="true"/>
-    <col min="16" max="16" width="3.28515625" customWidth="true"/>
-    <col min="17" max="17" width="3.28515625" customWidth="true"/>
-    <col min="18" max="18" width="3.28515625" customWidth="true"/>
-    <col min="19" max="19" width="3.28515625" customWidth="true"/>
-    <col min="20" max="20" width="3.28515625" customWidth="true"/>
-    <col min="21" max="21" width="3.28515625" customWidth="true"/>
-    <col min="22" max="22" width="3.28515625" customWidth="true"/>
-    <col min="23" max="23" width="3.28515625" customWidth="true"/>
-    <col min="24" max="24" width="3.28515625" customWidth="true"/>
-    <col min="25" max="25" width="3.28515625" customWidth="true"/>
-    <col min="26" max="26" width="3.28515625" customWidth="true"/>
-    <col min="27" max="27" width="3.28515625" customWidth="true"/>
-    <col min="28" max="28" width="3.28515625" customWidth="true"/>
-    <col min="29" max="29" width="3.28515625" customWidth="true"/>
-    <col min="30" max="30" width="3.28515625" customWidth="true"/>
-    <col min="31" max="31" width="3.28515625" customWidth="true"/>
-    <col min="32" max="32" width="3.28515625" customWidth="true"/>
-    <col min="33" max="33" width="3.28515625" customWidth="true"/>
-    <col min="34" max="34" width="3.28515625" customWidth="true"/>
-    <col min="35" max="35" width="3.28515625" customWidth="true"/>
-    <col min="36" max="36" width="3.28515625" customWidth="true"/>
-    <col min="37" max="37" width="3.28515625" customWidth="true"/>
-    <col min="38" max="38" width="3.28515625" customWidth="true"/>
-    <col min="39" max="39" width="3.28515625" customWidth="true"/>
-    <col min="40" max="40" width="3.28515625" customWidth="true"/>
-    <col min="41" max="41" width="3.28515625" customWidth="true"/>
-    <col min="42" max="42" width="3.28515625" customWidth="true"/>
-    <col min="43" max="43" width="3.28515625" customWidth="true"/>
-    <col min="44" max="44" width="3.28515625" customWidth="true"/>
-    <col min="45" max="45" width="3.28515625" customWidth="true"/>
-    <col min="46" max="46" width="3.28515625" customWidth="true"/>
-    <col min="47" max="47" width="3.28515625" customWidth="true"/>
-    <col min="48" max="48" width="3.28515625" customWidth="true"/>
-    <col min="49" max="49" width="3.28515625" customWidth="true"/>
-    <col min="50" max="50" width="3.28515625" customWidth="true"/>
-    <col min="51" max="51" width="3.28515625" customWidth="true"/>
-    <col min="52" max="52" width="3.28515625" customWidth="true"/>
-    <col min="53" max="53" width="3.28515625" customWidth="true"/>
+    <col min="6" max="6" width="1.640625" customWidth="true"/>
+    <col min="7" max="7" width="1.640625" customWidth="true"/>
+    <col min="8" max="8" width="1.640625" customWidth="true"/>
+    <col min="9" max="9" width="1.640625" customWidth="true"/>
+    <col min="10" max="10" width="1.640625" customWidth="true"/>
+    <col min="11" max="11" width="1.640625" customWidth="true"/>
+    <col min="12" max="12" width="1.640625" customWidth="true"/>
+    <col min="13" max="13" width="1.640625" customWidth="true"/>
+    <col min="14" max="14" width="1.640625" customWidth="true"/>
+    <col min="15" max="15" width="1.640625" customWidth="true"/>
+    <col min="16" max="16" width="1.640625" customWidth="true"/>
+    <col min="17" max="17" width="1.640625" customWidth="true"/>
+    <col min="18" max="18" width="1.640625" customWidth="true"/>
+    <col min="19" max="19" width="1.640625" customWidth="true"/>
+    <col min="20" max="20" width="1.640625" customWidth="true"/>
+    <col min="21" max="21" width="1.640625" customWidth="true"/>
+    <col min="22" max="22" width="1.640625" customWidth="true"/>
+    <col min="23" max="23" width="1.640625" customWidth="true"/>
+    <col min="24" max="24" width="1.640625" customWidth="true"/>
+    <col min="25" max="25" width="1.640625" customWidth="true"/>
+    <col min="26" max="26" width="1.640625" customWidth="true"/>
+    <col min="27" max="27" width="1.640625" customWidth="true"/>
+    <col min="28" max="28" width="1.640625" customWidth="true"/>
+    <col min="29" max="29" width="1.640625" customWidth="true"/>
+    <col min="30" max="30" width="1.640625" customWidth="true"/>
+    <col min="31" max="31" width="1.640625" customWidth="true"/>
+    <col min="32" max="32" width="1.640625" customWidth="true"/>
+    <col min="33" max="33" width="1.640625" customWidth="true"/>
+    <col min="34" max="34" width="1.640625" customWidth="true"/>
+    <col min="35" max="35" width="1.640625" customWidth="true"/>
+    <col min="36" max="36" width="1.640625" customWidth="true"/>
+    <col min="37" max="37" width="1.640625" customWidth="true"/>
+    <col min="38" max="38" width="1.640625" customWidth="true"/>
+    <col min="39" max="39" width="1.640625" customWidth="true"/>
+    <col min="40" max="40" width="1.640625" customWidth="true"/>
+    <col min="41" max="41" width="1.640625" customWidth="true"/>
+    <col min="42" max="42" width="1.640625" customWidth="true"/>
+    <col min="43" max="43" width="1.640625" customWidth="true"/>
+    <col min="44" max="44" width="1.640625" customWidth="true"/>
+    <col min="45" max="45" width="1.640625" customWidth="true"/>
+    <col min="46" max="46" width="1.640625" customWidth="true"/>
+    <col min="47" max="47" width="1.640625" customWidth="true"/>
+    <col min="48" max="48" width="1.640625" customWidth="true"/>
+    <col min="49" max="49" width="1.640625" customWidth="true"/>
+    <col min="50" max="50" width="1.640625" customWidth="true"/>
+    <col min="51" max="51" width="1.640625" customWidth="true"/>
+    <col min="52" max="52" width="1.640625" customWidth="true"/>
+    <col min="53" max="53" width="1.640625" customWidth="true"/>
+    <col min="54" max="54" width="1.640625" customWidth="true"/>
+    <col min="55" max="55" width="1.640625" customWidth="true"/>
+    <col min="56" max="56" width="1.640625" customWidth="true"/>
+    <col min="57" max="57" width="1.640625" customWidth="true"/>
+    <col min="58" max="58" width="1.640625" customWidth="true"/>
+    <col min="59" max="59" width="1.640625" customWidth="true"/>
+    <col min="60" max="60" width="1.640625" customWidth="true"/>
+    <col min="61" max="61" width="1.640625" customWidth="true"/>
+    <col min="62" max="62" width="1.640625" customWidth="true"/>
+    <col min="63" max="63" width="1.640625" customWidth="true"/>
+    <col min="64" max="64" width="1.640625" customWidth="true"/>
+    <col min="65" max="65" width="1.640625" customWidth="true"/>
+    <col min="66" max="66" width="1.640625" customWidth="true"/>
+    <col min="67" max="67" width="1.640625" customWidth="true"/>
+    <col min="68" max="68" width="1.640625" customWidth="true"/>
+    <col min="69" max="69" width="1.640625" customWidth="true"/>
+    <col min="70" max="70" width="1.640625" customWidth="true"/>
+    <col min="71" max="71" width="1.640625" customWidth="true"/>
+    <col min="72" max="72" width="1.640625" customWidth="true"/>
+    <col min="73" max="73" width="1.640625" customWidth="true"/>
+    <col min="74" max="74" width="1.640625" customWidth="true"/>
+    <col min="75" max="75" width="1.640625" customWidth="true"/>
+    <col min="76" max="76" width="1.640625" customWidth="true"/>
+    <col min="77" max="77" width="1.640625" customWidth="true"/>
+    <col min="78" max="78" width="1.640625" customWidth="true"/>
+    <col min="79" max="79" width="1.640625" customWidth="true"/>
+    <col min="80" max="80" width="1.640625" customWidth="true"/>
+    <col min="81" max="81" width="1.640625" customWidth="true"/>
+    <col min="82" max="82" width="1.640625" customWidth="true"/>
+    <col min="83" max="83" width="1.640625" customWidth="true"/>
+    <col min="84" max="84" width="1.640625" customWidth="true"/>
+    <col min="85" max="85" width="1.640625" customWidth="true"/>
+    <col min="86" max="86" width="1.640625" customWidth="true"/>
+    <col min="87" max="87" width="1.640625" customWidth="true"/>
+    <col min="88" max="88" width="1.640625" customWidth="true"/>
+    <col min="89" max="89" width="1.640625" customWidth="true"/>
+    <col min="90" max="90" width="1.640625" customWidth="true"/>
+    <col min="91" max="91" width="1.640625" customWidth="true"/>
+    <col min="92" max="92" width="1.640625" customWidth="true"/>
+    <col min="93" max="93" width="1.640625" customWidth="true"/>
+    <col min="94" max="94" width="1.640625" customWidth="true"/>
+    <col min="95" max="95" width="1.640625" customWidth="true"/>
+    <col min="96" max="96" width="1.640625" customWidth="true"/>
+    <col min="97" max="97" width="1.640625" customWidth="true"/>
+    <col min="98" max="98" width="1.640625" customWidth="true"/>
+    <col min="99" max="99" width="1.640625" customWidth="true"/>
+    <col min="100" max="100" width="1.640625" customWidth="true"/>
+    <col min="101" max="101" width="1.640625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -9495,701 +9583,1181 @@
         <v>7.0</v>
       </c>
       <c r="G3" s="120"/>
-      <c r="H3" t="n" s="115">
+      <c r="H3" s="120"/>
+      <c r="I3" s="121"/>
+      <c r="J3" t="n" s="115">
         <v>8.0</v>
       </c>
-      <c r="I3" s="120"/>
-      <c r="J3" t="n" s="115">
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
+      <c r="M3" s="121"/>
+      <c r="N3" t="n" s="115">
         <v>9.0</v>
       </c>
-      <c r="K3" s="120"/>
-      <c r="L3" t="n" s="115">
+      <c r="O3" s="120"/>
+      <c r="P3" s="120"/>
+      <c r="Q3" s="121"/>
+      <c r="R3" t="n" s="115">
         <v>10.0</v>
       </c>
-      <c r="M3" s="120"/>
-      <c r="N3" t="n" s="115">
+      <c r="S3" s="120"/>
+      <c r="T3" s="120"/>
+      <c r="U3" s="121"/>
+      <c r="V3" t="n" s="115">
         <v>11.0</v>
       </c>
-      <c r="O3" s="120"/>
-      <c r="P3" t="n" s="115">
+      <c r="W3" s="120"/>
+      <c r="X3" s="120"/>
+      <c r="Y3" s="121"/>
+      <c r="Z3" t="n" s="115">
         <v>12.0</v>
       </c>
-      <c r="Q3" s="120"/>
-      <c r="R3" t="n" s="115">
+      <c r="AA3" s="120"/>
+      <c r="AB3" s="120"/>
+      <c r="AC3" s="121"/>
+      <c r="AD3" t="n" s="115">
         <v>13.0</v>
       </c>
-      <c r="S3" s="120"/>
-      <c r="T3" t="n" s="115">
+      <c r="AE3" s="120"/>
+      <c r="AF3" s="120"/>
+      <c r="AG3" s="121"/>
+      <c r="AH3" t="n" s="115">
         <v>14.0</v>
       </c>
-      <c r="U3" s="120"/>
-      <c r="V3" t="n" s="115">
+      <c r="AI3" s="120"/>
+      <c r="AJ3" s="120"/>
+      <c r="AK3" s="121"/>
+      <c r="AL3" t="n" s="115">
         <v>15.0</v>
       </c>
-      <c r="W3" s="120"/>
-      <c r="X3" t="n" s="115">
+      <c r="AM3" s="120"/>
+      <c r="AN3" s="120"/>
+      <c r="AO3" s="121"/>
+      <c r="AP3" t="n" s="115">
         <v>16.0</v>
       </c>
-      <c r="Y3" s="120"/>
-      <c r="Z3" t="n" s="115">
+      <c r="AQ3" s="120"/>
+      <c r="AR3" s="120"/>
+      <c r="AS3" s="121"/>
+      <c r="AT3" t="n" s="115">
         <v>17.0</v>
       </c>
-      <c r="AA3" s="120"/>
-      <c r="AB3" t="n" s="115">
+      <c r="AU3" s="120"/>
+      <c r="AV3" s="120"/>
+      <c r="AW3" s="121"/>
+      <c r="AX3" t="n" s="115">
         <v>18.0</v>
       </c>
-      <c r="AC3" s="120"/>
-      <c r="AD3" t="n" s="115">
+      <c r="AY3" s="120"/>
+      <c r="AZ3" s="120"/>
+      <c r="BA3" s="121"/>
+      <c r="BB3" t="n" s="115">
         <v>19.0</v>
       </c>
-      <c r="AE3" s="120"/>
-      <c r="AF3" t="n" s="115">
+      <c r="BC3" s="120"/>
+      <c r="BD3" s="120"/>
+      <c r="BE3" s="121"/>
+      <c r="BF3" t="n" s="115">
         <v>20.0</v>
       </c>
-      <c r="AG3" s="120"/>
-      <c r="AH3" t="n" s="115">
+      <c r="BG3" s="120"/>
+      <c r="BH3" s="120"/>
+      <c r="BI3" s="121"/>
+      <c r="BJ3" t="n" s="115">
         <v>21.0</v>
       </c>
-      <c r="AI3" s="120"/>
-      <c r="AJ3" t="n" s="115">
+      <c r="BK3" s="120"/>
+      <c r="BL3" s="120"/>
+      <c r="BM3" s="121"/>
+      <c r="BN3" t="n" s="115">
         <v>22.0</v>
       </c>
-      <c r="AK3" s="120"/>
-      <c r="AL3" t="n" s="115">
+      <c r="BO3" s="120"/>
+      <c r="BP3" s="120"/>
+      <c r="BQ3" s="121"/>
+      <c r="BR3" t="n" s="115">
         <v>23.0</v>
       </c>
-      <c r="AM3" s="120"/>
-      <c r="AN3" t="n" s="115">
+      <c r="BS3" s="120"/>
+      <c r="BT3" s="120"/>
+      <c r="BU3" s="121"/>
+      <c r="BV3" t="n" s="115">
         <v>24.0</v>
       </c>
-      <c r="AO3" s="120"/>
-      <c r="AP3" t="n" s="115">
+      <c r="BW3" s="120"/>
+      <c r="BX3" s="120"/>
+      <c r="BY3" s="121"/>
+      <c r="BZ3" t="n" s="115">
         <v>1.0</v>
       </c>
-      <c r="AQ3" s="120"/>
-      <c r="AR3" t="n" s="115">
+      <c r="CA3" s="120"/>
+      <c r="CB3" s="120"/>
+      <c r="CC3" s="121"/>
+      <c r="CD3" t="n" s="115">
         <v>2.0</v>
       </c>
-      <c r="AS3" s="120"/>
-      <c r="AT3" t="n" s="115">
+      <c r="CE3" s="120"/>
+      <c r="CF3" s="120"/>
+      <c r="CG3" s="121"/>
+      <c r="CH3" t="n" s="115">
         <v>3.0</v>
       </c>
-      <c r="AU3" s="120"/>
-      <c r="AV3" t="n" s="115">
+      <c r="CI3" s="120"/>
+      <c r="CJ3" s="120"/>
+      <c r="CK3" s="121"/>
+      <c r="CL3" t="n" s="115">
         <v>4.0</v>
       </c>
-      <c r="AW3" s="120"/>
-      <c r="AX3" t="n" s="115">
+      <c r="CM3" s="120"/>
+      <c r="CN3" s="120"/>
+      <c r="CO3" s="121"/>
+      <c r="CP3" t="n" s="115">
         <v>5.0</v>
       </c>
-      <c r="AY3" s="120"/>
-      <c r="AZ3" t="n" s="115">
+      <c r="CQ3" s="120"/>
+      <c r="CR3" s="120"/>
+      <c r="CS3" s="121"/>
+      <c r="CT3" t="n" s="115">
         <v>6.0</v>
       </c>
-      <c r="BA3" s="120"/>
+      <c r="CU3" s="120"/>
+      <c r="CV3" s="120"/>
+      <c r="CW3" s="121"/>
     </row>
     <row r="4">
-      <c r="A4" s="124"/>
-      <c r="B4" s="124"/>
-      <c r="C4" s="124"/>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="124"/>
-      <c r="H4" s="124"/>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
-      <c r="K4" s="124"/>
-      <c r="L4" s="124"/>
-      <c r="M4" s="124"/>
-      <c r="N4" s="124"/>
-      <c r="O4" s="124"/>
-      <c r="P4" s="124"/>
-      <c r="Q4" s="124"/>
-      <c r="R4" s="124"/>
-      <c r="S4" s="124"/>
-      <c r="T4" s="124"/>
-      <c r="U4" s="124"/>
-      <c r="V4" s="124"/>
-      <c r="W4" s="124"/>
-      <c r="X4" s="124"/>
-      <c r="Y4" s="124"/>
-      <c r="Z4" s="124"/>
-      <c r="AA4" s="124"/>
-      <c r="AB4" s="124"/>
-      <c r="AC4" s="124"/>
-      <c r="AD4" s="124"/>
-      <c r="AE4" s="124"/>
-      <c r="AF4" s="124"/>
-      <c r="AG4" s="124"/>
-      <c r="AH4" s="124"/>
-      <c r="AI4" s="124"/>
-      <c r="AJ4" s="124"/>
-      <c r="AK4" s="124"/>
-      <c r="AL4" s="124"/>
-      <c r="AM4" s="124"/>
-      <c r="AN4" s="124"/>
-      <c r="AO4" s="124"/>
-      <c r="AP4" s="124"/>
-      <c r="AQ4" s="124"/>
-      <c r="AR4" s="124"/>
-      <c r="AS4" s="124"/>
-      <c r="AT4" s="124"/>
-      <c r="AU4" s="124"/>
-      <c r="AV4" s="124"/>
-      <c r="AW4" s="124"/>
-      <c r="AX4" s="124"/>
-      <c r="AY4" s="124"/>
-      <c r="AZ4" s="124"/>
-      <c r="BA4" s="124"/>
+      <c r="A4" s="125"/>
+      <c r="B4" s="125"/>
+      <c r="C4" s="125"/>
+      <c r="D4" s="125"/>
+      <c r="E4" s="125"/>
+      <c r="F4" s="123"/>
+      <c r="G4" s="123"/>
+      <c r="H4" s="123"/>
+      <c r="I4" s="123"/>
+      <c r="J4" s="123"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="123"/>
+      <c r="M4" s="123"/>
+      <c r="N4" s="123"/>
+      <c r="O4" s="123"/>
+      <c r="P4" s="123"/>
+      <c r="Q4" s="123"/>
+      <c r="R4" s="123"/>
+      <c r="S4" s="123"/>
+      <c r="T4" s="123"/>
+      <c r="U4" s="123"/>
+      <c r="V4" s="123"/>
+      <c r="W4" s="123"/>
+      <c r="X4" s="123"/>
+      <c r="Y4" s="123"/>
+      <c r="Z4" s="123"/>
+      <c r="AA4" s="123"/>
+      <c r="AB4" s="123"/>
+      <c r="AC4" s="123"/>
+      <c r="AD4" s="123"/>
+      <c r="AE4" s="123"/>
+      <c r="AF4" s="123"/>
+      <c r="AG4" s="123"/>
+      <c r="AH4" s="123"/>
+      <c r="AI4" s="123"/>
+      <c r="AJ4" s="123"/>
+      <c r="AK4" s="123"/>
+      <c r="AL4" s="123"/>
+      <c r="AM4" s="123"/>
+      <c r="AN4" s="123"/>
+      <c r="AO4" s="123"/>
+      <c r="AP4" s="123"/>
+      <c r="AQ4" s="123"/>
+      <c r="AR4" s="123"/>
+      <c r="AS4" s="123"/>
+      <c r="AT4" s="123"/>
+      <c r="AU4" s="123"/>
+      <c r="AV4" s="123"/>
+      <c r="AW4" s="123"/>
+      <c r="AX4" s="123"/>
+      <c r="AY4" s="123"/>
+      <c r="AZ4" s="123"/>
+      <c r="BA4" s="123"/>
+      <c r="BB4" s="123"/>
+      <c r="BC4" s="123"/>
+      <c r="BD4" s="123"/>
+      <c r="BE4" s="123"/>
+      <c r="BF4" s="123"/>
+      <c r="BG4" s="123"/>
+      <c r="BH4" s="123"/>
+      <c r="BI4" s="123"/>
+      <c r="BJ4" s="123"/>
+      <c r="BK4" s="123"/>
+      <c r="BL4" s="123"/>
+      <c r="BM4" s="123"/>
+      <c r="BN4" s="123"/>
+      <c r="BO4" s="123"/>
+      <c r="BP4" s="123"/>
+      <c r="BQ4" s="123"/>
+      <c r="BR4" s="123"/>
+      <c r="BS4" s="123"/>
+      <c r="BT4" s="123"/>
+      <c r="BU4" s="123"/>
+      <c r="BV4" s="123"/>
+      <c r="BW4" s="123"/>
+      <c r="BX4" s="123"/>
+      <c r="BY4" s="123"/>
+      <c r="BZ4" s="123"/>
+      <c r="CA4" s="123"/>
+      <c r="CB4" s="123"/>
+      <c r="CC4" s="123"/>
+      <c r="CD4" s="123"/>
+      <c r="CE4" s="123"/>
+      <c r="CF4" s="123"/>
+      <c r="CG4" s="123"/>
+      <c r="CH4" s="123"/>
+      <c r="CI4" s="123"/>
+      <c r="CJ4" s="123"/>
+      <c r="CK4" s="123"/>
+      <c r="CL4" s="123"/>
+      <c r="CM4" s="123"/>
+      <c r="CN4" s="123"/>
+      <c r="CO4" s="123"/>
+      <c r="CP4" s="123"/>
+      <c r="CQ4" s="123"/>
+      <c r="CR4" s="123"/>
+      <c r="CS4" s="123"/>
+      <c r="CT4" s="123"/>
+      <c r="CU4" s="123"/>
+      <c r="CV4" s="123"/>
+      <c r="CW4" s="123"/>
     </row>
     <row r="5">
-      <c r="A5" t="s" s="124">
+      <c r="A5" t="s" s="125">
         <v>82</v>
       </c>
-      <c r="B5" t="s" s="124">
+      <c r="B5" t="s" s="125">
         <v>81</v>
       </c>
-      <c r="C5" t="s" s="124">
+      <c r="C5" t="s" s="125">
         <v>26</v>
       </c>
-      <c r="D5" t="s" s="124">
+      <c r="D5" t="s" s="125">
         <v>83</v>
       </c>
-      <c r="E5" t="s" s="124">
+      <c r="E5" t="s" s="125">
         <v>84</v>
       </c>
-      <c r="F5" s="124"/>
-      <c r="G5" s="124"/>
-      <c r="H5" s="124"/>
-      <c r="I5" s="124"/>
-      <c r="J5" s="124"/>
-      <c r="K5" s="125"/>
-      <c r="L5" s="126"/>
-      <c r="M5" s="127"/>
-      <c r="N5" s="128"/>
-      <c r="O5" s="129"/>
-      <c r="P5" s="130"/>
-      <c r="Q5" s="131"/>
-      <c r="R5" s="132"/>
-      <c r="S5" s="133"/>
-      <c r="T5" s="134"/>
-      <c r="U5" s="135"/>
-      <c r="V5" s="136"/>
-      <c r="W5" s="137"/>
-      <c r="X5" s="138"/>
-      <c r="Y5" s="139"/>
-      <c r="Z5" s="140"/>
-      <c r="AA5" s="141"/>
-      <c r="AB5" s="142"/>
-      <c r="AC5" s="143"/>
-      <c r="AD5" s="144"/>
-      <c r="AE5" s="145"/>
-      <c r="AF5" s="146"/>
-      <c r="AG5" s="147"/>
-      <c r="AH5" s="148"/>
-      <c r="AI5" s="149"/>
-      <c r="AJ5" s="124"/>
-      <c r="AK5" s="124"/>
-      <c r="AL5" s="124"/>
-      <c r="AM5" s="124"/>
-      <c r="AN5" s="124"/>
-      <c r="AO5" s="124"/>
-      <c r="AP5" s="124"/>
-      <c r="AQ5" s="124"/>
-      <c r="AR5" s="124"/>
-      <c r="AS5" s="124"/>
-      <c r="AT5" s="124"/>
-      <c r="AU5" s="124"/>
-      <c r="AV5" s="124"/>
-      <c r="AW5" s="124"/>
-      <c r="AX5" s="124"/>
-      <c r="AY5" s="124"/>
-      <c r="AZ5" s="124"/>
-      <c r="BA5" s="124"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="123"/>
+      <c r="H5" s="123"/>
+      <c r="I5" s="123"/>
+      <c r="J5" s="123"/>
+      <c r="K5" s="126"/>
+      <c r="L5" s="127"/>
+      <c r="M5" s="128"/>
+      <c r="N5" s="129"/>
+      <c r="O5" s="130"/>
+      <c r="P5" s="131"/>
+      <c r="Q5" s="132"/>
+      <c r="R5" s="133"/>
+      <c r="S5" s="134"/>
+      <c r="T5" s="135"/>
+      <c r="U5" s="136"/>
+      <c r="V5" s="137"/>
+      <c r="W5" s="138"/>
+      <c r="X5" s="139"/>
+      <c r="Y5" s="140"/>
+      <c r="Z5" s="141"/>
+      <c r="AA5" s="142"/>
+      <c r="AB5" s="143"/>
+      <c r="AC5" s="144"/>
+      <c r="AD5" s="145"/>
+      <c r="AE5" s="146"/>
+      <c r="AF5" s="147"/>
+      <c r="AG5" s="148"/>
+      <c r="AH5" s="149"/>
+      <c r="AI5" s="150"/>
+      <c r="AJ5" s="123"/>
+      <c r="AK5" s="123"/>
+      <c r="AL5" s="123"/>
+      <c r="AM5" s="123"/>
+      <c r="AN5" s="123"/>
+      <c r="AO5" s="123"/>
+      <c r="AP5" s="123"/>
+      <c r="AQ5" s="123"/>
+      <c r="AR5" s="123"/>
+      <c r="AS5" s="123"/>
+      <c r="AT5" s="123"/>
+      <c r="AU5" s="123"/>
+      <c r="AV5" s="123"/>
+      <c r="AW5" s="123"/>
+      <c r="AX5" s="123"/>
+      <c r="AY5" s="123"/>
+      <c r="AZ5" s="123"/>
+      <c r="BA5" s="123"/>
+      <c r="BB5" s="123"/>
+      <c r="BC5" s="123"/>
+      <c r="BD5" s="123"/>
+      <c r="BE5" s="123"/>
+      <c r="BF5" s="123"/>
+      <c r="BG5" s="123"/>
+      <c r="BH5" s="123"/>
+      <c r="BI5" s="123"/>
+      <c r="BJ5" s="123"/>
+      <c r="BK5" s="123"/>
+      <c r="BL5" s="123"/>
+      <c r="BM5" s="123"/>
+      <c r="BN5" s="123"/>
+      <c r="BO5" s="123"/>
+      <c r="BP5" s="123"/>
+      <c r="BQ5" s="123"/>
+      <c r="BR5" s="123"/>
+      <c r="BS5" s="123"/>
+      <c r="BT5" s="123"/>
+      <c r="BU5" s="123"/>
+      <c r="BV5" s="123"/>
+      <c r="BW5" s="123"/>
+      <c r="BX5" s="123"/>
+      <c r="BY5" s="123"/>
+      <c r="BZ5" s="123"/>
+      <c r="CA5" s="123"/>
+      <c r="CB5" s="123"/>
+      <c r="CC5" s="123"/>
+      <c r="CD5" s="123"/>
+      <c r="CE5" s="123"/>
+      <c r="CF5" s="123"/>
+      <c r="CG5" s="123"/>
+      <c r="CH5" s="123"/>
+      <c r="CI5" s="123"/>
+      <c r="CJ5" s="123"/>
+      <c r="CK5" s="123"/>
+      <c r="CL5" s="123"/>
+      <c r="CM5" s="123"/>
+      <c r="CN5" s="123"/>
+      <c r="CO5" s="123"/>
+      <c r="CP5" s="123"/>
+      <c r="CQ5" s="123"/>
+      <c r="CR5" s="123"/>
+      <c r="CS5" s="123"/>
+      <c r="CT5" s="123"/>
+      <c r="CU5" s="123"/>
+      <c r="CV5" s="123"/>
+      <c r="CW5" s="123"/>
     </row>
     <row r="6">
-      <c r="A6" t="s" s="124">
+      <c r="A6" t="s" s="125">
         <v>82</v>
       </c>
-      <c r="B6" t="s" s="124">
+      <c r="B6" t="s" s="125">
         <v>85</v>
       </c>
-      <c r="C6" t="s" s="124">
+      <c r="C6" t="s" s="125">
         <v>27</v>
       </c>
-      <c r="D6" t="s" s="124">
+      <c r="D6" t="s" s="125">
         <v>83</v>
       </c>
-      <c r="E6" t="s" s="124">
+      <c r="E6" t="s" s="125">
         <v>86</v>
       </c>
-      <c r="F6" s="124"/>
-      <c r="G6" s="124"/>
-      <c r="H6" s="124"/>
-      <c r="I6" s="150"/>
-      <c r="J6" s="151"/>
-      <c r="K6" s="152"/>
-      <c r="L6" s="153"/>
-      <c r="M6" s="154"/>
-      <c r="N6" s="155"/>
-      <c r="O6" s="156"/>
-      <c r="P6" s="157"/>
-      <c r="Q6" s="158"/>
-      <c r="R6" s="159"/>
-      <c r="S6" s="160"/>
-      <c r="T6" s="161"/>
-      <c r="U6" s="162"/>
-      <c r="V6" s="163"/>
-      <c r="W6" s="164"/>
-      <c r="X6" s="165"/>
-      <c r="Y6" s="166"/>
-      <c r="Z6" s="167"/>
-      <c r="AA6" s="168"/>
-      <c r="AB6" s="169"/>
-      <c r="AC6" s="170"/>
-      <c r="AD6" s="171"/>
-      <c r="AE6" s="172"/>
-      <c r="AF6" s="173"/>
-      <c r="AG6" s="174"/>
-      <c r="AH6" s="175"/>
-      <c r="AI6" s="176"/>
-      <c r="AJ6" s="124"/>
-      <c r="AK6" s="124"/>
-      <c r="AL6" s="124"/>
-      <c r="AM6" s="124"/>
-      <c r="AN6" s="124"/>
-      <c r="AO6" s="124"/>
-      <c r="AP6" s="124"/>
-      <c r="AQ6" s="124"/>
-      <c r="AR6" s="124"/>
-      <c r="AS6" s="124"/>
-      <c r="AT6" s="124"/>
-      <c r="AU6" s="124"/>
-      <c r="AV6" s="124"/>
-      <c r="AW6" s="124"/>
-      <c r="AX6" s="124"/>
-      <c r="AY6" s="124"/>
-      <c r="AZ6" s="124"/>
-      <c r="BA6" s="124"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="123"/>
+      <c r="H6" s="123"/>
+      <c r="I6" s="151"/>
+      <c r="J6" s="152"/>
+      <c r="K6" s="153"/>
+      <c r="L6" s="154"/>
+      <c r="M6" s="155"/>
+      <c r="N6" s="156"/>
+      <c r="O6" s="157"/>
+      <c r="P6" s="158"/>
+      <c r="Q6" s="159"/>
+      <c r="R6" s="160"/>
+      <c r="S6" s="161"/>
+      <c r="T6" s="162"/>
+      <c r="U6" s="163"/>
+      <c r="V6" s="164"/>
+      <c r="W6" s="165"/>
+      <c r="X6" s="166"/>
+      <c r="Y6" s="167"/>
+      <c r="Z6" s="168"/>
+      <c r="AA6" s="169"/>
+      <c r="AB6" s="170"/>
+      <c r="AC6" s="171"/>
+      <c r="AD6" s="172"/>
+      <c r="AE6" s="173"/>
+      <c r="AF6" s="174"/>
+      <c r="AG6" s="175"/>
+      <c r="AH6" s="176"/>
+      <c r="AI6" s="177"/>
+      <c r="AJ6" s="123"/>
+      <c r="AK6" s="123"/>
+      <c r="AL6" s="123"/>
+      <c r="AM6" s="123"/>
+      <c r="AN6" s="123"/>
+      <c r="AO6" s="123"/>
+      <c r="AP6" s="123"/>
+      <c r="AQ6" s="123"/>
+      <c r="AR6" s="123"/>
+      <c r="AS6" s="123"/>
+      <c r="AT6" s="123"/>
+      <c r="AU6" s="123"/>
+      <c r="AV6" s="123"/>
+      <c r="AW6" s="123"/>
+      <c r="AX6" s="123"/>
+      <c r="AY6" s="123"/>
+      <c r="AZ6" s="123"/>
+      <c r="BA6" s="123"/>
+      <c r="BB6" s="123"/>
+      <c r="BC6" s="123"/>
+      <c r="BD6" s="123"/>
+      <c r="BE6" s="123"/>
+      <c r="BF6" s="123"/>
+      <c r="BG6" s="123"/>
+      <c r="BH6" s="123"/>
+      <c r="BI6" s="123"/>
+      <c r="BJ6" s="123"/>
+      <c r="BK6" s="123"/>
+      <c r="BL6" s="123"/>
+      <c r="BM6" s="123"/>
+      <c r="BN6" s="123"/>
+      <c r="BO6" s="123"/>
+      <c r="BP6" s="123"/>
+      <c r="BQ6" s="123"/>
+      <c r="BR6" s="123"/>
+      <c r="BS6" s="123"/>
+      <c r="BT6" s="123"/>
+      <c r="BU6" s="123"/>
+      <c r="BV6" s="123"/>
+      <c r="BW6" s="123"/>
+      <c r="BX6" s="123"/>
+      <c r="BY6" s="123"/>
+      <c r="BZ6" s="123"/>
+      <c r="CA6" s="123"/>
+      <c r="CB6" s="123"/>
+      <c r="CC6" s="123"/>
+      <c r="CD6" s="123"/>
+      <c r="CE6" s="123"/>
+      <c r="CF6" s="123"/>
+      <c r="CG6" s="123"/>
+      <c r="CH6" s="123"/>
+      <c r="CI6" s="123"/>
+      <c r="CJ6" s="123"/>
+      <c r="CK6" s="123"/>
+      <c r="CL6" s="123"/>
+      <c r="CM6" s="123"/>
+      <c r="CN6" s="123"/>
+      <c r="CO6" s="123"/>
+      <c r="CP6" s="123"/>
+      <c r="CQ6" s="123"/>
+      <c r="CR6" s="123"/>
+      <c r="CS6" s="123"/>
+      <c r="CT6" s="123"/>
+      <c r="CU6" s="123"/>
+      <c r="CV6" s="123"/>
+      <c r="CW6" s="123"/>
     </row>
     <row r="7">
-      <c r="A7" t="s" s="124">
+      <c r="A7" t="s" s="125">
         <v>82</v>
       </c>
-      <c r="B7" t="s" s="124">
+      <c r="B7" t="s" s="125">
         <v>87</v>
       </c>
-      <c r="C7" t="s" s="124">
+      <c r="C7" t="s" s="125">
         <v>28</v>
       </c>
-      <c r="D7" t="s" s="124">
+      <c r="D7" t="s" s="125">
         <v>83</v>
       </c>
-      <c r="E7" t="s" s="124">
+      <c r="E7" t="s" s="125">
         <v>51</v>
       </c>
-      <c r="F7" s="124"/>
-      <c r="G7" s="124"/>
-      <c r="H7" s="124"/>
-      <c r="I7" s="124"/>
-      <c r="J7" s="124"/>
-      <c r="K7" s="177"/>
-      <c r="L7" s="178"/>
-      <c r="M7" s="179"/>
-      <c r="N7" s="180"/>
-      <c r="O7" s="181"/>
-      <c r="P7" s="182"/>
-      <c r="Q7" s="183"/>
-      <c r="R7" s="184"/>
-      <c r="S7" s="185"/>
-      <c r="T7" s="186"/>
-      <c r="U7" s="187"/>
-      <c r="V7" s="188"/>
-      <c r="W7" s="189"/>
-      <c r="X7" s="124"/>
-      <c r="Y7" s="124"/>
-      <c r="Z7" s="124"/>
-      <c r="AA7" s="124"/>
-      <c r="AB7" s="124"/>
-      <c r="AC7" s="124"/>
-      <c r="AD7" s="124"/>
-      <c r="AE7" s="124"/>
-      <c r="AF7" s="124"/>
-      <c r="AG7" s="124"/>
-      <c r="AH7" s="124"/>
-      <c r="AI7" s="124"/>
-      <c r="AJ7" s="124"/>
-      <c r="AK7" s="124"/>
-      <c r="AL7" s="124"/>
-      <c r="AM7" s="124"/>
-      <c r="AN7" s="124"/>
-      <c r="AO7" s="124"/>
-      <c r="AP7" s="124"/>
-      <c r="AQ7" s="124"/>
-      <c r="AR7" s="124"/>
-      <c r="AS7" s="124"/>
-      <c r="AT7" s="124"/>
-      <c r="AU7" s="124"/>
-      <c r="AV7" s="124"/>
-      <c r="AW7" s="124"/>
-      <c r="AX7" s="124"/>
-      <c r="AY7" s="124"/>
-      <c r="AZ7" s="124"/>
-      <c r="BA7" s="124"/>
+      <c r="F7" s="123"/>
+      <c r="G7" s="123"/>
+      <c r="H7" s="123"/>
+      <c r="I7" s="123"/>
+      <c r="J7" s="123"/>
+      <c r="K7" s="178"/>
+      <c r="L7" s="179"/>
+      <c r="M7" s="180"/>
+      <c r="N7" s="181"/>
+      <c r="O7" s="182"/>
+      <c r="P7" s="183"/>
+      <c r="Q7" s="184"/>
+      <c r="R7" s="185"/>
+      <c r="S7" s="186"/>
+      <c r="T7" s="187"/>
+      <c r="U7" s="188"/>
+      <c r="V7" s="189"/>
+      <c r="W7" s="190"/>
+      <c r="X7" s="123"/>
+      <c r="Y7" s="123"/>
+      <c r="Z7" s="123"/>
+      <c r="AA7" s="123"/>
+      <c r="AB7" s="123"/>
+      <c r="AC7" s="123"/>
+      <c r="AD7" s="123"/>
+      <c r="AE7" s="123"/>
+      <c r="AF7" s="123"/>
+      <c r="AG7" s="123"/>
+      <c r="AH7" s="123"/>
+      <c r="AI7" s="123"/>
+      <c r="AJ7" s="123"/>
+      <c r="AK7" s="123"/>
+      <c r="AL7" s="123"/>
+      <c r="AM7" s="123"/>
+      <c r="AN7" s="123"/>
+      <c r="AO7" s="123"/>
+      <c r="AP7" s="123"/>
+      <c r="AQ7" s="123"/>
+      <c r="AR7" s="123"/>
+      <c r="AS7" s="123"/>
+      <c r="AT7" s="123"/>
+      <c r="AU7" s="123"/>
+      <c r="AV7" s="123"/>
+      <c r="AW7" s="123"/>
+      <c r="AX7" s="123"/>
+      <c r="AY7" s="123"/>
+      <c r="AZ7" s="123"/>
+      <c r="BA7" s="123"/>
+      <c r="BB7" s="123"/>
+      <c r="BC7" s="123"/>
+      <c r="BD7" s="123"/>
+      <c r="BE7" s="123"/>
+      <c r="BF7" s="123"/>
+      <c r="BG7" s="123"/>
+      <c r="BH7" s="123"/>
+      <c r="BI7" s="123"/>
+      <c r="BJ7" s="123"/>
+      <c r="BK7" s="123"/>
+      <c r="BL7" s="123"/>
+      <c r="BM7" s="123"/>
+      <c r="BN7" s="123"/>
+      <c r="BO7" s="123"/>
+      <c r="BP7" s="123"/>
+      <c r="BQ7" s="123"/>
+      <c r="BR7" s="123"/>
+      <c r="BS7" s="123"/>
+      <c r="BT7" s="123"/>
+      <c r="BU7" s="123"/>
+      <c r="BV7" s="123"/>
+      <c r="BW7" s="123"/>
+      <c r="BX7" s="123"/>
+      <c r="BY7" s="123"/>
+      <c r="BZ7" s="123"/>
+      <c r="CA7" s="123"/>
+      <c r="CB7" s="123"/>
+      <c r="CC7" s="123"/>
+      <c r="CD7" s="123"/>
+      <c r="CE7" s="123"/>
+      <c r="CF7" s="123"/>
+      <c r="CG7" s="123"/>
+      <c r="CH7" s="123"/>
+      <c r="CI7" s="123"/>
+      <c r="CJ7" s="123"/>
+      <c r="CK7" s="123"/>
+      <c r="CL7" s="123"/>
+      <c r="CM7" s="123"/>
+      <c r="CN7" s="123"/>
+      <c r="CO7" s="123"/>
+      <c r="CP7" s="123"/>
+      <c r="CQ7" s="123"/>
+      <c r="CR7" s="123"/>
+      <c r="CS7" s="123"/>
+      <c r="CT7" s="123"/>
+      <c r="CU7" s="123"/>
+      <c r="CV7" s="123"/>
+      <c r="CW7" s="123"/>
     </row>
     <row r="8">
-      <c r="A8" t="s" s="124">
+      <c r="A8" t="s" s="125">
         <v>82</v>
       </c>
-      <c r="B8" t="s" s="124">
+      <c r="B8" t="s" s="125">
         <v>88</v>
       </c>
-      <c r="C8" t="s" s="124">
+      <c r="C8" t="s" s="125">
         <v>29</v>
       </c>
-      <c r="D8" t="s" s="124">
+      <c r="D8" t="s" s="125">
         <v>83</v>
       </c>
-      <c r="E8" t="s" s="124">
+      <c r="E8" t="s" s="125">
         <v>89</v>
       </c>
-      <c r="F8" s="124"/>
-      <c r="G8" s="124"/>
-      <c r="H8" s="124"/>
-      <c r="I8" s="124"/>
-      <c r="J8" s="124"/>
-      <c r="K8" s="124"/>
-      <c r="L8" s="190"/>
-      <c r="M8" s="191"/>
-      <c r="N8" s="192"/>
-      <c r="O8" s="193"/>
-      <c r="P8" s="194"/>
-      <c r="Q8" s="195"/>
-      <c r="R8" s="196"/>
-      <c r="S8" s="197"/>
-      <c r="T8" s="198"/>
-      <c r="U8" s="199"/>
-      <c r="V8" s="200"/>
-      <c r="W8" s="201"/>
-      <c r="X8" s="202"/>
-      <c r="Y8" s="203"/>
-      <c r="Z8" s="204"/>
-      <c r="AA8" s="205"/>
-      <c r="AB8" s="206"/>
-      <c r="AC8" s="207"/>
-      <c r="AD8" s="208"/>
-      <c r="AE8" s="209"/>
-      <c r="AF8" s="210"/>
-      <c r="AG8" s="211"/>
-      <c r="AH8" s="212"/>
-      <c r="AI8" s="124"/>
-      <c r="AJ8" s="124"/>
-      <c r="AK8" s="124"/>
-      <c r="AL8" s="124"/>
-      <c r="AM8" s="124"/>
-      <c r="AN8" s="124"/>
-      <c r="AO8" s="124"/>
-      <c r="AP8" s="124"/>
-      <c r="AQ8" s="124"/>
-      <c r="AR8" s="124"/>
-      <c r="AS8" s="124"/>
-      <c r="AT8" s="124"/>
-      <c r="AU8" s="124"/>
-      <c r="AV8" s="124"/>
-      <c r="AW8" s="124"/>
-      <c r="AX8" s="124"/>
-      <c r="AY8" s="124"/>
-      <c r="AZ8" s="124"/>
-      <c r="BA8" s="124"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="123"/>
+      <c r="H8" s="123"/>
+      <c r="I8" s="123"/>
+      <c r="J8" s="123"/>
+      <c r="K8" s="123"/>
+      <c r="L8" s="191"/>
+      <c r="M8" s="192"/>
+      <c r="N8" s="193"/>
+      <c r="O8" s="194"/>
+      <c r="P8" s="195"/>
+      <c r="Q8" s="196"/>
+      <c r="R8" s="197"/>
+      <c r="S8" s="198"/>
+      <c r="T8" s="199"/>
+      <c r="U8" s="200"/>
+      <c r="V8" s="201"/>
+      <c r="W8" s="202"/>
+      <c r="X8" s="203"/>
+      <c r="Y8" s="204"/>
+      <c r="Z8" s="205"/>
+      <c r="AA8" s="206"/>
+      <c r="AB8" s="207"/>
+      <c r="AC8" s="208"/>
+      <c r="AD8" s="209"/>
+      <c r="AE8" s="210"/>
+      <c r="AF8" s="211"/>
+      <c r="AG8" s="212"/>
+      <c r="AH8" s="213"/>
+      <c r="AI8" s="123"/>
+      <c r="AJ8" s="123"/>
+      <c r="AK8" s="123"/>
+      <c r="AL8" s="123"/>
+      <c r="AM8" s="123"/>
+      <c r="AN8" s="123"/>
+      <c r="AO8" s="123"/>
+      <c r="AP8" s="123"/>
+      <c r="AQ8" s="123"/>
+      <c r="AR8" s="123"/>
+      <c r="AS8" s="123"/>
+      <c r="AT8" s="123"/>
+      <c r="AU8" s="123"/>
+      <c r="AV8" s="123"/>
+      <c r="AW8" s="123"/>
+      <c r="AX8" s="123"/>
+      <c r="AY8" s="123"/>
+      <c r="AZ8" s="123"/>
+      <c r="BA8" s="123"/>
+      <c r="BB8" s="123"/>
+      <c r="BC8" s="123"/>
+      <c r="BD8" s="123"/>
+      <c r="BE8" s="123"/>
+      <c r="BF8" s="123"/>
+      <c r="BG8" s="123"/>
+      <c r="BH8" s="123"/>
+      <c r="BI8" s="123"/>
+      <c r="BJ8" s="123"/>
+      <c r="BK8" s="123"/>
+      <c r="BL8" s="123"/>
+      <c r="BM8" s="123"/>
+      <c r="BN8" s="123"/>
+      <c r="BO8" s="123"/>
+      <c r="BP8" s="123"/>
+      <c r="BQ8" s="123"/>
+      <c r="BR8" s="123"/>
+      <c r="BS8" s="123"/>
+      <c r="BT8" s="123"/>
+      <c r="BU8" s="123"/>
+      <c r="BV8" s="123"/>
+      <c r="BW8" s="123"/>
+      <c r="BX8" s="123"/>
+      <c r="BY8" s="123"/>
+      <c r="BZ8" s="123"/>
+      <c r="CA8" s="123"/>
+      <c r="CB8" s="123"/>
+      <c r="CC8" s="123"/>
+      <c r="CD8" s="123"/>
+      <c r="CE8" s="123"/>
+      <c r="CF8" s="123"/>
+      <c r="CG8" s="123"/>
+      <c r="CH8" s="123"/>
+      <c r="CI8" s="123"/>
+      <c r="CJ8" s="123"/>
+      <c r="CK8" s="123"/>
+      <c r="CL8" s="123"/>
+      <c r="CM8" s="123"/>
+      <c r="CN8" s="123"/>
+      <c r="CO8" s="123"/>
+      <c r="CP8" s="123"/>
+      <c r="CQ8" s="123"/>
+      <c r="CR8" s="123"/>
+      <c r="CS8" s="123"/>
+      <c r="CT8" s="123"/>
+      <c r="CU8" s="123"/>
+      <c r="CV8" s="123"/>
+      <c r="CW8" s="123"/>
     </row>
     <row r="9">
-      <c r="A9" t="s" s="124">
+      <c r="A9" t="s" s="125">
         <v>82</v>
       </c>
-      <c r="B9" t="s" s="124">
+      <c r="B9" t="s" s="125">
         <v>90</v>
       </c>
-      <c r="C9" t="s" s="124">
+      <c r="C9" t="s" s="125">
         <v>30</v>
       </c>
-      <c r="D9" t="s" s="124">
+      <c r="D9" t="s" s="125">
         <v>83</v>
       </c>
-      <c r="E9" t="s" s="124">
+      <c r="E9" t="s" s="125">
         <v>91</v>
       </c>
-      <c r="F9" s="124"/>
-      <c r="G9" s="124"/>
-      <c r="H9" s="124"/>
-      <c r="I9" s="124"/>
-      <c r="J9" s="124"/>
-      <c r="K9" s="124"/>
-      <c r="L9" s="213"/>
-      <c r="M9" s="214"/>
-      <c r="N9" s="215"/>
-      <c r="O9" s="216"/>
-      <c r="P9" s="217"/>
-      <c r="Q9" s="218"/>
-      <c r="R9" s="219"/>
-      <c r="S9" s="220"/>
-      <c r="T9" s="221"/>
-      <c r="U9" s="222"/>
-      <c r="V9" s="223"/>
-      <c r="W9" s="224"/>
-      <c r="X9" s="225"/>
-      <c r="Y9" s="226"/>
-      <c r="Z9" s="227"/>
-      <c r="AA9" s="228"/>
-      <c r="AB9" s="229"/>
-      <c r="AC9" s="230"/>
-      <c r="AD9" s="231"/>
-      <c r="AE9" s="232"/>
-      <c r="AF9" s="233"/>
-      <c r="AG9" s="234"/>
-      <c r="AH9" s="235"/>
-      <c r="AI9" s="236"/>
-      <c r="AJ9" s="124"/>
-      <c r="AK9" s="124"/>
-      <c r="AL9" s="124"/>
-      <c r="AM9" s="124"/>
-      <c r="AN9" s="124"/>
-      <c r="AO9" s="124"/>
-      <c r="AP9" s="124"/>
-      <c r="AQ9" s="124"/>
-      <c r="AR9" s="124"/>
-      <c r="AS9" s="124"/>
-      <c r="AT9" s="124"/>
-      <c r="AU9" s="124"/>
-      <c r="AV9" s="124"/>
-      <c r="AW9" s="124"/>
-      <c r="AX9" s="124"/>
-      <c r="AY9" s="124"/>
-      <c r="AZ9" s="124"/>
-      <c r="BA9" s="124"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="123"/>
+      <c r="H9" s="123"/>
+      <c r="I9" s="123"/>
+      <c r="J9" s="123"/>
+      <c r="K9" s="123"/>
+      <c r="L9" s="214"/>
+      <c r="M9" s="215"/>
+      <c r="N9" s="216"/>
+      <c r="O9" s="217"/>
+      <c r="P9" s="218"/>
+      <c r="Q9" s="219"/>
+      <c r="R9" s="220"/>
+      <c r="S9" s="221"/>
+      <c r="T9" s="222"/>
+      <c r="U9" s="223"/>
+      <c r="V9" s="224"/>
+      <c r="W9" s="225"/>
+      <c r="X9" s="226"/>
+      <c r="Y9" s="227"/>
+      <c r="Z9" s="228"/>
+      <c r="AA9" s="229"/>
+      <c r="AB9" s="230"/>
+      <c r="AC9" s="231"/>
+      <c r="AD9" s="232"/>
+      <c r="AE9" s="233"/>
+      <c r="AF9" s="234"/>
+      <c r="AG9" s="235"/>
+      <c r="AH9" s="236"/>
+      <c r="AI9" s="237"/>
+      <c r="AJ9" s="123"/>
+      <c r="AK9" s="123"/>
+      <c r="AL9" s="123"/>
+      <c r="AM9" s="123"/>
+      <c r="AN9" s="123"/>
+      <c r="AO9" s="123"/>
+      <c r="AP9" s="123"/>
+      <c r="AQ9" s="123"/>
+      <c r="AR9" s="123"/>
+      <c r="AS9" s="123"/>
+      <c r="AT9" s="123"/>
+      <c r="AU9" s="123"/>
+      <c r="AV9" s="123"/>
+      <c r="AW9" s="123"/>
+      <c r="AX9" s="123"/>
+      <c r="AY9" s="123"/>
+      <c r="AZ9" s="123"/>
+      <c r="BA9" s="123"/>
+      <c r="BB9" s="123"/>
+      <c r="BC9" s="123"/>
+      <c r="BD9" s="123"/>
+      <c r="BE9" s="123"/>
+      <c r="BF9" s="123"/>
+      <c r="BG9" s="123"/>
+      <c r="BH9" s="123"/>
+      <c r="BI9" s="123"/>
+      <c r="BJ9" s="123"/>
+      <c r="BK9" s="123"/>
+      <c r="BL9" s="123"/>
+      <c r="BM9" s="123"/>
+      <c r="BN9" s="123"/>
+      <c r="BO9" s="123"/>
+      <c r="BP9" s="123"/>
+      <c r="BQ9" s="123"/>
+      <c r="BR9" s="123"/>
+      <c r="BS9" s="123"/>
+      <c r="BT9" s="123"/>
+      <c r="BU9" s="123"/>
+      <c r="BV9" s="123"/>
+      <c r="BW9" s="123"/>
+      <c r="BX9" s="123"/>
+      <c r="BY9" s="123"/>
+      <c r="BZ9" s="123"/>
+      <c r="CA9" s="123"/>
+      <c r="CB9" s="123"/>
+      <c r="CC9" s="123"/>
+      <c r="CD9" s="123"/>
+      <c r="CE9" s="123"/>
+      <c r="CF9" s="123"/>
+      <c r="CG9" s="123"/>
+      <c r="CH9" s="123"/>
+      <c r="CI9" s="123"/>
+      <c r="CJ9" s="123"/>
+      <c r="CK9" s="123"/>
+      <c r="CL9" s="123"/>
+      <c r="CM9" s="123"/>
+      <c r="CN9" s="123"/>
+      <c r="CO9" s="123"/>
+      <c r="CP9" s="123"/>
+      <c r="CQ9" s="123"/>
+      <c r="CR9" s="123"/>
+      <c r="CS9" s="123"/>
+      <c r="CT9" s="123"/>
+      <c r="CU9" s="123"/>
+      <c r="CV9" s="123"/>
+      <c r="CW9" s="123"/>
     </row>
     <row r="10">
-      <c r="A10" t="s" s="124">
+      <c r="A10" t="s" s="125">
         <v>82</v>
       </c>
-      <c r="B10" t="s" s="124">
+      <c r="B10" t="s" s="125">
         <v>92</v>
       </c>
-      <c r="C10" t="s" s="124">
+      <c r="C10" t="s" s="125">
         <v>31</v>
       </c>
-      <c r="D10" t="s" s="124">
+      <c r="D10" t="s" s="125">
         <v>83</v>
       </c>
-      <c r="E10" t="s" s="124">
+      <c r="E10" t="s" s="125">
         <v>93</v>
       </c>
-      <c r="F10" s="124"/>
-      <c r="G10" s="124"/>
-      <c r="H10" s="124"/>
-      <c r="I10" s="124"/>
-      <c r="J10" s="124"/>
-      <c r="K10" s="124"/>
-      <c r="L10" s="237"/>
-      <c r="M10" s="238"/>
-      <c r="N10" s="239"/>
-      <c r="O10" s="240"/>
-      <c r="P10" s="241"/>
-      <c r="Q10" s="242"/>
-      <c r="R10" s="243"/>
-      <c r="S10" s="244"/>
-      <c r="T10" s="245"/>
-      <c r="U10" s="246"/>
-      <c r="V10" s="247"/>
-      <c r="W10" s="248"/>
-      <c r="X10" s="249"/>
-      <c r="Y10" s="250"/>
-      <c r="Z10" s="251"/>
-      <c r="AA10" s="252"/>
-      <c r="AB10" s="253"/>
-      <c r="AC10" s="254"/>
-      <c r="AD10" s="255"/>
-      <c r="AE10" s="256"/>
-      <c r="AF10" s="257"/>
-      <c r="AG10" s="258"/>
-      <c r="AH10" s="259"/>
-      <c r="AI10" s="260"/>
-      <c r="AJ10" s="124"/>
-      <c r="AK10" s="124"/>
-      <c r="AL10" s="124"/>
-      <c r="AM10" s="124"/>
-      <c r="AN10" s="124"/>
-      <c r="AO10" s="124"/>
-      <c r="AP10" s="124"/>
-      <c r="AQ10" s="124"/>
-      <c r="AR10" s="124"/>
-      <c r="AS10" s="124"/>
-      <c r="AT10" s="124"/>
-      <c r="AU10" s="124"/>
-      <c r="AV10" s="124"/>
-      <c r="AW10" s="124"/>
-      <c r="AX10" s="124"/>
-      <c r="AY10" s="124"/>
-      <c r="AZ10" s="124"/>
-      <c r="BA10" s="124"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="123"/>
+      <c r="H10" s="123"/>
+      <c r="I10" s="123"/>
+      <c r="J10" s="123"/>
+      <c r="K10" s="123"/>
+      <c r="L10" s="238"/>
+      <c r="M10" s="239"/>
+      <c r="N10" s="240"/>
+      <c r="O10" s="241"/>
+      <c r="P10" s="242"/>
+      <c r="Q10" s="243"/>
+      <c r="R10" s="244"/>
+      <c r="S10" s="245"/>
+      <c r="T10" s="246"/>
+      <c r="U10" s="247"/>
+      <c r="V10" s="248"/>
+      <c r="W10" s="249"/>
+      <c r="X10" s="250"/>
+      <c r="Y10" s="251"/>
+      <c r="Z10" s="252"/>
+      <c r="AA10" s="253"/>
+      <c r="AB10" s="254"/>
+      <c r="AC10" s="255"/>
+      <c r="AD10" s="256"/>
+      <c r="AE10" s="257"/>
+      <c r="AF10" s="258"/>
+      <c r="AG10" s="259"/>
+      <c r="AH10" s="260"/>
+      <c r="AI10" s="261"/>
+      <c r="AJ10" s="123"/>
+      <c r="AK10" s="123"/>
+      <c r="AL10" s="123"/>
+      <c r="AM10" s="123"/>
+      <c r="AN10" s="123"/>
+      <c r="AO10" s="123"/>
+      <c r="AP10" s="123"/>
+      <c r="AQ10" s="123"/>
+      <c r="AR10" s="123"/>
+      <c r="AS10" s="123"/>
+      <c r="AT10" s="123"/>
+      <c r="AU10" s="123"/>
+      <c r="AV10" s="123"/>
+      <c r="AW10" s="123"/>
+      <c r="AX10" s="123"/>
+      <c r="AY10" s="123"/>
+      <c r="AZ10" s="123"/>
+      <c r="BA10" s="123"/>
+      <c r="BB10" s="123"/>
+      <c r="BC10" s="123"/>
+      <c r="BD10" s="123"/>
+      <c r="BE10" s="123"/>
+      <c r="BF10" s="123"/>
+      <c r="BG10" s="123"/>
+      <c r="BH10" s="123"/>
+      <c r="BI10" s="123"/>
+      <c r="BJ10" s="123"/>
+      <c r="BK10" s="123"/>
+      <c r="BL10" s="123"/>
+      <c r="BM10" s="123"/>
+      <c r="BN10" s="123"/>
+      <c r="BO10" s="123"/>
+      <c r="BP10" s="123"/>
+      <c r="BQ10" s="123"/>
+      <c r="BR10" s="123"/>
+      <c r="BS10" s="123"/>
+      <c r="BT10" s="123"/>
+      <c r="BU10" s="123"/>
+      <c r="BV10" s="123"/>
+      <c r="BW10" s="123"/>
+      <c r="BX10" s="123"/>
+      <c r="BY10" s="123"/>
+      <c r="BZ10" s="123"/>
+      <c r="CA10" s="123"/>
+      <c r="CB10" s="123"/>
+      <c r="CC10" s="123"/>
+      <c r="CD10" s="123"/>
+      <c r="CE10" s="123"/>
+      <c r="CF10" s="123"/>
+      <c r="CG10" s="123"/>
+      <c r="CH10" s="123"/>
+      <c r="CI10" s="123"/>
+      <c r="CJ10" s="123"/>
+      <c r="CK10" s="123"/>
+      <c r="CL10" s="123"/>
+      <c r="CM10" s="123"/>
+      <c r="CN10" s="123"/>
+      <c r="CO10" s="123"/>
+      <c r="CP10" s="123"/>
+      <c r="CQ10" s="123"/>
+      <c r="CR10" s="123"/>
+      <c r="CS10" s="123"/>
+      <c r="CT10" s="123"/>
+      <c r="CU10" s="123"/>
+      <c r="CV10" s="123"/>
+      <c r="CW10" s="123"/>
     </row>
     <row r="11">
-      <c r="A11" t="s" s="124">
+      <c r="A11" t="s" s="125">
         <v>82</v>
       </c>
-      <c r="B11" t="s" s="124">
+      <c r="B11" t="s" s="125">
         <v>94</v>
       </c>
-      <c r="C11" t="s" s="124">
+      <c r="C11" t="s" s="125">
         <v>95</v>
       </c>
-      <c r="D11" t="s" s="124">
+      <c r="D11" t="s" s="125">
         <v>83</v>
       </c>
-      <c r="E11" t="s" s="124">
+      <c r="E11" t="s" s="125">
         <v>55</v>
       </c>
-      <c r="F11" s="124"/>
-      <c r="G11" s="124"/>
-      <c r="H11" s="124"/>
-      <c r="I11" s="124"/>
-      <c r="J11" s="124"/>
-      <c r="K11" s="124"/>
-      <c r="L11" s="124"/>
-      <c r="M11" s="124"/>
-      <c r="N11" s="124"/>
-      <c r="O11" s="124"/>
-      <c r="P11" s="124"/>
-      <c r="Q11" s="124"/>
-      <c r="R11" s="124"/>
-      <c r="S11" s="124"/>
-      <c r="T11" s="124"/>
-      <c r="U11" s="124"/>
-      <c r="V11" s="124"/>
-      <c r="W11" s="124"/>
-      <c r="X11" s="124"/>
-      <c r="Y11" s="124"/>
-      <c r="Z11" s="124"/>
-      <c r="AA11" s="124"/>
-      <c r="AB11" s="124"/>
-      <c r="AC11" s="124"/>
-      <c r="AD11" s="124"/>
-      <c r="AE11" s="124"/>
-      <c r="AF11" s="124"/>
-      <c r="AG11" s="124"/>
-      <c r="AH11" s="124"/>
-      <c r="AI11" s="124"/>
-      <c r="AJ11" s="124"/>
-      <c r="AK11" s="124"/>
-      <c r="AL11" s="124"/>
-      <c r="AM11" s="124"/>
-      <c r="AN11" s="124"/>
-      <c r="AO11" s="261"/>
-      <c r="AP11" s="124"/>
-      <c r="AQ11" s="124"/>
-      <c r="AR11" s="124"/>
-      <c r="AS11" s="124"/>
-      <c r="AT11" s="124"/>
-      <c r="AU11" s="124"/>
-      <c r="AV11" s="124"/>
-      <c r="AW11" s="124"/>
-      <c r="AX11" s="124"/>
-      <c r="AY11" s="124"/>
-      <c r="AZ11" s="124"/>
-      <c r="BA11" s="124"/>
+      <c r="F11" s="123"/>
+      <c r="G11" s="123"/>
+      <c r="H11" s="123"/>
+      <c r="I11" s="123"/>
+      <c r="J11" s="123"/>
+      <c r="K11" s="123"/>
+      <c r="L11" s="123"/>
+      <c r="M11" s="123"/>
+      <c r="N11" s="123"/>
+      <c r="O11" s="123"/>
+      <c r="P11" s="123"/>
+      <c r="Q11" s="123"/>
+      <c r="R11" s="123"/>
+      <c r="S11" s="123"/>
+      <c r="T11" s="123"/>
+      <c r="U11" s="123"/>
+      <c r="V11" s="123"/>
+      <c r="W11" s="123"/>
+      <c r="X11" s="123"/>
+      <c r="Y11" s="123"/>
+      <c r="Z11" s="123"/>
+      <c r="AA11" s="123"/>
+      <c r="AB11" s="123"/>
+      <c r="AC11" s="123"/>
+      <c r="AD11" s="123"/>
+      <c r="AE11" s="123"/>
+      <c r="AF11" s="123"/>
+      <c r="AG11" s="123"/>
+      <c r="AH11" s="123"/>
+      <c r="AI11" s="123"/>
+      <c r="AJ11" s="123"/>
+      <c r="AK11" s="123"/>
+      <c r="AL11" s="123"/>
+      <c r="AM11" s="123"/>
+      <c r="AN11" s="123"/>
+      <c r="AO11" s="262"/>
+      <c r="AP11" s="123"/>
+      <c r="AQ11" s="123"/>
+      <c r="AR11" s="123"/>
+      <c r="AS11" s="123"/>
+      <c r="AT11" s="123"/>
+      <c r="AU11" s="123"/>
+      <c r="AV11" s="123"/>
+      <c r="AW11" s="123"/>
+      <c r="AX11" s="123"/>
+      <c r="AY11" s="123"/>
+      <c r="AZ11" s="123"/>
+      <c r="BA11" s="123"/>
+      <c r="BB11" s="123"/>
+      <c r="BC11" s="123"/>
+      <c r="BD11" s="123"/>
+      <c r="BE11" s="123"/>
+      <c r="BF11" s="123"/>
+      <c r="BG11" s="123"/>
+      <c r="BH11" s="123"/>
+      <c r="BI11" s="123"/>
+      <c r="BJ11" s="123"/>
+      <c r="BK11" s="123"/>
+      <c r="BL11" s="123"/>
+      <c r="BM11" s="123"/>
+      <c r="BN11" s="123"/>
+      <c r="BO11" s="123"/>
+      <c r="BP11" s="123"/>
+      <c r="BQ11" s="123"/>
+      <c r="BR11" s="123"/>
+      <c r="BS11" s="123"/>
+      <c r="BT11" s="123"/>
+      <c r="BU11" s="123"/>
+      <c r="BV11" s="123"/>
+      <c r="BW11" s="123"/>
+      <c r="BX11" s="123"/>
+      <c r="BY11" s="123"/>
+      <c r="BZ11" s="123"/>
+      <c r="CA11" s="123"/>
+      <c r="CB11" s="123"/>
+      <c r="CC11" s="123"/>
+      <c r="CD11" s="123"/>
+      <c r="CE11" s="123"/>
+      <c r="CF11" s="123"/>
+      <c r="CG11" s="123"/>
+      <c r="CH11" s="123"/>
+      <c r="CI11" s="123"/>
+      <c r="CJ11" s="123"/>
+      <c r="CK11" s="123"/>
+      <c r="CL11" s="123"/>
+      <c r="CM11" s="123"/>
+      <c r="CN11" s="123"/>
+      <c r="CO11" s="123"/>
+      <c r="CP11" s="123"/>
+      <c r="CQ11" s="123"/>
+      <c r="CR11" s="123"/>
+      <c r="CS11" s="123"/>
+      <c r="CT11" s="123"/>
+      <c r="CU11" s="123"/>
+      <c r="CV11" s="123"/>
+      <c r="CW11" s="123"/>
     </row>
     <row r="12">
-      <c r="A12" t="s" s="124">
+      <c r="A12" t="s" s="125">
         <v>82</v>
       </c>
-      <c r="B12" t="s" s="124">
+      <c r="B12" t="s" s="125">
         <v>96</v>
       </c>
-      <c r="C12" t="s" s="124">
+      <c r="C12" t="s" s="125">
         <v>97</v>
       </c>
-      <c r="D12" t="s" s="124">
+      <c r="D12" t="s" s="125">
         <v>83</v>
       </c>
-      <c r="E12" t="s" s="124">
+      <c r="E12" t="s" s="125">
         <v>98</v>
       </c>
-      <c r="F12" s="124"/>
-      <c r="G12" s="124"/>
-      <c r="H12" s="124"/>
-      <c r="I12" s="124"/>
-      <c r="J12" s="124"/>
-      <c r="K12" s="262"/>
-      <c r="L12" s="263"/>
-      <c r="M12" s="264"/>
-      <c r="N12" s="265"/>
-      <c r="O12" s="266"/>
-      <c r="P12" s="267"/>
-      <c r="Q12" s="268"/>
-      <c r="R12" s="269"/>
-      <c r="S12" s="270"/>
-      <c r="T12" s="271"/>
-      <c r="U12" s="272"/>
-      <c r="V12" s="273"/>
-      <c r="W12" s="274"/>
-      <c r="X12" s="275"/>
-      <c r="Y12" s="276"/>
-      <c r="Z12" s="277"/>
-      <c r="AA12" s="278"/>
-      <c r="AB12" s="279"/>
-      <c r="AC12" s="280"/>
-      <c r="AD12" s="281"/>
-      <c r="AE12" s="282"/>
-      <c r="AF12" s="283"/>
-      <c r="AG12" s="284"/>
-      <c r="AH12" s="285"/>
-      <c r="AI12" s="124"/>
-      <c r="AJ12" s="124"/>
-      <c r="AK12" s="124"/>
-      <c r="AL12" s="124"/>
-      <c r="AM12" s="124"/>
-      <c r="AN12" s="124"/>
-      <c r="AO12" s="124"/>
-      <c r="AP12" s="124"/>
-      <c r="AQ12" s="124"/>
-      <c r="AR12" s="124"/>
-      <c r="AS12" s="124"/>
-      <c r="AT12" s="124"/>
-      <c r="AU12" s="124"/>
-      <c r="AV12" s="124"/>
-      <c r="AW12" s="124"/>
-      <c r="AX12" s="124"/>
-      <c r="AY12" s="124"/>
-      <c r="AZ12" s="124"/>
-      <c r="BA12" s="124"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="123"/>
+      <c r="H12" s="123"/>
+      <c r="I12" s="123"/>
+      <c r="J12" s="123"/>
+      <c r="K12" s="263"/>
+      <c r="L12" s="264"/>
+      <c r="M12" s="265"/>
+      <c r="N12" s="266"/>
+      <c r="O12" s="267"/>
+      <c r="P12" s="268"/>
+      <c r="Q12" s="269"/>
+      <c r="R12" s="270"/>
+      <c r="S12" s="271"/>
+      <c r="T12" s="272"/>
+      <c r="U12" s="273"/>
+      <c r="V12" s="274"/>
+      <c r="W12" s="275"/>
+      <c r="X12" s="276"/>
+      <c r="Y12" s="277"/>
+      <c r="Z12" s="278"/>
+      <c r="AA12" s="279"/>
+      <c r="AB12" s="280"/>
+      <c r="AC12" s="281"/>
+      <c r="AD12" s="282"/>
+      <c r="AE12" s="283"/>
+      <c r="AF12" s="284"/>
+      <c r="AG12" s="285"/>
+      <c r="AH12" s="286"/>
+      <c r="AI12" s="123"/>
+      <c r="AJ12" s="123"/>
+      <c r="AK12" s="123"/>
+      <c r="AL12" s="123"/>
+      <c r="AM12" s="123"/>
+      <c r="AN12" s="123"/>
+      <c r="AO12" s="123"/>
+      <c r="AP12" s="123"/>
+      <c r="AQ12" s="123"/>
+      <c r="AR12" s="123"/>
+      <c r="AS12" s="123"/>
+      <c r="AT12" s="123"/>
+      <c r="AU12" s="123"/>
+      <c r="AV12" s="123"/>
+      <c r="AW12" s="123"/>
+      <c r="AX12" s="123"/>
+      <c r="AY12" s="123"/>
+      <c r="AZ12" s="123"/>
+      <c r="BA12" s="123"/>
+      <c r="BB12" s="123"/>
+      <c r="BC12" s="123"/>
+      <c r="BD12" s="123"/>
+      <c r="BE12" s="123"/>
+      <c r="BF12" s="123"/>
+      <c r="BG12" s="123"/>
+      <c r="BH12" s="123"/>
+      <c r="BI12" s="123"/>
+      <c r="BJ12" s="123"/>
+      <c r="BK12" s="123"/>
+      <c r="BL12" s="123"/>
+      <c r="BM12" s="123"/>
+      <c r="BN12" s="123"/>
+      <c r="BO12" s="123"/>
+      <c r="BP12" s="123"/>
+      <c r="BQ12" s="123"/>
+      <c r="BR12" s="123"/>
+      <c r="BS12" s="123"/>
+      <c r="BT12" s="123"/>
+      <c r="BU12" s="123"/>
+      <c r="BV12" s="123"/>
+      <c r="BW12" s="123"/>
+      <c r="BX12" s="123"/>
+      <c r="BY12" s="123"/>
+      <c r="BZ12" s="123"/>
+      <c r="CA12" s="123"/>
+      <c r="CB12" s="123"/>
+      <c r="CC12" s="123"/>
+      <c r="CD12" s="123"/>
+      <c r="CE12" s="123"/>
+      <c r="CF12" s="123"/>
+      <c r="CG12" s="123"/>
+      <c r="CH12" s="123"/>
+      <c r="CI12" s="123"/>
+      <c r="CJ12" s="123"/>
+      <c r="CK12" s="123"/>
+      <c r="CL12" s="123"/>
+      <c r="CM12" s="123"/>
+      <c r="CN12" s="123"/>
+      <c r="CO12" s="123"/>
+      <c r="CP12" s="123"/>
+      <c r="CQ12" s="123"/>
+      <c r="CR12" s="123"/>
+      <c r="CS12" s="123"/>
+      <c r="CT12" s="123"/>
+      <c r="CU12" s="123"/>
+      <c r="CV12" s="123"/>
+      <c r="CW12" s="123"/>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AD3:AE3"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AJ3:AK3"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="AN3:AO3"/>
-    <mergeCell ref="AP3:AQ3"/>
-    <mergeCell ref="AR3:AS3"/>
-    <mergeCell ref="AT3:AU3"/>
-    <mergeCell ref="AV3:AW3"/>
-    <mergeCell ref="AX3:AY3"/>
-    <mergeCell ref="AZ3:BA3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="V3:Y3"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="AD3:AG3"/>
+    <mergeCell ref="AH3:AK3"/>
+    <mergeCell ref="AL3:AO3"/>
+    <mergeCell ref="AP3:AS3"/>
+    <mergeCell ref="AT3:AW3"/>
+    <mergeCell ref="AX3:BA3"/>
+    <mergeCell ref="BB3:BE3"/>
+    <mergeCell ref="BF3:BI3"/>
+    <mergeCell ref="BJ3:BM3"/>
+    <mergeCell ref="BN3:BQ3"/>
+    <mergeCell ref="BR3:BU3"/>
+    <mergeCell ref="BV3:BY3"/>
+    <mergeCell ref="BZ3:CC3"/>
+    <mergeCell ref="CD3:CG3"/>
+    <mergeCell ref="CH3:CK3"/>
+    <mergeCell ref="CL3:CO3"/>
+    <mergeCell ref="CP3:CS3"/>
+    <mergeCell ref="CT3:CW3"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
swing connection well done
</commit_message>
<xml_diff>
--- a/sourse - копия.xlsx
+++ b/sourse - копия.xlsx
@@ -4993,10 +4993,20 @@
     <xf numFmtId="0" fontId="11" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5010,23 +5020,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5037,7 +5044,13 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5049,24 +5062,11 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="center"/>
     </xf>
@@ -6128,24 +6128,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="136" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="138"/>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
-      <c r="E1" s="138"/>
-      <c r="F1" s="138"/>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
-      <c r="I1" s="138"/>
-      <c r="J1" s="138"/>
-      <c r="K1" s="138"/>
-      <c r="L1" s="138"/>
-      <c r="M1" s="138"/>
-      <c r="N1" s="138"/>
-      <c r="O1" s="138"/>
-      <c r="P1" s="138"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
+      <c r="J1" s="136"/>
+      <c r="K1" s="136"/>
+      <c r="L1" s="136"/>
+      <c r="M1" s="136"/>
+      <c r="N1" s="136"/>
+      <c r="O1" s="136"/>
+      <c r="P1" s="136"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -8853,63 +8853,63 @@
       </c>
     </row>
     <row r="2" spans="1:53" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="146" t="s">
+      <c r="A2" s="137" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="146"/>
+      <c r="B2" s="137"/>
       <c r="C2" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="147" t="s">
+      <c r="F2" s="138" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="147"/>
-      <c r="H2" s="147"/>
-      <c r="I2" s="147"/>
-      <c r="J2" s="147"/>
-      <c r="K2" s="147"/>
-      <c r="L2" s="147"/>
-      <c r="M2" s="147"/>
-      <c r="N2" s="147"/>
-      <c r="O2" s="147"/>
-      <c r="P2" s="147"/>
-      <c r="Q2" s="147"/>
-      <c r="R2" s="147"/>
-      <c r="S2" s="147"/>
-      <c r="T2" s="147"/>
-      <c r="U2" s="147"/>
-      <c r="V2" s="147"/>
-      <c r="W2" s="147"/>
-      <c r="X2" s="147"/>
-      <c r="Y2" s="147"/>
-      <c r="Z2" s="147"/>
-      <c r="AA2" s="147"/>
-      <c r="AB2" s="147"/>
-      <c r="AC2" s="147"/>
-      <c r="AD2" s="147"/>
-      <c r="AE2" s="147"/>
-      <c r="AF2" s="147"/>
-      <c r="AG2" s="147"/>
-      <c r="AH2" s="147"/>
-      <c r="AI2" s="147"/>
-      <c r="AJ2" s="147"/>
-      <c r="AK2" s="147"/>
-      <c r="AL2" s="147"/>
-      <c r="AM2" s="147"/>
-      <c r="AN2" s="147"/>
-      <c r="AO2" s="147"/>
-      <c r="AP2" s="147"/>
-      <c r="AQ2" s="147"/>
-      <c r="AR2" s="147"/>
-      <c r="AS2" s="147"/>
-      <c r="AT2" s="147"/>
-      <c r="AU2" s="147"/>
-      <c r="AV2" s="147"/>
-      <c r="AW2" s="147"/>
-      <c r="AX2" s="147"/>
-      <c r="AY2" s="147"/>
-      <c r="AZ2" s="147"/>
-      <c r="BA2" s="147"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
+      <c r="L2" s="138"/>
+      <c r="M2" s="138"/>
+      <c r="N2" s="138"/>
+      <c r="O2" s="138"/>
+      <c r="P2" s="138"/>
+      <c r="Q2" s="138"/>
+      <c r="R2" s="138"/>
+      <c r="S2" s="138"/>
+      <c r="T2" s="138"/>
+      <c r="U2" s="138"/>
+      <c r="V2" s="138"/>
+      <c r="W2" s="138"/>
+      <c r="X2" s="138"/>
+      <c r="Y2" s="138"/>
+      <c r="Z2" s="138"/>
+      <c r="AA2" s="138"/>
+      <c r="AB2" s="138"/>
+      <c r="AC2" s="138"/>
+      <c r="AD2" s="138"/>
+      <c r="AE2" s="138"/>
+      <c r="AF2" s="138"/>
+      <c r="AG2" s="138"/>
+      <c r="AH2" s="138"/>
+      <c r="AI2" s="138"/>
+      <c r="AJ2" s="138"/>
+      <c r="AK2" s="138"/>
+      <c r="AL2" s="138"/>
+      <c r="AM2" s="138"/>
+      <c r="AN2" s="138"/>
+      <c r="AO2" s="138"/>
+      <c r="AP2" s="138"/>
+      <c r="AQ2" s="138"/>
+      <c r="AR2" s="138"/>
+      <c r="AS2" s="138"/>
+      <c r="AT2" s="138"/>
+      <c r="AU2" s="138"/>
+      <c r="AV2" s="138"/>
+      <c r="AW2" s="138"/>
+      <c r="AX2" s="138"/>
+      <c r="AY2" s="138"/>
+      <c r="AZ2" s="138"/>
+      <c r="BA2" s="138"/>
     </row>
     <row r="3" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
@@ -8927,102 +8927,102 @@
       <c r="E3" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="143">
+      <c r="F3" s="139">
         <v>7</v>
       </c>
-      <c r="G3" s="143"/>
-      <c r="H3" s="143">
+      <c r="G3" s="139"/>
+      <c r="H3" s="139">
         <v>8</v>
       </c>
-      <c r="I3" s="143"/>
-      <c r="J3" s="143">
+      <c r="I3" s="139"/>
+      <c r="J3" s="139">
         <v>9</v>
       </c>
-      <c r="K3" s="143"/>
-      <c r="L3" s="143">
+      <c r="K3" s="139"/>
+      <c r="L3" s="139">
         <v>10</v>
       </c>
-      <c r="M3" s="143"/>
-      <c r="N3" s="143">
+      <c r="M3" s="139"/>
+      <c r="N3" s="139">
         <v>11</v>
       </c>
-      <c r="O3" s="143"/>
-      <c r="P3" s="143">
+      <c r="O3" s="139"/>
+      <c r="P3" s="139">
         <v>12</v>
       </c>
-      <c r="Q3" s="143"/>
-      <c r="R3" s="143">
+      <c r="Q3" s="139"/>
+      <c r="R3" s="139">
         <v>13</v>
       </c>
-      <c r="S3" s="143"/>
-      <c r="T3" s="143">
+      <c r="S3" s="139"/>
+      <c r="T3" s="139">
         <v>14</v>
       </c>
-      <c r="U3" s="143"/>
-      <c r="V3" s="143">
+      <c r="U3" s="139"/>
+      <c r="V3" s="139">
         <v>15</v>
       </c>
-      <c r="W3" s="143"/>
-      <c r="X3" s="143">
+      <c r="W3" s="139"/>
+      <c r="X3" s="139">
         <v>16</v>
       </c>
-      <c r="Y3" s="143"/>
-      <c r="Z3" s="145">
+      <c r="Y3" s="139"/>
+      <c r="Z3" s="146">
         <v>17</v>
       </c>
-      <c r="AA3" s="145"/>
-      <c r="AB3" s="145">
+      <c r="AA3" s="146"/>
+      <c r="AB3" s="146">
         <v>18</v>
       </c>
-      <c r="AC3" s="145"/>
-      <c r="AD3" s="143">
+      <c r="AC3" s="146"/>
+      <c r="AD3" s="139">
         <v>19</v>
       </c>
-      <c r="AE3" s="143"/>
-      <c r="AF3" s="143">
+      <c r="AE3" s="139"/>
+      <c r="AF3" s="139">
         <v>20</v>
       </c>
-      <c r="AG3" s="143"/>
-      <c r="AH3" s="143">
+      <c r="AG3" s="139"/>
+      <c r="AH3" s="139">
         <v>21</v>
       </c>
-      <c r="AI3" s="143"/>
-      <c r="AJ3" s="143">
+      <c r="AI3" s="139"/>
+      <c r="AJ3" s="139">
         <v>22</v>
       </c>
-      <c r="AK3" s="143"/>
-      <c r="AL3" s="143">
+      <c r="AK3" s="139"/>
+      <c r="AL3" s="139">
         <v>23</v>
       </c>
-      <c r="AM3" s="143"/>
-      <c r="AN3" s="143">
+      <c r="AM3" s="139"/>
+      <c r="AN3" s="139">
         <v>24</v>
       </c>
-      <c r="AO3" s="143"/>
-      <c r="AP3" s="143">
+      <c r="AO3" s="139"/>
+      <c r="AP3" s="139">
         <v>1</v>
       </c>
-      <c r="AQ3" s="143"/>
-      <c r="AR3" s="143">
+      <c r="AQ3" s="139"/>
+      <c r="AR3" s="139">
         <v>2</v>
       </c>
-      <c r="AS3" s="143"/>
-      <c r="AT3" s="143">
+      <c r="AS3" s="139"/>
+      <c r="AT3" s="139">
         <v>3</v>
       </c>
-      <c r="AU3" s="143"/>
-      <c r="AV3" s="143">
+      <c r="AU3" s="139"/>
+      <c r="AV3" s="139">
         <v>4</v>
       </c>
-      <c r="AW3" s="143"/>
-      <c r="AX3" s="143">
+      <c r="AW3" s="139"/>
+      <c r="AX3" s="139">
         <v>5</v>
       </c>
-      <c r="AY3" s="143"/>
-      <c r="AZ3" s="143">
+      <c r="AY3" s="139"/>
+      <c r="AZ3" s="139">
         <v>6</v>
       </c>
-      <c r="BA3" s="148"/>
+      <c r="BA3" s="140"/>
     </row>
     <row r="4" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="94" t="s">
@@ -9082,7 +9082,7 @@
       <c r="BA4" s="97"/>
     </row>
     <row r="5" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="139" t="s">
+      <c r="A5" s="141" t="s">
         <v>72</v>
       </c>
       <c r="B5" s="59" t="s">
@@ -9149,7 +9149,7 @@
       <c r="BA5" s="50"/>
     </row>
     <row r="6" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="142"/>
+      <c r="A6" s="144"/>
       <c r="B6" s="34" t="s">
         <v>62</v>
       </c>
@@ -9216,7 +9216,7 @@
       <c r="BA6" s="51"/>
     </row>
     <row r="7" spans="1:53" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="140"/>
+      <c r="A7" s="142"/>
       <c r="B7" s="40" t="s">
         <v>62</v>
       </c>
@@ -9281,7 +9281,7 @@
       <c r="BA7" s="57"/>
     </row>
     <row r="8" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="141" t="s">
+      <c r="A8" s="143" t="s">
         <v>67</v>
       </c>
       <c r="B8" s="38" t="s">
@@ -9348,7 +9348,7 @@
       <c r="BA8" s="74"/>
     </row>
     <row r="9" spans="1:53" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="144"/>
+      <c r="A9" s="145"/>
       <c r="B9" s="87" t="s">
         <v>32</v>
       </c>
@@ -9411,7 +9411,7 @@
       <c r="BA9" s="70"/>
     </row>
     <row r="10" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="139" t="s">
+      <c r="A10" s="141" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="59" t="s">
@@ -9476,7 +9476,7 @@
       <c r="BA10" s="50"/>
     </row>
     <row r="11" spans="1:53" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="140"/>
+      <c r="A11" s="142"/>
       <c r="B11" s="40" t="s">
         <v>69</v>
       </c>
@@ -9535,7 +9535,7 @@
       <c r="BA11" s="57"/>
     </row>
     <row r="12" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="141" t="s">
+      <c r="A12" s="143" t="s">
         <v>70</v>
       </c>
       <c r="B12" s="58" t="s">
@@ -9604,7 +9604,7 @@
       <c r="BA12" s="71"/>
     </row>
     <row r="13" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="142"/>
+      <c r="A13" s="144"/>
       <c r="B13" s="34" t="s">
         <v>24</v>
       </c>
@@ -9671,7 +9671,7 @@
       <c r="BA13" s="51"/>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A14" s="142"/>
+      <c r="A14" s="144"/>
       <c r="B14" s="34" t="s">
         <v>24</v>
       </c>
@@ -9736,7 +9736,7 @@
       <c r="BA14" s="51"/>
     </row>
     <row r="15" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A15" s="142"/>
+      <c r="A15" s="144"/>
       <c r="B15" s="34" t="s">
         <v>24</v>
       </c>
@@ -9799,7 +9799,7 @@
       <c r="BA15" s="51"/>
     </row>
     <row r="16" spans="1:53" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="142"/>
+      <c r="A16" s="144"/>
       <c r="B16" s="34" t="s">
         <v>45</v>
       </c>
@@ -9860,7 +9860,7 @@
       <c r="BA16" s="51"/>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A17" s="142"/>
+      <c r="A17" s="144"/>
       <c r="B17" s="34" t="s">
         <v>24</v>
       </c>
@@ -9925,7 +9925,7 @@
       <c r="BA17" s="51"/>
     </row>
     <row r="18" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="140"/>
+      <c r="A18" s="142"/>
       <c r="B18" s="40" t="s">
         <v>24</v>
       </c>
@@ -9990,7 +9990,7 @@
       <c r="BA18" s="57"/>
     </row>
     <row r="19" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="141" t="s">
+      <c r="A19" s="143" t="s">
         <v>71</v>
       </c>
       <c r="B19" s="38" t="s">
@@ -10057,7 +10057,7 @@
       <c r="BA19" s="71"/>
     </row>
     <row r="20" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A20" s="142"/>
+      <c r="A20" s="144"/>
       <c r="B20" s="41" t="s">
         <v>32</v>
       </c>
@@ -10120,7 +10120,7 @@
       <c r="BA20" s="51"/>
     </row>
     <row r="21" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="140"/>
+      <c r="A21" s="142"/>
       <c r="B21" s="60" t="s">
         <v>32</v>
       </c>
@@ -10643,21 +10643,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:BA2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="AX3:AY3"/>
-    <mergeCell ref="AZ3:BA3"/>
-    <mergeCell ref="AN3:AO3"/>
-    <mergeCell ref="AP3:AQ3"/>
-    <mergeCell ref="AR3:AS3"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A18"/>
     <mergeCell ref="A19:A21"/>
@@ -10674,6 +10659,21 @@
     <mergeCell ref="AB3:AC3"/>
     <mergeCell ref="AD3:AE3"/>
     <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:BA2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="AX3:AY3"/>
+    <mergeCell ref="AZ3:BA3"/>
+    <mergeCell ref="AN3:AO3"/>
+    <mergeCell ref="AP3:AQ3"/>
+    <mergeCell ref="AR3:AS3"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>
@@ -10703,63 +10703,63 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:53" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="146" t="s">
+      <c r="A2" s="137" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="146"/>
+      <c r="B2" s="137"/>
       <c r="C2" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="F2" s="147" t="s">
+      <c r="F2" s="138" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="147"/>
-      <c r="H2" s="147"/>
-      <c r="I2" s="147"/>
-      <c r="J2" s="147"/>
-      <c r="K2" s="147"/>
-      <c r="L2" s="147"/>
-      <c r="M2" s="147"/>
-      <c r="N2" s="147"/>
-      <c r="O2" s="147"/>
-      <c r="P2" s="147"/>
-      <c r="Q2" s="147"/>
-      <c r="R2" s="147"/>
-      <c r="S2" s="147"/>
-      <c r="T2" s="147"/>
-      <c r="U2" s="147"/>
-      <c r="V2" s="147"/>
-      <c r="W2" s="147"/>
-      <c r="X2" s="147"/>
-      <c r="Y2" s="147"/>
-      <c r="Z2" s="147"/>
-      <c r="AA2" s="147"/>
-      <c r="AB2" s="147"/>
-      <c r="AC2" s="147"/>
-      <c r="AD2" s="147"/>
-      <c r="AE2" s="147"/>
-      <c r="AF2" s="147"/>
-      <c r="AG2" s="147"/>
-      <c r="AH2" s="147"/>
-      <c r="AI2" s="147"/>
-      <c r="AJ2" s="147"/>
-      <c r="AK2" s="147"/>
-      <c r="AL2" s="147"/>
-      <c r="AM2" s="147"/>
-      <c r="AN2" s="147"/>
-      <c r="AO2" s="147"/>
-      <c r="AP2" s="147"/>
-      <c r="AQ2" s="147"/>
-      <c r="AR2" s="147"/>
-      <c r="AS2" s="147"/>
-      <c r="AT2" s="147"/>
-      <c r="AU2" s="147"/>
-      <c r="AV2" s="147"/>
-      <c r="AW2" s="147"/>
-      <c r="AX2" s="147"/>
-      <c r="AY2" s="147"/>
-      <c r="AZ2" s="147"/>
-      <c r="BA2" s="147"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
+      <c r="L2" s="138"/>
+      <c r="M2" s="138"/>
+      <c r="N2" s="138"/>
+      <c r="O2" s="138"/>
+      <c r="P2" s="138"/>
+      <c r="Q2" s="138"/>
+      <c r="R2" s="138"/>
+      <c r="S2" s="138"/>
+      <c r="T2" s="138"/>
+      <c r="U2" s="138"/>
+      <c r="V2" s="138"/>
+      <c r="W2" s="138"/>
+      <c r="X2" s="138"/>
+      <c r="Y2" s="138"/>
+      <c r="Z2" s="138"/>
+      <c r="AA2" s="138"/>
+      <c r="AB2" s="138"/>
+      <c r="AC2" s="138"/>
+      <c r="AD2" s="138"/>
+      <c r="AE2" s="138"/>
+      <c r="AF2" s="138"/>
+      <c r="AG2" s="138"/>
+      <c r="AH2" s="138"/>
+      <c r="AI2" s="138"/>
+      <c r="AJ2" s="138"/>
+      <c r="AK2" s="138"/>
+      <c r="AL2" s="138"/>
+      <c r="AM2" s="138"/>
+      <c r="AN2" s="138"/>
+      <c r="AO2" s="138"/>
+      <c r="AP2" s="138"/>
+      <c r="AQ2" s="138"/>
+      <c r="AR2" s="138"/>
+      <c r="AS2" s="138"/>
+      <c r="AT2" s="138"/>
+      <c r="AU2" s="138"/>
+      <c r="AV2" s="138"/>
+      <c r="AW2" s="138"/>
+      <c r="AX2" s="138"/>
+      <c r="AY2" s="138"/>
+      <c r="AZ2" s="138"/>
+      <c r="BA2" s="138"/>
     </row>
     <row r="3" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
@@ -10777,102 +10777,102 @@
       <c r="E3" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="143">
+      <c r="F3" s="139">
         <v>7</v>
       </c>
-      <c r="G3" s="143"/>
-      <c r="H3" s="143">
+      <c r="G3" s="139"/>
+      <c r="H3" s="139">
         <v>8</v>
       </c>
-      <c r="I3" s="143"/>
-      <c r="J3" s="143">
+      <c r="I3" s="139"/>
+      <c r="J3" s="139">
         <v>9</v>
       </c>
-      <c r="K3" s="143"/>
-      <c r="L3" s="143">
+      <c r="K3" s="139"/>
+      <c r="L3" s="139">
         <v>10</v>
       </c>
-      <c r="M3" s="143"/>
-      <c r="N3" s="143">
+      <c r="M3" s="139"/>
+      <c r="N3" s="139">
         <v>11</v>
       </c>
-      <c r="O3" s="143"/>
-      <c r="P3" s="143">
+      <c r="O3" s="139"/>
+      <c r="P3" s="139">
         <v>12</v>
       </c>
-      <c r="Q3" s="143"/>
-      <c r="R3" s="143">
+      <c r="Q3" s="139"/>
+      <c r="R3" s="139">
         <v>13</v>
       </c>
-      <c r="S3" s="143"/>
-      <c r="T3" s="143">
+      <c r="S3" s="139"/>
+      <c r="T3" s="139">
         <v>14</v>
       </c>
-      <c r="U3" s="143"/>
-      <c r="V3" s="143">
+      <c r="U3" s="139"/>
+      <c r="V3" s="139">
         <v>15</v>
       </c>
-      <c r="W3" s="143"/>
-      <c r="X3" s="143">
+      <c r="W3" s="139"/>
+      <c r="X3" s="139">
         <v>16</v>
       </c>
-      <c r="Y3" s="143"/>
-      <c r="Z3" s="145">
+      <c r="Y3" s="139"/>
+      <c r="Z3" s="146">
         <v>17</v>
       </c>
-      <c r="AA3" s="145"/>
-      <c r="AB3" s="145">
+      <c r="AA3" s="146"/>
+      <c r="AB3" s="146">
         <v>18</v>
       </c>
-      <c r="AC3" s="145"/>
-      <c r="AD3" s="143">
+      <c r="AC3" s="146"/>
+      <c r="AD3" s="139">
         <v>19</v>
       </c>
-      <c r="AE3" s="143"/>
-      <c r="AF3" s="143">
+      <c r="AE3" s="139"/>
+      <c r="AF3" s="139">
         <v>20</v>
       </c>
-      <c r="AG3" s="143"/>
-      <c r="AH3" s="143">
+      <c r="AG3" s="139"/>
+      <c r="AH3" s="139">
         <v>21</v>
       </c>
-      <c r="AI3" s="143"/>
-      <c r="AJ3" s="143">
+      <c r="AI3" s="139"/>
+      <c r="AJ3" s="139">
         <v>22</v>
       </c>
-      <c r="AK3" s="143"/>
-      <c r="AL3" s="143">
+      <c r="AK3" s="139"/>
+      <c r="AL3" s="139">
         <v>23</v>
       </c>
-      <c r="AM3" s="143"/>
-      <c r="AN3" s="143">
+      <c r="AM3" s="139"/>
+      <c r="AN3" s="139">
         <v>24</v>
       </c>
-      <c r="AO3" s="143"/>
-      <c r="AP3" s="143">
+      <c r="AO3" s="139"/>
+      <c r="AP3" s="139">
         <v>1</v>
       </c>
-      <c r="AQ3" s="143"/>
-      <c r="AR3" s="143">
+      <c r="AQ3" s="139"/>
+      <c r="AR3" s="139">
         <v>2</v>
       </c>
-      <c r="AS3" s="143"/>
-      <c r="AT3" s="143">
+      <c r="AS3" s="139"/>
+      <c r="AT3" s="139">
         <v>3</v>
       </c>
-      <c r="AU3" s="143"/>
-      <c r="AV3" s="143">
+      <c r="AU3" s="139"/>
+      <c r="AV3" s="139">
         <v>4</v>
       </c>
-      <c r="AW3" s="143"/>
-      <c r="AX3" s="143">
+      <c r="AW3" s="139"/>
+      <c r="AX3" s="139">
         <v>5</v>
       </c>
-      <c r="AY3" s="143"/>
-      <c r="AZ3" s="143">
+      <c r="AY3" s="139"/>
+      <c r="AZ3" s="139">
         <v>6</v>
       </c>
-      <c r="BA3" s="148"/>
+      <c r="BA3" s="140"/>
     </row>
     <row r="4" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="94" t="s">
@@ -10932,7 +10932,7 @@
       <c r="BA4" s="97"/>
     </row>
     <row r="5" spans="1:53" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="139" t="s">
+      <c r="A5" s="141" t="s">
         <v>82</v>
       </c>
       <c r="B5" s="18" t="s">
@@ -10999,7 +10999,7 @@
       <c r="BA5" s="50"/>
     </row>
     <row r="6" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="142"/>
+      <c r="A6" s="144"/>
       <c r="B6" s="34" t="s">
         <v>24</v>
       </c>
@@ -11064,7 +11064,7 @@
       <c r="BA6" s="51"/>
     </row>
     <row r="7" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="142"/>
+      <c r="A7" s="144"/>
       <c r="B7" s="34" t="s">
         <v>24</v>
       </c>
@@ -11129,7 +11129,7 @@
       <c r="BA7" s="51"/>
     </row>
     <row r="8" spans="1:53" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="142"/>
+      <c r="A8" s="144"/>
       <c r="B8" s="34" t="s">
         <v>24</v>
       </c>
@@ -11194,7 +11194,7 @@
       <c r="BA8" s="51"/>
     </row>
     <row r="9" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="142"/>
+      <c r="A9" s="144"/>
       <c r="B9" s="34" t="s">
         <v>24</v>
       </c>
@@ -11259,7 +11259,7 @@
       <c r="BA9" s="51"/>
     </row>
     <row r="10" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="142"/>
+      <c r="A10" s="144"/>
       <c r="B10" s="34" t="s">
         <v>24</v>
       </c>
@@ -11324,7 +11324,7 @@
       <c r="BA10" s="51"/>
     </row>
     <row r="11" spans="1:53" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="144"/>
+      <c r="A11" s="145"/>
       <c r="B11" s="120" t="s">
         <v>45</v>
       </c>
@@ -11387,7 +11387,7 @@
       <c r="BA11" s="70"/>
     </row>
     <row r="12" spans="1:53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="139" t="s">
+      <c r="A12" s="141" t="s">
         <v>83</v>
       </c>
       <c r="B12" s="124" t="s">
@@ -11454,7 +11454,7 @@
       <c r="BA12" s="50"/>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A13" s="142"/>
+      <c r="A13" s="144"/>
       <c r="B13" s="41" t="s">
         <v>32</v>
       </c>
@@ -11521,7 +11521,7 @@
       <c r="BA13" s="51"/>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A14" s="142"/>
+      <c r="A14" s="144"/>
       <c r="B14" s="41" t="s">
         <v>32</v>
       </c>
@@ -11588,7 +11588,7 @@
       <c r="BA14" s="51"/>
     </row>
     <row r="15" spans="1:53" x14ac:dyDescent="0.25">
-      <c r="A15" s="142"/>
+      <c r="A15" s="144"/>
       <c r="B15" s="41" t="s">
         <v>32</v>
       </c>
@@ -12017,6 +12017,16 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:BA2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T3:U3"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="AH3:AI3"/>
     <mergeCell ref="AJ3:AK3"/>
@@ -12028,21 +12038,11 @@
     <mergeCell ref="AB3:AC3"/>
     <mergeCell ref="AD3:AE3"/>
     <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:BA2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="T3:U3"/>
     <mergeCell ref="AT3:AU3"/>
     <mergeCell ref="AV3:AW3"/>
     <mergeCell ref="AX3:AY3"/>
     <mergeCell ref="AZ3:BA3"/>
+    <mergeCell ref="A5:A11"/>
     <mergeCell ref="AP3:AQ3"/>
     <mergeCell ref="AR3:AS3"/>
   </mergeCells>
@@ -12059,7 +12059,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="X18" sqref="X18"/>
-      <selection pane="bottomLeft" activeCell="AS30" sqref="AS30"/>
+      <selection pane="bottomLeft" activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12074,63 +12074,63 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:101" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="146" t="s">
+      <c r="A2" s="137" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="146"/>
+      <c r="B2" s="137"/>
       <c r="C2" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="147" t="s">
+      <c r="F2" s="138" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="147"/>
-      <c r="H2" s="147"/>
-      <c r="I2" s="147"/>
-      <c r="J2" s="147"/>
-      <c r="K2" s="147"/>
-      <c r="L2" s="147"/>
-      <c r="M2" s="147"/>
-      <c r="N2" s="147"/>
-      <c r="O2" s="147"/>
-      <c r="P2" s="147"/>
-      <c r="Q2" s="147"/>
-      <c r="R2" s="147"/>
-      <c r="S2" s="147"/>
-      <c r="T2" s="147"/>
-      <c r="U2" s="147"/>
-      <c r="V2" s="147"/>
-      <c r="W2" s="147"/>
-      <c r="X2" s="147"/>
-      <c r="Y2" s="147"/>
-      <c r="Z2" s="147"/>
-      <c r="AA2" s="147"/>
-      <c r="AB2" s="147"/>
-      <c r="AC2" s="147"/>
-      <c r="AD2" s="147"/>
-      <c r="AE2" s="147"/>
-      <c r="AF2" s="147"/>
-      <c r="AG2" s="147"/>
-      <c r="AH2" s="147"/>
-      <c r="AI2" s="147"/>
-      <c r="AJ2" s="147"/>
-      <c r="AK2" s="147"/>
-      <c r="AL2" s="147"/>
-      <c r="AM2" s="147"/>
-      <c r="AN2" s="147"/>
-      <c r="AO2" s="147"/>
-      <c r="AP2" s="147"/>
-      <c r="AQ2" s="147"/>
-      <c r="AR2" s="147"/>
-      <c r="AS2" s="147"/>
-      <c r="AT2" s="147"/>
-      <c r="AU2" s="147"/>
-      <c r="AV2" s="147"/>
-      <c r="AW2" s="147"/>
-      <c r="AX2" s="147"/>
-      <c r="AY2" s="147"/>
-      <c r="AZ2" s="147"/>
-      <c r="BA2" s="147"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
+      <c r="L2" s="138"/>
+      <c r="M2" s="138"/>
+      <c r="N2" s="138"/>
+      <c r="O2" s="138"/>
+      <c r="P2" s="138"/>
+      <c r="Q2" s="138"/>
+      <c r="R2" s="138"/>
+      <c r="S2" s="138"/>
+      <c r="T2" s="138"/>
+      <c r="U2" s="138"/>
+      <c r="V2" s="138"/>
+      <c r="W2" s="138"/>
+      <c r="X2" s="138"/>
+      <c r="Y2" s="138"/>
+      <c r="Z2" s="138"/>
+      <c r="AA2" s="138"/>
+      <c r="AB2" s="138"/>
+      <c r="AC2" s="138"/>
+      <c r="AD2" s="138"/>
+      <c r="AE2" s="138"/>
+      <c r="AF2" s="138"/>
+      <c r="AG2" s="138"/>
+      <c r="AH2" s="138"/>
+      <c r="AI2" s="138"/>
+      <c r="AJ2" s="138"/>
+      <c r="AK2" s="138"/>
+      <c r="AL2" s="138"/>
+      <c r="AM2" s="138"/>
+      <c r="AN2" s="138"/>
+      <c r="AO2" s="138"/>
+      <c r="AP2" s="138"/>
+      <c r="AQ2" s="138"/>
+      <c r="AR2" s="138"/>
+      <c r="AS2" s="138"/>
+      <c r="AT2" s="138"/>
+      <c r="AU2" s="138"/>
+      <c r="AV2" s="138"/>
+      <c r="AW2" s="138"/>
+      <c r="AX2" s="138"/>
+      <c r="AY2" s="138"/>
+      <c r="AZ2" s="138"/>
+      <c r="BA2" s="138"/>
     </row>
     <row r="3" spans="1:101" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="104" t="s">
@@ -12148,150 +12148,150 @@
       <c r="E3" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="156">
+      <c r="F3" s="147">
         <v>7</v>
       </c>
-      <c r="G3" s="157"/>
-      <c r="H3" s="157"/>
-      <c r="I3" s="158"/>
-      <c r="J3" s="149">
+      <c r="G3" s="148"/>
+      <c r="H3" s="148"/>
+      <c r="I3" s="149"/>
+      <c r="J3" s="150">
         <v>8</v>
       </c>
-      <c r="K3" s="150"/>
-      <c r="L3" s="150"/>
-      <c r="M3" s="151"/>
-      <c r="N3" s="149">
+      <c r="K3" s="151"/>
+      <c r="L3" s="151"/>
+      <c r="M3" s="152"/>
+      <c r="N3" s="150">
         <v>9</v>
       </c>
-      <c r="O3" s="150"/>
-      <c r="P3" s="150"/>
-      <c r="Q3" s="151"/>
-      <c r="R3" s="149">
+      <c r="O3" s="151"/>
+      <c r="P3" s="151"/>
+      <c r="Q3" s="152"/>
+      <c r="R3" s="150">
         <v>10</v>
       </c>
-      <c r="S3" s="150"/>
-      <c r="T3" s="150"/>
-      <c r="U3" s="151"/>
-      <c r="V3" s="149">
+      <c r="S3" s="151"/>
+      <c r="T3" s="151"/>
+      <c r="U3" s="152"/>
+      <c r="V3" s="150">
         <v>11</v>
       </c>
-      <c r="W3" s="150"/>
-      <c r="X3" s="150"/>
-      <c r="Y3" s="151"/>
-      <c r="Z3" s="159">
+      <c r="W3" s="151"/>
+      <c r="X3" s="151"/>
+      <c r="Y3" s="152"/>
+      <c r="Z3" s="153">
         <v>12</v>
       </c>
-      <c r="AA3" s="160"/>
-      <c r="AB3" s="160"/>
-      <c r="AC3" s="161"/>
-      <c r="AD3" s="149">
+      <c r="AA3" s="154"/>
+      <c r="AB3" s="154"/>
+      <c r="AC3" s="155"/>
+      <c r="AD3" s="150">
         <v>13</v>
       </c>
-      <c r="AE3" s="150"/>
-      <c r="AF3" s="150"/>
-      <c r="AG3" s="151"/>
-      <c r="AH3" s="149">
+      <c r="AE3" s="151"/>
+      <c r="AF3" s="151"/>
+      <c r="AG3" s="152"/>
+      <c r="AH3" s="150">
         <v>14</v>
       </c>
-      <c r="AI3" s="150"/>
-      <c r="AJ3" s="150"/>
-      <c r="AK3" s="151"/>
-      <c r="AL3" s="149">
+      <c r="AI3" s="151"/>
+      <c r="AJ3" s="151"/>
+      <c r="AK3" s="152"/>
+      <c r="AL3" s="150">
         <v>15</v>
       </c>
-      <c r="AM3" s="150"/>
-      <c r="AN3" s="150"/>
-      <c r="AO3" s="151"/>
-      <c r="AP3" s="149">
+      <c r="AM3" s="151"/>
+      <c r="AN3" s="151"/>
+      <c r="AO3" s="152"/>
+      <c r="AP3" s="150">
         <v>16</v>
       </c>
-      <c r="AQ3" s="150"/>
-      <c r="AR3" s="150"/>
-      <c r="AS3" s="151"/>
-      <c r="AT3" s="149">
+      <c r="AQ3" s="151"/>
+      <c r="AR3" s="151"/>
+      <c r="AS3" s="152"/>
+      <c r="AT3" s="150">
         <v>17</v>
       </c>
-      <c r="AU3" s="150"/>
-      <c r="AV3" s="150"/>
-      <c r="AW3" s="151"/>
-      <c r="AX3" s="149">
+      <c r="AU3" s="151"/>
+      <c r="AV3" s="151"/>
+      <c r="AW3" s="152"/>
+      <c r="AX3" s="150">
         <v>18</v>
       </c>
-      <c r="AY3" s="150"/>
-      <c r="AZ3" s="150"/>
-      <c r="BA3" s="152"/>
-      <c r="BB3" s="156">
+      <c r="AY3" s="151"/>
+      <c r="AZ3" s="151"/>
+      <c r="BA3" s="159"/>
+      <c r="BB3" s="147">
         <v>19</v>
       </c>
-      <c r="BC3" s="157"/>
-      <c r="BD3" s="157"/>
-      <c r="BE3" s="158"/>
-      <c r="BF3" s="149">
+      <c r="BC3" s="148"/>
+      <c r="BD3" s="148"/>
+      <c r="BE3" s="149"/>
+      <c r="BF3" s="150">
         <v>20</v>
       </c>
-      <c r="BG3" s="150"/>
-      <c r="BH3" s="150"/>
-      <c r="BI3" s="151"/>
-      <c r="BJ3" s="149">
+      <c r="BG3" s="151"/>
+      <c r="BH3" s="151"/>
+      <c r="BI3" s="152"/>
+      <c r="BJ3" s="150">
         <v>21</v>
       </c>
-      <c r="BK3" s="150"/>
-      <c r="BL3" s="150"/>
-      <c r="BM3" s="151"/>
-      <c r="BN3" s="149">
+      <c r="BK3" s="151"/>
+      <c r="BL3" s="151"/>
+      <c r="BM3" s="152"/>
+      <c r="BN3" s="150">
         <v>22</v>
       </c>
-      <c r="BO3" s="150"/>
-      <c r="BP3" s="150"/>
-      <c r="BQ3" s="151"/>
-      <c r="BR3" s="149">
+      <c r="BO3" s="151"/>
+      <c r="BP3" s="151"/>
+      <c r="BQ3" s="152"/>
+      <c r="BR3" s="150">
         <v>23</v>
       </c>
-      <c r="BS3" s="150"/>
-      <c r="BT3" s="150"/>
-      <c r="BU3" s="150"/>
-      <c r="BV3" s="153">
+      <c r="BS3" s="151"/>
+      <c r="BT3" s="151"/>
+      <c r="BU3" s="151"/>
+      <c r="BV3" s="156">
         <v>24</v>
       </c>
-      <c r="BW3" s="154"/>
-      <c r="BX3" s="154"/>
-      <c r="BY3" s="155"/>
-      <c r="BZ3" s="150">
+      <c r="BW3" s="157"/>
+      <c r="BX3" s="157"/>
+      <c r="BY3" s="158"/>
+      <c r="BZ3" s="151">
         <v>1</v>
       </c>
-      <c r="CA3" s="150"/>
-      <c r="CB3" s="150"/>
-      <c r="CC3" s="151"/>
-      <c r="CD3" s="149">
+      <c r="CA3" s="151"/>
+      <c r="CB3" s="151"/>
+      <c r="CC3" s="152"/>
+      <c r="CD3" s="150">
         <v>2</v>
       </c>
-      <c r="CE3" s="150"/>
-      <c r="CF3" s="150"/>
-      <c r="CG3" s="151"/>
-      <c r="CH3" s="149">
+      <c r="CE3" s="151"/>
+      <c r="CF3" s="151"/>
+      <c r="CG3" s="152"/>
+      <c r="CH3" s="150">
         <v>3</v>
       </c>
-      <c r="CI3" s="150"/>
-      <c r="CJ3" s="150"/>
-      <c r="CK3" s="151"/>
-      <c r="CL3" s="149">
+      <c r="CI3" s="151"/>
+      <c r="CJ3" s="151"/>
+      <c r="CK3" s="152"/>
+      <c r="CL3" s="150">
         <v>4</v>
       </c>
-      <c r="CM3" s="150"/>
-      <c r="CN3" s="150"/>
-      <c r="CO3" s="151"/>
-      <c r="CP3" s="149">
+      <c r="CM3" s="151"/>
+      <c r="CN3" s="151"/>
+      <c r="CO3" s="152"/>
+      <c r="CP3" s="150">
         <v>5</v>
       </c>
-      <c r="CQ3" s="150"/>
-      <c r="CR3" s="150"/>
-      <c r="CS3" s="151"/>
-      <c r="CT3" s="149">
+      <c r="CQ3" s="151"/>
+      <c r="CR3" s="151"/>
+      <c r="CS3" s="152"/>
+      <c r="CT3" s="150">
         <v>6</v>
       </c>
-      <c r="CU3" s="150"/>
-      <c r="CV3" s="150"/>
-      <c r="CW3" s="152"/>
+      <c r="CU3" s="151"/>
+      <c r="CV3" s="151"/>
+      <c r="CW3" s="159"/>
     </row>
     <row r="4" spans="1:101" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="106" t="s">
@@ -12399,7 +12399,7 @@
       <c r="CW4" s="112"/>
     </row>
     <row r="5" spans="1:101" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="139" t="s">
+      <c r="A5" s="141" t="s">
         <v>82</v>
       </c>
       <c r="B5" s="18" t="s">
@@ -12512,7 +12512,7 @@
       <c r="CW5" s="117"/>
     </row>
     <row r="6" spans="1:101" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="142"/>
+      <c r="A6" s="144"/>
       <c r="B6" s="34" t="s">
         <v>24</v>
       </c>
@@ -12623,7 +12623,7 @@
       <c r="CW6" s="117"/>
     </row>
     <row r="7" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A7" s="142"/>
+      <c r="A7" s="144"/>
       <c r="B7" s="34" t="s">
         <v>24</v>
       </c>
@@ -12734,7 +12734,7 @@
       <c r="CW7" s="117"/>
     </row>
     <row r="8" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A8" s="142"/>
+      <c r="A8" s="144"/>
       <c r="B8" s="34" t="s">
         <v>24</v>
       </c>
@@ -12845,7 +12845,7 @@
       <c r="CW8" s="117"/>
     </row>
     <row r="9" spans="1:101" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="142"/>
+      <c r="A9" s="144"/>
       <c r="B9" s="34" t="s">
         <v>24</v>
       </c>
@@ -12956,7 +12956,7 @@
       <c r="CW9" s="117"/>
     </row>
     <row r="10" spans="1:101" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="142"/>
+      <c r="A10" s="144"/>
       <c r="B10" s="34" t="s">
         <v>24</v>
       </c>
@@ -13067,7 +13067,7 @@
       <c r="CW10" s="117"/>
     </row>
     <row r="11" spans="1:101" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="144"/>
+      <c r="A11" s="145"/>
       <c r="B11" s="120" t="s">
         <v>45</v>
       </c>
@@ -13176,7 +13176,7 @@
       <c r="CW11" s="117"/>
     </row>
     <row r="12" spans="1:101" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="139" t="s">
+      <c r="A12" s="141" t="s">
         <v>83</v>
       </c>
       <c r="B12" s="124" t="s">
@@ -13289,7 +13289,7 @@
       <c r="CW12" s="117"/>
     </row>
     <row r="13" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A13" s="142"/>
+      <c r="A13" s="144"/>
       <c r="B13" s="41" t="s">
         <v>32</v>
       </c>
@@ -13400,7 +13400,7 @@
       <c r="CW13" s="117"/>
     </row>
     <row r="14" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A14" s="142"/>
+      <c r="A14" s="144"/>
       <c r="B14" s="41" t="s">
         <v>32</v>
       </c>
@@ -13511,7 +13511,7 @@
       <c r="CW14" s="117"/>
     </row>
     <row r="15" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A15" s="142"/>
+      <c r="A15" s="144"/>
       <c r="B15" s="41" t="s">
         <v>32</v>
       </c>
@@ -13682,67 +13682,67 @@
       <c r="C17" s="79"/>
       <c r="D17" s="80"/>
       <c r="E17" s="81"/>
-      <c r="F17" s="136"/>
-      <c r="G17" s="136"/>
-      <c r="H17" s="136"/>
-      <c r="I17" s="136"/>
-      <c r="J17" s="136"/>
-      <c r="K17" s="136"/>
-      <c r="L17" s="136"/>
-      <c r="M17" s="136"/>
-      <c r="N17" s="136"/>
-      <c r="O17" s="137"/>
-      <c r="P17" s="137"/>
-      <c r="Q17" s="137"/>
-      <c r="R17" s="137"/>
-      <c r="S17" s="137"/>
-      <c r="T17" s="137"/>
-      <c r="U17" s="137"/>
-      <c r="V17" s="137"/>
-      <c r="W17" s="137"/>
-      <c r="X17" s="137"/>
-      <c r="Y17" s="137"/>
-      <c r="Z17" s="137"/>
-      <c r="AA17" s="137"/>
-      <c r="AB17" s="137"/>
-      <c r="AC17" s="137"/>
-      <c r="AD17" s="137"/>
-      <c r="AE17" s="137"/>
-      <c r="AF17" s="137"/>
-      <c r="AG17" s="137"/>
-      <c r="AH17" s="137"/>
-      <c r="AI17" s="137"/>
-      <c r="AJ17" s="137"/>
-      <c r="AK17" s="137"/>
-      <c r="AL17" s="137"/>
-      <c r="AM17" s="137"/>
-      <c r="AN17" s="137"/>
-      <c r="AO17" s="137"/>
-      <c r="AP17" s="137"/>
-      <c r="AQ17" s="137"/>
-      <c r="AR17" s="137"/>
-      <c r="AS17" s="137"/>
-      <c r="AT17" s="137"/>
-      <c r="AU17" s="137"/>
-      <c r="AV17" s="137"/>
-      <c r="AW17" s="137"/>
-      <c r="AX17" s="137"/>
-      <c r="AY17" s="137"/>
-      <c r="AZ17" s="137"/>
-      <c r="BA17" s="137"/>
-      <c r="BB17" s="137"/>
-      <c r="BC17" s="137"/>
-      <c r="BD17" s="137"/>
-      <c r="BE17" s="137"/>
-      <c r="BF17" s="137"/>
-      <c r="BG17" s="137"/>
-      <c r="BH17" s="137"/>
-      <c r="BI17" s="136"/>
-      <c r="BJ17" s="136"/>
-      <c r="BK17" s="136"/>
-      <c r="BL17" s="136"/>
-      <c r="BM17" s="136"/>
-      <c r="BN17" s="136"/>
+      <c r="F17" s="160"/>
+      <c r="G17" s="160"/>
+      <c r="H17" s="160"/>
+      <c r="I17" s="160"/>
+      <c r="J17" s="160"/>
+      <c r="K17" s="160"/>
+      <c r="L17" s="160"/>
+      <c r="M17" s="160"/>
+      <c r="N17" s="160"/>
+      <c r="O17" s="161"/>
+      <c r="P17" s="161"/>
+      <c r="Q17" s="161"/>
+      <c r="R17" s="161"/>
+      <c r="S17" s="161"/>
+      <c r="T17" s="161"/>
+      <c r="U17" s="161"/>
+      <c r="V17" s="161"/>
+      <c r="W17" s="161"/>
+      <c r="X17" s="161"/>
+      <c r="Y17" s="161"/>
+      <c r="Z17" s="161"/>
+      <c r="AA17" s="161"/>
+      <c r="AB17" s="161"/>
+      <c r="AC17" s="161"/>
+      <c r="AD17" s="161"/>
+      <c r="AE17" s="161"/>
+      <c r="AF17" s="161"/>
+      <c r="AG17" s="161"/>
+      <c r="AH17" s="161"/>
+      <c r="AI17" s="161"/>
+      <c r="AJ17" s="161"/>
+      <c r="AK17" s="161"/>
+      <c r="AL17" s="161"/>
+      <c r="AM17" s="161"/>
+      <c r="AN17" s="161"/>
+      <c r="AO17" s="161"/>
+      <c r="AP17" s="161"/>
+      <c r="AQ17" s="161"/>
+      <c r="AR17" s="161"/>
+      <c r="AS17" s="161"/>
+      <c r="AT17" s="161"/>
+      <c r="AU17" s="161"/>
+      <c r="AV17" s="161"/>
+      <c r="AW17" s="161"/>
+      <c r="AX17" s="161"/>
+      <c r="AY17" s="161"/>
+      <c r="AZ17" s="161"/>
+      <c r="BA17" s="161"/>
+      <c r="BB17" s="161"/>
+      <c r="BC17" s="161"/>
+      <c r="BD17" s="161"/>
+      <c r="BE17" s="161"/>
+      <c r="BF17" s="161"/>
+      <c r="BG17" s="161"/>
+      <c r="BH17" s="161"/>
+      <c r="BI17" s="160"/>
+      <c r="BJ17" s="160"/>
+      <c r="BK17" s="160"/>
+      <c r="BL17" s="160"/>
+      <c r="BM17" s="160"/>
+      <c r="BN17" s="160"/>
     </row>
     <row r="18" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A18" s="77"/>
@@ -13750,67 +13750,67 @@
       <c r="C18" s="79"/>
       <c r="D18" s="80"/>
       <c r="E18" s="129"/>
-      <c r="F18" s="136"/>
-      <c r="G18" s="136"/>
-      <c r="H18" s="136"/>
-      <c r="I18" s="136"/>
-      <c r="J18" s="136"/>
-      <c r="K18" s="136"/>
-      <c r="L18" s="136"/>
-      <c r="M18" s="136"/>
-      <c r="N18" s="136"/>
-      <c r="O18" s="137"/>
-      <c r="P18" s="137"/>
-      <c r="Q18" s="137"/>
-      <c r="R18" s="137"/>
-      <c r="S18" s="137"/>
-      <c r="T18" s="137"/>
-      <c r="U18" s="137"/>
-      <c r="V18" s="137"/>
-      <c r="W18" s="137"/>
-      <c r="X18" s="137"/>
-      <c r="Y18" s="137"/>
-      <c r="Z18" s="137"/>
-      <c r="AA18" s="137"/>
-      <c r="AB18" s="137"/>
-      <c r="AC18" s="137"/>
-      <c r="AD18" s="137"/>
-      <c r="AE18" s="137"/>
-      <c r="AF18" s="137"/>
-      <c r="AG18" s="137"/>
-      <c r="AH18" s="137"/>
-      <c r="AI18" s="137"/>
-      <c r="AJ18" s="137"/>
-      <c r="AK18" s="137"/>
-      <c r="AL18" s="137"/>
-      <c r="AM18" s="137"/>
-      <c r="AN18" s="137"/>
-      <c r="AO18" s="137"/>
-      <c r="AP18" s="137"/>
-      <c r="AQ18" s="137"/>
-      <c r="AR18" s="137"/>
-      <c r="AS18" s="137"/>
-      <c r="AT18" s="137"/>
-      <c r="AU18" s="137"/>
-      <c r="AV18" s="137"/>
-      <c r="AW18" s="137"/>
-      <c r="AX18" s="137"/>
-      <c r="AY18" s="137"/>
-      <c r="AZ18" s="137"/>
-      <c r="BA18" s="137"/>
-      <c r="BB18" s="137"/>
-      <c r="BC18" s="137"/>
-      <c r="BD18" s="137"/>
-      <c r="BE18" s="137"/>
-      <c r="BF18" s="137"/>
-      <c r="BG18" s="137"/>
-      <c r="BH18" s="137"/>
-      <c r="BI18" s="136"/>
-      <c r="BJ18" s="136"/>
-      <c r="BK18" s="136"/>
-      <c r="BL18" s="136"/>
-      <c r="BM18" s="136"/>
-      <c r="BN18" s="136"/>
+      <c r="F18" s="160"/>
+      <c r="G18" s="160"/>
+      <c r="H18" s="160"/>
+      <c r="I18" s="160"/>
+      <c r="J18" s="160"/>
+      <c r="K18" s="160"/>
+      <c r="L18" s="160"/>
+      <c r="M18" s="160"/>
+      <c r="N18" s="160"/>
+      <c r="O18" s="161"/>
+      <c r="P18" s="161"/>
+      <c r="Q18" s="161"/>
+      <c r="R18" s="161"/>
+      <c r="S18" s="161"/>
+      <c r="T18" s="161"/>
+      <c r="U18" s="161"/>
+      <c r="V18" s="161"/>
+      <c r="W18" s="161"/>
+      <c r="X18" s="161"/>
+      <c r="Y18" s="161"/>
+      <c r="Z18" s="161"/>
+      <c r="AA18" s="161"/>
+      <c r="AB18" s="161"/>
+      <c r="AC18" s="161"/>
+      <c r="AD18" s="161"/>
+      <c r="AE18" s="161"/>
+      <c r="AF18" s="161"/>
+      <c r="AG18" s="161"/>
+      <c r="AH18" s="161"/>
+      <c r="AI18" s="161"/>
+      <c r="AJ18" s="161"/>
+      <c r="AK18" s="161"/>
+      <c r="AL18" s="161"/>
+      <c r="AM18" s="161"/>
+      <c r="AN18" s="161"/>
+      <c r="AO18" s="161"/>
+      <c r="AP18" s="161"/>
+      <c r="AQ18" s="161"/>
+      <c r="AR18" s="161"/>
+      <c r="AS18" s="161"/>
+      <c r="AT18" s="161"/>
+      <c r="AU18" s="161"/>
+      <c r="AV18" s="161"/>
+      <c r="AW18" s="161"/>
+      <c r="AX18" s="161"/>
+      <c r="AY18" s="161"/>
+      <c r="AZ18" s="161"/>
+      <c r="BA18" s="161"/>
+      <c r="BB18" s="161"/>
+      <c r="BC18" s="161"/>
+      <c r="BD18" s="161"/>
+      <c r="BE18" s="161"/>
+      <c r="BF18" s="161"/>
+      <c r="BG18" s="161"/>
+      <c r="BH18" s="161"/>
+      <c r="BI18" s="160"/>
+      <c r="BJ18" s="160"/>
+      <c r="BK18" s="160"/>
+      <c r="BL18" s="160"/>
+      <c r="BM18" s="160"/>
+      <c r="BN18" s="160"/>
     </row>
     <row r="19" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A19" s="77"/>
@@ -13818,67 +13818,67 @@
       <c r="C19" s="79"/>
       <c r="D19" s="80"/>
       <c r="E19" s="81"/>
-      <c r="F19" s="136"/>
-      <c r="G19" s="136"/>
-      <c r="H19" s="136"/>
-      <c r="I19" s="136"/>
-      <c r="J19" s="136"/>
-      <c r="K19" s="136"/>
-      <c r="L19" s="136"/>
-      <c r="M19" s="136"/>
-      <c r="N19" s="136"/>
-      <c r="O19" s="136"/>
-      <c r="P19" s="136"/>
-      <c r="Q19" s="136"/>
-      <c r="R19" s="136"/>
-      <c r="S19" s="136"/>
-      <c r="T19" s="136"/>
-      <c r="U19" s="136"/>
-      <c r="V19" s="136"/>
-      <c r="W19" s="136"/>
-      <c r="X19" s="136"/>
-      <c r="Y19" s="136"/>
-      <c r="Z19" s="136"/>
-      <c r="AA19" s="136"/>
-      <c r="AB19" s="136"/>
-      <c r="AC19" s="136"/>
-      <c r="AD19" s="137"/>
-      <c r="AE19" s="137"/>
-      <c r="AF19" s="137"/>
-      <c r="AG19" s="137"/>
-      <c r="AH19" s="137"/>
-      <c r="AI19" s="137"/>
-      <c r="AJ19" s="137"/>
-      <c r="AK19" s="136"/>
-      <c r="AL19" s="136"/>
-      <c r="AM19" s="136"/>
-      <c r="AN19" s="136"/>
-      <c r="AO19" s="136"/>
-      <c r="AP19" s="136"/>
-      <c r="AQ19" s="136"/>
-      <c r="AR19" s="136"/>
-      <c r="AS19" s="136"/>
-      <c r="AT19" s="136"/>
-      <c r="AU19" s="136"/>
-      <c r="AV19" s="136"/>
-      <c r="AW19" s="136"/>
-      <c r="AX19" s="136"/>
-      <c r="AY19" s="136"/>
-      <c r="AZ19" s="136"/>
-      <c r="BA19" s="136"/>
-      <c r="BB19" s="136"/>
-      <c r="BC19" s="136"/>
-      <c r="BD19" s="136"/>
-      <c r="BE19" s="136"/>
-      <c r="BF19" s="136"/>
-      <c r="BG19" s="136"/>
-      <c r="BH19" s="136"/>
-      <c r="BI19" s="136"/>
-      <c r="BJ19" s="136"/>
-      <c r="BK19" s="136"/>
-      <c r="BL19" s="136"/>
-      <c r="BM19" s="136"/>
-      <c r="BN19" s="136"/>
+      <c r="F19" s="160"/>
+      <c r="G19" s="160"/>
+      <c r="H19" s="160"/>
+      <c r="I19" s="160"/>
+      <c r="J19" s="160"/>
+      <c r="K19" s="160"/>
+      <c r="L19" s="160"/>
+      <c r="M19" s="160"/>
+      <c r="N19" s="160"/>
+      <c r="O19" s="160"/>
+      <c r="P19" s="160"/>
+      <c r="Q19" s="160"/>
+      <c r="R19" s="160"/>
+      <c r="S19" s="160"/>
+      <c r="T19" s="160"/>
+      <c r="U19" s="160"/>
+      <c r="V19" s="160"/>
+      <c r="W19" s="160"/>
+      <c r="X19" s="160"/>
+      <c r="Y19" s="160"/>
+      <c r="Z19" s="160"/>
+      <c r="AA19" s="160"/>
+      <c r="AB19" s="160"/>
+      <c r="AC19" s="160"/>
+      <c r="AD19" s="161"/>
+      <c r="AE19" s="161"/>
+      <c r="AF19" s="161"/>
+      <c r="AG19" s="161"/>
+      <c r="AH19" s="161"/>
+      <c r="AI19" s="161"/>
+      <c r="AJ19" s="161"/>
+      <c r="AK19" s="160"/>
+      <c r="AL19" s="160"/>
+      <c r="AM19" s="160"/>
+      <c r="AN19" s="160"/>
+      <c r="AO19" s="160"/>
+      <c r="AP19" s="160"/>
+      <c r="AQ19" s="160"/>
+      <c r="AR19" s="160"/>
+      <c r="AS19" s="160"/>
+      <c r="AT19" s="160"/>
+      <c r="AU19" s="160"/>
+      <c r="AV19" s="160"/>
+      <c r="AW19" s="160"/>
+      <c r="AX19" s="160"/>
+      <c r="AY19" s="160"/>
+      <c r="AZ19" s="160"/>
+      <c r="BA19" s="160"/>
+      <c r="BB19" s="160"/>
+      <c r="BC19" s="160"/>
+      <c r="BD19" s="160"/>
+      <c r="BE19" s="160"/>
+      <c r="BF19" s="160"/>
+      <c r="BG19" s="160"/>
+      <c r="BH19" s="160"/>
+      <c r="BI19" s="160"/>
+      <c r="BJ19" s="160"/>
+      <c r="BK19" s="160"/>
+      <c r="BL19" s="160"/>
+      <c r="BM19" s="160"/>
+      <c r="BN19" s="160"/>
     </row>
     <row r="20" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A20" s="77"/>
@@ -13886,67 +13886,67 @@
       <c r="C20" s="79"/>
       <c r="D20" s="80"/>
       <c r="E20" s="81"/>
-      <c r="F20" s="136"/>
-      <c r="G20" s="136"/>
-      <c r="H20" s="136"/>
-      <c r="I20" s="136"/>
-      <c r="J20" s="136"/>
-      <c r="K20" s="136"/>
-      <c r="L20" s="136"/>
-      <c r="M20" s="136"/>
-      <c r="N20" s="136"/>
-      <c r="O20" s="136"/>
-      <c r="P20" s="136"/>
-      <c r="Q20" s="136"/>
-      <c r="R20" s="136"/>
-      <c r="S20" s="137"/>
-      <c r="T20" s="137"/>
-      <c r="U20" s="137"/>
-      <c r="V20" s="137"/>
-      <c r="W20" s="137"/>
-      <c r="X20" s="137"/>
-      <c r="Y20" s="137"/>
-      <c r="Z20" s="137"/>
-      <c r="AA20" s="137"/>
-      <c r="AB20" s="137"/>
-      <c r="AC20" s="137"/>
-      <c r="AD20" s="137"/>
-      <c r="AE20" s="137"/>
-      <c r="AF20" s="137"/>
-      <c r="AG20" s="137"/>
-      <c r="AH20" s="137"/>
-      <c r="AI20" s="137"/>
-      <c r="AJ20" s="137"/>
-      <c r="AK20" s="137"/>
-      <c r="AL20" s="137"/>
-      <c r="AM20" s="137"/>
-      <c r="AN20" s="137"/>
-      <c r="AO20" s="137"/>
-      <c r="AP20" s="137"/>
-      <c r="AQ20" s="137"/>
-      <c r="AR20" s="137"/>
-      <c r="AS20" s="137"/>
-      <c r="AT20" s="137"/>
-      <c r="AU20" s="137"/>
-      <c r="AV20" s="137"/>
-      <c r="AW20" s="137"/>
-      <c r="AX20" s="137"/>
-      <c r="AY20" s="137"/>
-      <c r="AZ20" s="137"/>
-      <c r="BA20" s="137"/>
-      <c r="BB20" s="137"/>
-      <c r="BC20" s="137"/>
-      <c r="BD20" s="137"/>
-      <c r="BE20" s="137"/>
-      <c r="BF20" s="137"/>
-      <c r="BG20" s="137"/>
-      <c r="BH20" s="136"/>
-      <c r="BI20" s="136"/>
-      <c r="BJ20" s="136"/>
-      <c r="BK20" s="136"/>
-      <c r="BL20" s="136"/>
-      <c r="BM20" s="136"/>
-      <c r="BN20" s="136"/>
+      <c r="F20" s="160"/>
+      <c r="G20" s="160"/>
+      <c r="H20" s="160"/>
+      <c r="I20" s="160"/>
+      <c r="J20" s="160"/>
+      <c r="K20" s="160"/>
+      <c r="L20" s="160"/>
+      <c r="M20" s="160"/>
+      <c r="N20" s="160"/>
+      <c r="O20" s="160"/>
+      <c r="P20" s="160"/>
+      <c r="Q20" s="160"/>
+      <c r="R20" s="160"/>
+      <c r="S20" s="161"/>
+      <c r="T20" s="161"/>
+      <c r="U20" s="161"/>
+      <c r="V20" s="161"/>
+      <c r="W20" s="161"/>
+      <c r="X20" s="161"/>
+      <c r="Y20" s="161"/>
+      <c r="Z20" s="161"/>
+      <c r="AA20" s="161"/>
+      <c r="AB20" s="161"/>
+      <c r="AC20" s="161"/>
+      <c r="AD20" s="161"/>
+      <c r="AE20" s="161"/>
+      <c r="AF20" s="161"/>
+      <c r="AG20" s="161"/>
+      <c r="AH20" s="161"/>
+      <c r="AI20" s="161"/>
+      <c r="AJ20" s="161"/>
+      <c r="AK20" s="161"/>
+      <c r="AL20" s="161"/>
+      <c r="AM20" s="161"/>
+      <c r="AN20" s="161"/>
+      <c r="AO20" s="161"/>
+      <c r="AP20" s="161"/>
+      <c r="AQ20" s="161"/>
+      <c r="AR20" s="161"/>
+      <c r="AS20" s="161"/>
+      <c r="AT20" s="161"/>
+      <c r="AU20" s="161"/>
+      <c r="AV20" s="161"/>
+      <c r="AW20" s="161"/>
+      <c r="AX20" s="161"/>
+      <c r="AY20" s="161"/>
+      <c r="AZ20" s="161"/>
+      <c r="BA20" s="161"/>
+      <c r="BB20" s="161"/>
+      <c r="BC20" s="161"/>
+      <c r="BD20" s="161"/>
+      <c r="BE20" s="161"/>
+      <c r="BF20" s="161"/>
+      <c r="BG20" s="161"/>
+      <c r="BH20" s="160"/>
+      <c r="BI20" s="160"/>
+      <c r="BJ20" s="160"/>
+      <c r="BK20" s="160"/>
+      <c r="BL20" s="160"/>
+      <c r="BM20" s="160"/>
+      <c r="BN20" s="160"/>
     </row>
     <row r="21" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A21" s="77"/>
@@ -13954,256 +13954,256 @@
       <c r="C21" s="79"/>
       <c r="D21" s="80"/>
       <c r="E21" s="81"/>
-      <c r="F21" s="136"/>
-      <c r="G21" s="136"/>
-      <c r="H21" s="136"/>
-      <c r="I21" s="136"/>
-      <c r="J21" s="136"/>
-      <c r="K21" s="136"/>
-      <c r="L21" s="136"/>
-      <c r="M21" s="136"/>
-      <c r="N21" s="136"/>
-      <c r="O21" s="137"/>
-      <c r="P21" s="137"/>
-      <c r="Q21" s="137"/>
-      <c r="R21" s="137"/>
-      <c r="S21" s="137"/>
-      <c r="T21" s="137"/>
-      <c r="U21" s="137"/>
-      <c r="V21" s="137"/>
-      <c r="W21" s="137"/>
-      <c r="X21" s="137"/>
-      <c r="Y21" s="137"/>
-      <c r="Z21" s="137"/>
-      <c r="AA21" s="137"/>
-      <c r="AB21" s="137"/>
-      <c r="AC21" s="137"/>
-      <c r="AD21" s="137"/>
-      <c r="AE21" s="137"/>
-      <c r="AF21" s="137"/>
-      <c r="AG21" s="137"/>
-      <c r="AH21" s="137"/>
-      <c r="AI21" s="137"/>
-      <c r="AJ21" s="137"/>
-      <c r="AK21" s="137"/>
-      <c r="AL21" s="137"/>
-      <c r="AM21" s="137"/>
-      <c r="AN21" s="137"/>
-      <c r="AO21" s="137"/>
-      <c r="AP21" s="137"/>
-      <c r="AQ21" s="137"/>
-      <c r="AR21" s="137"/>
-      <c r="AS21" s="137"/>
-      <c r="AT21" s="137"/>
-      <c r="AU21" s="137"/>
-      <c r="AV21" s="137"/>
-      <c r="AW21" s="137"/>
-      <c r="AX21" s="137"/>
-      <c r="AY21" s="137"/>
-      <c r="AZ21" s="137"/>
-      <c r="BA21" s="137"/>
-      <c r="BB21" s="137"/>
-      <c r="BC21" s="137"/>
-      <c r="BD21" s="137"/>
-      <c r="BE21" s="137"/>
-      <c r="BF21" s="137"/>
-      <c r="BG21" s="137"/>
-      <c r="BH21" s="136"/>
-      <c r="BI21" s="136"/>
-      <c r="BJ21" s="136"/>
-      <c r="BK21" s="136"/>
-      <c r="BL21" s="136"/>
-      <c r="BM21" s="136"/>
-      <c r="BN21" s="136"/>
+      <c r="F21" s="160"/>
+      <c r="G21" s="160"/>
+      <c r="H21" s="160"/>
+      <c r="I21" s="160"/>
+      <c r="J21" s="160"/>
+      <c r="K21" s="160"/>
+      <c r="L21" s="160"/>
+      <c r="M21" s="160"/>
+      <c r="N21" s="160"/>
+      <c r="O21" s="161"/>
+      <c r="P21" s="161"/>
+      <c r="Q21" s="161"/>
+      <c r="R21" s="161"/>
+      <c r="S21" s="161"/>
+      <c r="T21" s="161"/>
+      <c r="U21" s="161"/>
+      <c r="V21" s="161"/>
+      <c r="W21" s="161"/>
+      <c r="X21" s="161"/>
+      <c r="Y21" s="161"/>
+      <c r="Z21" s="161"/>
+      <c r="AA21" s="161"/>
+      <c r="AB21" s="161"/>
+      <c r="AC21" s="161"/>
+      <c r="AD21" s="161"/>
+      <c r="AE21" s="161"/>
+      <c r="AF21" s="161"/>
+      <c r="AG21" s="161"/>
+      <c r="AH21" s="161"/>
+      <c r="AI21" s="161"/>
+      <c r="AJ21" s="161"/>
+      <c r="AK21" s="161"/>
+      <c r="AL21" s="161"/>
+      <c r="AM21" s="161"/>
+      <c r="AN21" s="161"/>
+      <c r="AO21" s="161"/>
+      <c r="AP21" s="161"/>
+      <c r="AQ21" s="161"/>
+      <c r="AR21" s="161"/>
+      <c r="AS21" s="161"/>
+      <c r="AT21" s="161"/>
+      <c r="AU21" s="161"/>
+      <c r="AV21" s="161"/>
+      <c r="AW21" s="161"/>
+      <c r="AX21" s="161"/>
+      <c r="AY21" s="161"/>
+      <c r="AZ21" s="161"/>
+      <c r="BA21" s="161"/>
+      <c r="BB21" s="161"/>
+      <c r="BC21" s="161"/>
+      <c r="BD21" s="161"/>
+      <c r="BE21" s="161"/>
+      <c r="BF21" s="161"/>
+      <c r="BG21" s="161"/>
+      <c r="BH21" s="160"/>
+      <c r="BI21" s="160"/>
+      <c r="BJ21" s="160"/>
+      <c r="BK21" s="160"/>
+      <c r="BL21" s="160"/>
+      <c r="BM21" s="160"/>
+      <c r="BN21" s="160"/>
     </row>
     <row r="22" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="F22" s="136"/>
-      <c r="G22" s="136"/>
-      <c r="H22" s="136"/>
-      <c r="I22" s="136"/>
-      <c r="J22" s="136"/>
-      <c r="K22" s="136"/>
-      <c r="L22" s="136"/>
-      <c r="M22" s="136"/>
-      <c r="N22" s="136"/>
-      <c r="O22" s="136"/>
-      <c r="P22" s="136"/>
-      <c r="Q22" s="137"/>
-      <c r="R22" s="137"/>
-      <c r="S22" s="137"/>
-      <c r="T22" s="137"/>
-      <c r="U22" s="137"/>
-      <c r="V22" s="137"/>
-      <c r="W22" s="137"/>
-      <c r="X22" s="137"/>
-      <c r="Y22" s="137"/>
-      <c r="Z22" s="137"/>
-      <c r="AA22" s="137"/>
-      <c r="AB22" s="137"/>
-      <c r="AC22" s="137"/>
-      <c r="AD22" s="137"/>
-      <c r="AE22" s="137"/>
-      <c r="AF22" s="137"/>
-      <c r="AG22" s="137"/>
-      <c r="AH22" s="137"/>
-      <c r="AI22" s="137"/>
-      <c r="AJ22" s="137"/>
-      <c r="AK22" s="137"/>
-      <c r="AL22" s="137"/>
-      <c r="AM22" s="137"/>
-      <c r="AN22" s="137"/>
-      <c r="AO22" s="137"/>
-      <c r="AP22" s="137"/>
-      <c r="AQ22" s="137"/>
-      <c r="AR22" s="137"/>
-      <c r="AS22" s="137"/>
-      <c r="AT22" s="137"/>
-      <c r="AU22" s="137"/>
-      <c r="AV22" s="137"/>
-      <c r="AW22" s="137"/>
-      <c r="AX22" s="137"/>
-      <c r="AY22" s="137"/>
-      <c r="AZ22" s="137"/>
-      <c r="BA22" s="137"/>
-      <c r="BB22" s="137"/>
-      <c r="BC22" s="137"/>
-      <c r="BD22" s="137"/>
-      <c r="BE22" s="137"/>
-      <c r="BF22" s="137"/>
-      <c r="BG22" s="137"/>
-      <c r="BH22" s="137"/>
-      <c r="BI22" s="136"/>
-      <c r="BJ22" s="136"/>
-      <c r="BK22" s="136"/>
-      <c r="BL22" s="136"/>
-      <c r="BM22" s="136"/>
-      <c r="BN22" s="136"/>
+      <c r="F22" s="160"/>
+      <c r="G22" s="160"/>
+      <c r="H22" s="160"/>
+      <c r="I22" s="160"/>
+      <c r="J22" s="160"/>
+      <c r="K22" s="160"/>
+      <c r="L22" s="160"/>
+      <c r="M22" s="160"/>
+      <c r="N22" s="160"/>
+      <c r="O22" s="160"/>
+      <c r="P22" s="160"/>
+      <c r="Q22" s="161"/>
+      <c r="R22" s="161"/>
+      <c r="S22" s="161"/>
+      <c r="T22" s="161"/>
+      <c r="U22" s="161"/>
+      <c r="V22" s="161"/>
+      <c r="W22" s="161"/>
+      <c r="X22" s="161"/>
+      <c r="Y22" s="161"/>
+      <c r="Z22" s="161"/>
+      <c r="AA22" s="161"/>
+      <c r="AB22" s="161"/>
+      <c r="AC22" s="161"/>
+      <c r="AD22" s="161"/>
+      <c r="AE22" s="161"/>
+      <c r="AF22" s="161"/>
+      <c r="AG22" s="161"/>
+      <c r="AH22" s="161"/>
+      <c r="AI22" s="161"/>
+      <c r="AJ22" s="161"/>
+      <c r="AK22" s="161"/>
+      <c r="AL22" s="161"/>
+      <c r="AM22" s="161"/>
+      <c r="AN22" s="161"/>
+      <c r="AO22" s="161"/>
+      <c r="AP22" s="161"/>
+      <c r="AQ22" s="161"/>
+      <c r="AR22" s="161"/>
+      <c r="AS22" s="161"/>
+      <c r="AT22" s="161"/>
+      <c r="AU22" s="161"/>
+      <c r="AV22" s="161"/>
+      <c r="AW22" s="161"/>
+      <c r="AX22" s="161"/>
+      <c r="AY22" s="161"/>
+      <c r="AZ22" s="161"/>
+      <c r="BA22" s="161"/>
+      <c r="BB22" s="161"/>
+      <c r="BC22" s="161"/>
+      <c r="BD22" s="161"/>
+      <c r="BE22" s="161"/>
+      <c r="BF22" s="161"/>
+      <c r="BG22" s="161"/>
+      <c r="BH22" s="161"/>
+      <c r="BI22" s="160"/>
+      <c r="BJ22" s="160"/>
+      <c r="BK22" s="160"/>
+      <c r="BL22" s="160"/>
+      <c r="BM22" s="160"/>
+      <c r="BN22" s="160"/>
     </row>
     <row r="23" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="F23" s="136"/>
-      <c r="G23" s="136"/>
-      <c r="H23" s="136"/>
-      <c r="I23" s="136"/>
-      <c r="J23" s="136"/>
-      <c r="K23" s="136"/>
-      <c r="L23" s="136"/>
-      <c r="M23" s="136"/>
-      <c r="N23" s="136"/>
-      <c r="O23" s="136"/>
-      <c r="P23" s="136"/>
-      <c r="Q23" s="136"/>
-      <c r="R23" s="136"/>
-      <c r="S23" s="136"/>
-      <c r="T23" s="136"/>
-      <c r="U23" s="136"/>
-      <c r="V23" s="136"/>
-      <c r="W23" s="136"/>
-      <c r="X23" s="136"/>
-      <c r="Y23" s="136"/>
-      <c r="Z23" s="136"/>
-      <c r="AA23" s="136"/>
-      <c r="AB23" s="136"/>
-      <c r="AC23" s="136"/>
-      <c r="AD23" s="136"/>
-      <c r="AE23" s="136"/>
-      <c r="AF23" s="136"/>
-      <c r="AG23" s="136"/>
-      <c r="AH23" s="136"/>
-      <c r="AI23" s="136"/>
-      <c r="AJ23" s="136"/>
-      <c r="AK23" s="136"/>
-      <c r="AL23" s="136"/>
-      <c r="AM23" s="136"/>
-      <c r="AN23" s="136"/>
-      <c r="AO23" s="136"/>
-      <c r="AP23" s="136"/>
-      <c r="AQ23" s="136"/>
-      <c r="AR23" s="136"/>
-      <c r="AS23" s="136"/>
-      <c r="AT23" s="136"/>
-      <c r="AU23" s="136"/>
-      <c r="AV23" s="136"/>
-      <c r="AW23" s="136"/>
-      <c r="AX23" s="136"/>
-      <c r="AY23" s="136"/>
-      <c r="AZ23" s="136"/>
-      <c r="BA23" s="136"/>
-      <c r="BB23" s="136"/>
-      <c r="BC23" s="136"/>
-      <c r="BD23" s="136"/>
-      <c r="BE23" s="136"/>
-      <c r="BF23" s="136"/>
-      <c r="BG23" s="136"/>
-      <c r="BH23" s="136"/>
-      <c r="BI23" s="136"/>
-      <c r="BJ23" s="136"/>
-      <c r="BK23" s="136"/>
-      <c r="BL23" s="136"/>
-      <c r="BM23" s="136"/>
-      <c r="BN23" s="136"/>
+      <c r="F23" s="160"/>
+      <c r="G23" s="160"/>
+      <c r="H23" s="160"/>
+      <c r="I23" s="160"/>
+      <c r="J23" s="160"/>
+      <c r="K23" s="160"/>
+      <c r="L23" s="160"/>
+      <c r="M23" s="160"/>
+      <c r="N23" s="160"/>
+      <c r="O23" s="160"/>
+      <c r="P23" s="160"/>
+      <c r="Q23" s="160"/>
+      <c r="R23" s="160"/>
+      <c r="S23" s="160"/>
+      <c r="T23" s="160"/>
+      <c r="U23" s="160"/>
+      <c r="V23" s="160"/>
+      <c r="W23" s="160"/>
+      <c r="X23" s="160"/>
+      <c r="Y23" s="160"/>
+      <c r="Z23" s="160"/>
+      <c r="AA23" s="160"/>
+      <c r="AB23" s="160"/>
+      <c r="AC23" s="160"/>
+      <c r="AD23" s="160"/>
+      <c r="AE23" s="160"/>
+      <c r="AF23" s="160"/>
+      <c r="AG23" s="160"/>
+      <c r="AH23" s="160"/>
+      <c r="AI23" s="160"/>
+      <c r="AJ23" s="160"/>
+      <c r="AK23" s="160"/>
+      <c r="AL23" s="160"/>
+      <c r="AM23" s="160"/>
+      <c r="AN23" s="160"/>
+      <c r="AO23" s="160"/>
+      <c r="AP23" s="160"/>
+      <c r="AQ23" s="160"/>
+      <c r="AR23" s="160"/>
+      <c r="AS23" s="160"/>
+      <c r="AT23" s="160"/>
+      <c r="AU23" s="160"/>
+      <c r="AV23" s="160"/>
+      <c r="AW23" s="160"/>
+      <c r="AX23" s="160"/>
+      <c r="AY23" s="160"/>
+      <c r="AZ23" s="160"/>
+      <c r="BA23" s="160"/>
+      <c r="BB23" s="160"/>
+      <c r="BC23" s="160"/>
+      <c r="BD23" s="160"/>
+      <c r="BE23" s="160"/>
+      <c r="BF23" s="160"/>
+      <c r="BG23" s="160"/>
+      <c r="BH23" s="160"/>
+      <c r="BI23" s="160"/>
+      <c r="BJ23" s="160"/>
+      <c r="BK23" s="160"/>
+      <c r="BL23" s="160"/>
+      <c r="BM23" s="160"/>
+      <c r="BN23" s="160"/>
     </row>
     <row r="24" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="F24" s="136"/>
-      <c r="G24" s="136"/>
-      <c r="H24" s="136"/>
-      <c r="I24" s="136"/>
-      <c r="J24" s="136"/>
-      <c r="K24" s="136"/>
-      <c r="L24" s="136"/>
-      <c r="M24" s="136"/>
-      <c r="N24" s="137"/>
-      <c r="O24" s="137"/>
-      <c r="P24" s="137"/>
-      <c r="Q24" s="137"/>
-      <c r="R24" s="137"/>
-      <c r="S24" s="137"/>
-      <c r="T24" s="137"/>
-      <c r="U24" s="137"/>
-      <c r="V24" s="137"/>
-      <c r="W24" s="137"/>
-      <c r="X24" s="137"/>
-      <c r="Y24" s="137"/>
-      <c r="Z24" s="137"/>
-      <c r="AA24" s="137"/>
-      <c r="AB24" s="137"/>
-      <c r="AC24" s="137"/>
-      <c r="AD24" s="137"/>
-      <c r="AE24" s="137"/>
-      <c r="AF24" s="137"/>
-      <c r="AG24" s="137"/>
-      <c r="AH24" s="137"/>
-      <c r="AI24" s="137"/>
-      <c r="AJ24" s="137"/>
-      <c r="AK24" s="137"/>
-      <c r="AL24" s="137"/>
-      <c r="AM24" s="137"/>
-      <c r="AN24" s="137"/>
-      <c r="AO24" s="137"/>
-      <c r="AP24" s="137"/>
-      <c r="AQ24" s="137"/>
-      <c r="AR24" s="137"/>
-      <c r="AS24" s="137"/>
-      <c r="AT24" s="137"/>
-      <c r="AU24" s="137"/>
-      <c r="AV24" s="137"/>
-      <c r="AW24" s="137"/>
-      <c r="AX24" s="137"/>
-      <c r="AY24" s="137"/>
-      <c r="AZ24" s="137"/>
-      <c r="BA24" s="137"/>
-      <c r="BB24" s="137"/>
-      <c r="BC24" s="137"/>
-      <c r="BD24" s="137"/>
-      <c r="BE24" s="137"/>
-      <c r="BF24" s="137"/>
-      <c r="BG24" s="137"/>
-      <c r="BH24" s="137"/>
-      <c r="BI24" s="136"/>
-      <c r="BJ24" s="136"/>
-      <c r="BK24" s="136"/>
-      <c r="BL24" s="136"/>
-      <c r="BM24" s="136"/>
-      <c r="BN24" s="136"/>
+      <c r="F24" s="160"/>
+      <c r="G24" s="160"/>
+      <c r="H24" s="160"/>
+      <c r="I24" s="160"/>
+      <c r="J24" s="160"/>
+      <c r="K24" s="160"/>
+      <c r="L24" s="160"/>
+      <c r="M24" s="160"/>
+      <c r="N24" s="161"/>
+      <c r="O24" s="161"/>
+      <c r="P24" s="161"/>
+      <c r="Q24" s="161"/>
+      <c r="R24" s="161"/>
+      <c r="S24" s="161"/>
+      <c r="T24" s="161"/>
+      <c r="U24" s="161"/>
+      <c r="V24" s="161"/>
+      <c r="W24" s="161"/>
+      <c r="X24" s="161"/>
+      <c r="Y24" s="161"/>
+      <c r="Z24" s="161"/>
+      <c r="AA24" s="161"/>
+      <c r="AB24" s="161"/>
+      <c r="AC24" s="161"/>
+      <c r="AD24" s="161"/>
+      <c r="AE24" s="161"/>
+      <c r="AF24" s="161"/>
+      <c r="AG24" s="161"/>
+      <c r="AH24" s="161"/>
+      <c r="AI24" s="161"/>
+      <c r="AJ24" s="161"/>
+      <c r="AK24" s="161"/>
+      <c r="AL24" s="161"/>
+      <c r="AM24" s="161"/>
+      <c r="AN24" s="161"/>
+      <c r="AO24" s="161"/>
+      <c r="AP24" s="161"/>
+      <c r="AQ24" s="161"/>
+      <c r="AR24" s="161"/>
+      <c r="AS24" s="161"/>
+      <c r="AT24" s="161"/>
+      <c r="AU24" s="161"/>
+      <c r="AV24" s="161"/>
+      <c r="AW24" s="161"/>
+      <c r="AX24" s="161"/>
+      <c r="AY24" s="161"/>
+      <c r="AZ24" s="161"/>
+      <c r="BA24" s="161"/>
+      <c r="BB24" s="161"/>
+      <c r="BC24" s="161"/>
+      <c r="BD24" s="161"/>
+      <c r="BE24" s="161"/>
+      <c r="BF24" s="161"/>
+      <c r="BG24" s="161"/>
+      <c r="BH24" s="161"/>
+      <c r="BI24" s="160"/>
+      <c r="BJ24" s="160"/>
+      <c r="BK24" s="160"/>
+      <c r="BL24" s="160"/>
+      <c r="BM24" s="160"/>
+      <c r="BN24" s="160"/>
     </row>
     <row r="25" spans="1:66" x14ac:dyDescent="0.25">
       <c r="I25" s="65"/>
@@ -14229,16 +14229,13 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:BA2"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="V3:Y3"/>
-    <mergeCell ref="Z3:AC3"/>
-    <mergeCell ref="AD3:AG3"/>
-    <mergeCell ref="AH3:AK3"/>
+    <mergeCell ref="CH3:CK3"/>
+    <mergeCell ref="CL3:CO3"/>
+    <mergeCell ref="CP3:CS3"/>
+    <mergeCell ref="CT3:CW3"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="BZ3:CC3"/>
+    <mergeCell ref="CD3:CG3"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="BJ3:BM3"/>
     <mergeCell ref="BN3:BQ3"/>
@@ -14250,13 +14247,16 @@
     <mergeCell ref="AX3:BA3"/>
     <mergeCell ref="BB3:BE3"/>
     <mergeCell ref="BF3:BI3"/>
-    <mergeCell ref="CH3:CK3"/>
-    <mergeCell ref="CL3:CO3"/>
-    <mergeCell ref="CP3:CS3"/>
-    <mergeCell ref="CT3:CW3"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="BZ3:CC3"/>
-    <mergeCell ref="CD3:CG3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:BA2"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="V3:Y3"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="AD3:AG3"/>
+    <mergeCell ref="AH3:AK3"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>
@@ -14547,102 +14547,102 @@
       <c r="C4" s="172"/>
       <c r="D4" s="172"/>
       <c r="E4" s="172"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
-      <c r="H4" s="136"/>
-      <c r="I4" s="136"/>
-      <c r="J4" s="136"/>
-      <c r="K4" s="136"/>
-      <c r="L4" s="136"/>
-      <c r="M4" s="136"/>
-      <c r="N4" s="136"/>
-      <c r="O4" s="136"/>
-      <c r="P4" s="136"/>
-      <c r="Q4" s="136"/>
-      <c r="R4" s="136"/>
-      <c r="S4" s="136"/>
-      <c r="T4" s="136"/>
-      <c r="U4" s="136"/>
-      <c r="V4" s="136"/>
-      <c r="W4" s="136"/>
-      <c r="X4" s="136"/>
-      <c r="Y4" s="136"/>
-      <c r="Z4" s="136"/>
-      <c r="AA4" s="136"/>
-      <c r="AB4" s="136"/>
-      <c r="AC4" s="136"/>
-      <c r="AD4" s="136"/>
-      <c r="AE4" s="136"/>
-      <c r="AF4" s="136"/>
-      <c r="AG4" s="136"/>
-      <c r="AH4" s="136"/>
-      <c r="AI4" s="136"/>
-      <c r="AJ4" s="136"/>
-      <c r="AK4" s="136"/>
-      <c r="AL4" s="136"/>
-      <c r="AM4" s="136"/>
-      <c r="AN4" s="136"/>
-      <c r="AO4" s="136"/>
-      <c r="AP4" s="136"/>
-      <c r="AQ4" s="136"/>
-      <c r="AR4" s="136"/>
-      <c r="AS4" s="136"/>
-      <c r="AT4" s="136"/>
-      <c r="AU4" s="136"/>
-      <c r="AV4" s="136"/>
-      <c r="AW4" s="136"/>
-      <c r="AX4" s="136"/>
-      <c r="AY4" s="136"/>
-      <c r="AZ4" s="136"/>
-      <c r="BA4" s="136"/>
-      <c r="BB4" s="136"/>
-      <c r="BC4" s="136"/>
-      <c r="BD4" s="136"/>
-      <c r="BE4" s="136"/>
-      <c r="BF4" s="136"/>
-      <c r="BG4" s="136"/>
-      <c r="BH4" s="136"/>
-      <c r="BI4" s="136"/>
-      <c r="BJ4" s="136"/>
-      <c r="BK4" s="136"/>
-      <c r="BL4" s="136"/>
-      <c r="BM4" s="136"/>
-      <c r="BN4" s="136"/>
-      <c r="BO4" s="136"/>
-      <c r="BP4" s="136"/>
-      <c r="BQ4" s="136"/>
-      <c r="BR4" s="136"/>
-      <c r="BS4" s="136"/>
-      <c r="BT4" s="136"/>
-      <c r="BU4" s="136"/>
-      <c r="BV4" s="136"/>
-      <c r="BW4" s="136"/>
-      <c r="BX4" s="136"/>
-      <c r="BY4" s="136"/>
-      <c r="BZ4" s="136"/>
-      <c r="CA4" s="136"/>
-      <c r="CB4" s="136"/>
-      <c r="CC4" s="136"/>
-      <c r="CD4" s="136"/>
-      <c r="CE4" s="136"/>
-      <c r="CF4" s="136"/>
-      <c r="CG4" s="136"/>
-      <c r="CH4" s="136"/>
-      <c r="CI4" s="136"/>
-      <c r="CJ4" s="136"/>
-      <c r="CK4" s="136"/>
-      <c r="CL4" s="136"/>
-      <c r="CM4" s="136"/>
-      <c r="CN4" s="136"/>
-      <c r="CO4" s="136"/>
-      <c r="CP4" s="136"/>
-      <c r="CQ4" s="136"/>
-      <c r="CR4" s="136"/>
-      <c r="CS4" s="136"/>
-      <c r="CT4" s="136"/>
-      <c r="CU4" s="136"/>
-      <c r="CV4" s="136"/>
-      <c r="CW4" s="136"/>
+      <c r="F4" s="160"/>
+      <c r="G4" s="160"/>
+      <c r="H4" s="160"/>
+      <c r="I4" s="160"/>
+      <c r="J4" s="160"/>
+      <c r="K4" s="160"/>
+      <c r="L4" s="160"/>
+      <c r="M4" s="160"/>
+      <c r="N4" s="160"/>
+      <c r="O4" s="160"/>
+      <c r="P4" s="160"/>
+      <c r="Q4" s="160"/>
+      <c r="R4" s="160"/>
+      <c r="S4" s="160"/>
+      <c r="T4" s="160"/>
+      <c r="U4" s="160"/>
+      <c r="V4" s="160"/>
+      <c r="W4" s="160"/>
+      <c r="X4" s="160"/>
+      <c r="Y4" s="160"/>
+      <c r="Z4" s="160"/>
+      <c r="AA4" s="160"/>
+      <c r="AB4" s="160"/>
+      <c r="AC4" s="160"/>
+      <c r="AD4" s="160"/>
+      <c r="AE4" s="160"/>
+      <c r="AF4" s="160"/>
+      <c r="AG4" s="160"/>
+      <c r="AH4" s="160"/>
+      <c r="AI4" s="160"/>
+      <c r="AJ4" s="160"/>
+      <c r="AK4" s="160"/>
+      <c r="AL4" s="160"/>
+      <c r="AM4" s="160"/>
+      <c r="AN4" s="160"/>
+      <c r="AO4" s="160"/>
+      <c r="AP4" s="160"/>
+      <c r="AQ4" s="160"/>
+      <c r="AR4" s="160"/>
+      <c r="AS4" s="160"/>
+      <c r="AT4" s="160"/>
+      <c r="AU4" s="160"/>
+      <c r="AV4" s="160"/>
+      <c r="AW4" s="160"/>
+      <c r="AX4" s="160"/>
+      <c r="AY4" s="160"/>
+      <c r="AZ4" s="160"/>
+      <c r="BA4" s="160"/>
+      <c r="BB4" s="160"/>
+      <c r="BC4" s="160"/>
+      <c r="BD4" s="160"/>
+      <c r="BE4" s="160"/>
+      <c r="BF4" s="160"/>
+      <c r="BG4" s="160"/>
+      <c r="BH4" s="160"/>
+      <c r="BI4" s="160"/>
+      <c r="BJ4" s="160"/>
+      <c r="BK4" s="160"/>
+      <c r="BL4" s="160"/>
+      <c r="BM4" s="160"/>
+      <c r="BN4" s="160"/>
+      <c r="BO4" s="160"/>
+      <c r="BP4" s="160"/>
+      <c r="BQ4" s="160"/>
+      <c r="BR4" s="160"/>
+      <c r="BS4" s="160"/>
+      <c r="BT4" s="160"/>
+      <c r="BU4" s="160"/>
+      <c r="BV4" s="160"/>
+      <c r="BW4" s="160"/>
+      <c r="BX4" s="160"/>
+      <c r="BY4" s="160"/>
+      <c r="BZ4" s="160"/>
+      <c r="CA4" s="160"/>
+      <c r="CB4" s="160"/>
+      <c r="CC4" s="160"/>
+      <c r="CD4" s="160"/>
+      <c r="CE4" s="160"/>
+      <c r="CF4" s="160"/>
+      <c r="CG4" s="160"/>
+      <c r="CH4" s="160"/>
+      <c r="CI4" s="160"/>
+      <c r="CJ4" s="160"/>
+      <c r="CK4" s="160"/>
+      <c r="CL4" s="160"/>
+      <c r="CM4" s="160"/>
+      <c r="CN4" s="160"/>
+      <c r="CO4" s="160"/>
+      <c r="CP4" s="160"/>
+      <c r="CQ4" s="160"/>
+      <c r="CR4" s="160"/>
+      <c r="CS4" s="160"/>
+      <c r="CT4" s="160"/>
+      <c r="CU4" s="160"/>
+      <c r="CV4" s="160"/>
+      <c r="CW4" s="160"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="172">
@@ -14660,8 +14660,8 @@
       <c r="E5" t="s" s="172">
         <v>94</v>
       </c>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
+      <c r="F5" s="160"/>
+      <c r="G5" s="160"/>
       <c r="H5" s="596"/>
       <c r="I5" s="597"/>
       <c r="J5" s="598"/>
@@ -14728,34 +14728,34 @@
       <c r="BS5" s="626"/>
       <c r="BT5" s="627"/>
       <c r="BU5" s="628"/>
-      <c r="BV5" s="136"/>
-      <c r="BW5" s="136"/>
-      <c r="BX5" s="136"/>
-      <c r="BY5" s="136"/>
-      <c r="BZ5" s="136"/>
-      <c r="CA5" s="136"/>
-      <c r="CB5" s="136"/>
-      <c r="CC5" s="136"/>
-      <c r="CD5" s="136"/>
-      <c r="CE5" s="136"/>
-      <c r="CF5" s="136"/>
-      <c r="CG5" s="136"/>
-      <c r="CH5" s="136"/>
-      <c r="CI5" s="136"/>
-      <c r="CJ5" s="136"/>
-      <c r="CK5" s="136"/>
-      <c r="CL5" s="136"/>
-      <c r="CM5" s="136"/>
-      <c r="CN5" s="136"/>
-      <c r="CO5" s="136"/>
-      <c r="CP5" s="136"/>
-      <c r="CQ5" s="136"/>
-      <c r="CR5" s="136"/>
-      <c r="CS5" s="136"/>
-      <c r="CT5" s="136"/>
-      <c r="CU5" s="136"/>
-      <c r="CV5" s="136"/>
-      <c r="CW5" s="136"/>
+      <c r="BV5" s="160"/>
+      <c r="BW5" s="160"/>
+      <c r="BX5" s="160"/>
+      <c r="BY5" s="160"/>
+      <c r="BZ5" s="160"/>
+      <c r="CA5" s="160"/>
+      <c r="CB5" s="160"/>
+      <c r="CC5" s="160"/>
+      <c r="CD5" s="160"/>
+      <c r="CE5" s="160"/>
+      <c r="CF5" s="160"/>
+      <c r="CG5" s="160"/>
+      <c r="CH5" s="160"/>
+      <c r="CI5" s="160"/>
+      <c r="CJ5" s="160"/>
+      <c r="CK5" s="160"/>
+      <c r="CL5" s="160"/>
+      <c r="CM5" s="160"/>
+      <c r="CN5" s="160"/>
+      <c r="CO5" s="160"/>
+      <c r="CP5" s="160"/>
+      <c r="CQ5" s="160"/>
+      <c r="CR5" s="160"/>
+      <c r="CS5" s="160"/>
+      <c r="CT5" s="160"/>
+      <c r="CU5" s="160"/>
+      <c r="CV5" s="160"/>
+      <c r="CW5" s="160"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="172">
@@ -14773,9 +14773,9 @@
       <c r="E6" t="s" s="172">
         <v>94</v>
       </c>
-      <c r="F6" s="136"/>
-      <c r="G6" s="136"/>
-      <c r="H6" s="136"/>
+      <c r="F6" s="160"/>
+      <c r="G6" s="160"/>
+      <c r="H6" s="160"/>
       <c r="I6" s="629"/>
       <c r="J6" s="630"/>
       <c r="K6" s="631"/>
@@ -14841,34 +14841,34 @@
       <c r="BS6" s="661"/>
       <c r="BT6" s="662"/>
       <c r="BU6" s="663"/>
-      <c r="BV6" s="136"/>
-      <c r="BW6" s="136"/>
-      <c r="BX6" s="136"/>
-      <c r="BY6" s="136"/>
-      <c r="BZ6" s="136"/>
-      <c r="CA6" s="136"/>
-      <c r="CB6" s="136"/>
-      <c r="CC6" s="136"/>
-      <c r="CD6" s="136"/>
-      <c r="CE6" s="136"/>
-      <c r="CF6" s="136"/>
-      <c r="CG6" s="136"/>
-      <c r="CH6" s="136"/>
-      <c r="CI6" s="136"/>
-      <c r="CJ6" s="136"/>
-      <c r="CK6" s="136"/>
-      <c r="CL6" s="136"/>
-      <c r="CM6" s="136"/>
-      <c r="CN6" s="136"/>
-      <c r="CO6" s="136"/>
-      <c r="CP6" s="136"/>
-      <c r="CQ6" s="136"/>
-      <c r="CR6" s="136"/>
-      <c r="CS6" s="136"/>
-      <c r="CT6" s="136"/>
-      <c r="CU6" s="136"/>
-      <c r="CV6" s="136"/>
-      <c r="CW6" s="136"/>
+      <c r="BV6" s="160"/>
+      <c r="BW6" s="160"/>
+      <c r="BX6" s="160"/>
+      <c r="BY6" s="160"/>
+      <c r="BZ6" s="160"/>
+      <c r="CA6" s="160"/>
+      <c r="CB6" s="160"/>
+      <c r="CC6" s="160"/>
+      <c r="CD6" s="160"/>
+      <c r="CE6" s="160"/>
+      <c r="CF6" s="160"/>
+      <c r="CG6" s="160"/>
+      <c r="CH6" s="160"/>
+      <c r="CI6" s="160"/>
+      <c r="CJ6" s="160"/>
+      <c r="CK6" s="160"/>
+      <c r="CL6" s="160"/>
+      <c r="CM6" s="160"/>
+      <c r="CN6" s="160"/>
+      <c r="CO6" s="160"/>
+      <c r="CP6" s="160"/>
+      <c r="CQ6" s="160"/>
+      <c r="CR6" s="160"/>
+      <c r="CS6" s="160"/>
+      <c r="CT6" s="160"/>
+      <c r="CU6" s="160"/>
+      <c r="CV6" s="160"/>
+      <c r="CW6" s="160"/>
     </row>
     <row r="7">
       <c r="A7" t="s" s="172">
@@ -14886,13 +14886,13 @@
       <c r="E7" t="s" s="172">
         <v>49</v>
       </c>
-      <c r="F7" s="136"/>
-      <c r="G7" s="136"/>
-      <c r="H7" s="136"/>
-      <c r="I7" s="136"/>
-      <c r="J7" s="136"/>
-      <c r="K7" s="136"/>
-      <c r="L7" s="136"/>
+      <c r="F7" s="160"/>
+      <c r="G7" s="160"/>
+      <c r="H7" s="160"/>
+      <c r="I7" s="160"/>
+      <c r="J7" s="160"/>
+      <c r="K7" s="160"/>
+      <c r="L7" s="160"/>
       <c r="M7" s="259"/>
       <c r="N7" s="260"/>
       <c r="O7" s="261"/>
@@ -14954,34 +14954,34 @@
       <c r="BS7" s="691"/>
       <c r="BT7" s="692"/>
       <c r="BU7" s="693"/>
-      <c r="BV7" s="136"/>
-      <c r="BW7" s="136"/>
-      <c r="BX7" s="136"/>
-      <c r="BY7" s="136"/>
-      <c r="BZ7" s="136"/>
-      <c r="CA7" s="136"/>
-      <c r="CB7" s="136"/>
-      <c r="CC7" s="136"/>
-      <c r="CD7" s="136"/>
-      <c r="CE7" s="136"/>
-      <c r="CF7" s="136"/>
-      <c r="CG7" s="136"/>
-      <c r="CH7" s="136"/>
-      <c r="CI7" s="136"/>
-      <c r="CJ7" s="136"/>
-      <c r="CK7" s="136"/>
-      <c r="CL7" s="136"/>
-      <c r="CM7" s="136"/>
-      <c r="CN7" s="136"/>
-      <c r="CO7" s="136"/>
-      <c r="CP7" s="136"/>
-      <c r="CQ7" s="136"/>
-      <c r="CR7" s="136"/>
-      <c r="CS7" s="136"/>
-      <c r="CT7" s="136"/>
-      <c r="CU7" s="136"/>
-      <c r="CV7" s="136"/>
-      <c r="CW7" s="136"/>
+      <c r="BV7" s="160"/>
+      <c r="BW7" s="160"/>
+      <c r="BX7" s="160"/>
+      <c r="BY7" s="160"/>
+      <c r="BZ7" s="160"/>
+      <c r="CA7" s="160"/>
+      <c r="CB7" s="160"/>
+      <c r="CC7" s="160"/>
+      <c r="CD7" s="160"/>
+      <c r="CE7" s="160"/>
+      <c r="CF7" s="160"/>
+      <c r="CG7" s="160"/>
+      <c r="CH7" s="160"/>
+      <c r="CI7" s="160"/>
+      <c r="CJ7" s="160"/>
+      <c r="CK7" s="160"/>
+      <c r="CL7" s="160"/>
+      <c r="CM7" s="160"/>
+      <c r="CN7" s="160"/>
+      <c r="CO7" s="160"/>
+      <c r="CP7" s="160"/>
+      <c r="CQ7" s="160"/>
+      <c r="CR7" s="160"/>
+      <c r="CS7" s="160"/>
+      <c r="CT7" s="160"/>
+      <c r="CU7" s="160"/>
+      <c r="CV7" s="160"/>
+      <c r="CW7" s="160"/>
     </row>
     <row r="8">
       <c r="A8" t="s" s="172">
@@ -14999,12 +14999,12 @@
       <c r="E8" t="s" s="172">
         <v>50</v>
       </c>
-      <c r="F8" s="136"/>
-      <c r="G8" s="136"/>
-      <c r="H8" s="136"/>
-      <c r="I8" s="136"/>
-      <c r="J8" s="136"/>
-      <c r="K8" s="136"/>
+      <c r="F8" s="160"/>
+      <c r="G8" s="160"/>
+      <c r="H8" s="160"/>
+      <c r="I8" s="160"/>
+      <c r="J8" s="160"/>
+      <c r="K8" s="160"/>
       <c r="L8" s="694"/>
       <c r="M8" s="305"/>
       <c r="N8" s="306"/>
@@ -15067,34 +15067,34 @@
       <c r="BS8" s="713"/>
       <c r="BT8" s="714"/>
       <c r="BU8" s="715"/>
-      <c r="BV8" s="136"/>
-      <c r="BW8" s="136"/>
-      <c r="BX8" s="136"/>
-      <c r="BY8" s="136"/>
-      <c r="BZ8" s="136"/>
-      <c r="CA8" s="136"/>
-      <c r="CB8" s="136"/>
-      <c r="CC8" s="136"/>
-      <c r="CD8" s="136"/>
-      <c r="CE8" s="136"/>
-      <c r="CF8" s="136"/>
-      <c r="CG8" s="136"/>
-      <c r="CH8" s="136"/>
-      <c r="CI8" s="136"/>
-      <c r="CJ8" s="136"/>
-      <c r="CK8" s="136"/>
-      <c r="CL8" s="136"/>
-      <c r="CM8" s="136"/>
-      <c r="CN8" s="136"/>
-      <c r="CO8" s="136"/>
-      <c r="CP8" s="136"/>
-      <c r="CQ8" s="136"/>
-      <c r="CR8" s="136"/>
-      <c r="CS8" s="136"/>
-      <c r="CT8" s="136"/>
-      <c r="CU8" s="136"/>
-      <c r="CV8" s="136"/>
-      <c r="CW8" s="136"/>
+      <c r="BV8" s="160"/>
+      <c r="BW8" s="160"/>
+      <c r="BX8" s="160"/>
+      <c r="BY8" s="160"/>
+      <c r="BZ8" s="160"/>
+      <c r="CA8" s="160"/>
+      <c r="CB8" s="160"/>
+      <c r="CC8" s="160"/>
+      <c r="CD8" s="160"/>
+      <c r="CE8" s="160"/>
+      <c r="CF8" s="160"/>
+      <c r="CG8" s="160"/>
+      <c r="CH8" s="160"/>
+      <c r="CI8" s="160"/>
+      <c r="CJ8" s="160"/>
+      <c r="CK8" s="160"/>
+      <c r="CL8" s="160"/>
+      <c r="CM8" s="160"/>
+      <c r="CN8" s="160"/>
+      <c r="CO8" s="160"/>
+      <c r="CP8" s="160"/>
+      <c r="CQ8" s="160"/>
+      <c r="CR8" s="160"/>
+      <c r="CS8" s="160"/>
+      <c r="CT8" s="160"/>
+      <c r="CU8" s="160"/>
+      <c r="CV8" s="160"/>
+      <c r="CW8" s="160"/>
     </row>
     <row r="9">
       <c r="A9" t="s" s="172">
@@ -15112,10 +15112,10 @@
       <c r="E9" t="s" s="172">
         <v>51</v>
       </c>
-      <c r="F9" s="136"/>
-      <c r="G9" s="136"/>
-      <c r="H9" s="136"/>
-      <c r="I9" s="136"/>
+      <c r="F9" s="160"/>
+      <c r="G9" s="160"/>
+      <c r="H9" s="160"/>
+      <c r="I9" s="160"/>
       <c r="J9" s="716"/>
       <c r="K9" s="717"/>
       <c r="L9" s="718"/>
@@ -15160,8 +15160,8 @@
       <c r="AY9" s="388"/>
       <c r="AZ9" s="389"/>
       <c r="BA9" s="390"/>
-      <c r="BB9" s="136"/>
-      <c r="BC9" s="136"/>
+      <c r="BB9" s="160"/>
+      <c r="BC9" s="160"/>
       <c r="BD9" s="729"/>
       <c r="BE9" s="730"/>
       <c r="BF9" s="731"/>
@@ -15180,34 +15180,34 @@
       <c r="BS9" s="744"/>
       <c r="BT9" s="745"/>
       <c r="BU9" s="746"/>
-      <c r="BV9" s="136"/>
-      <c r="BW9" s="136"/>
-      <c r="BX9" s="136"/>
-      <c r="BY9" s="136"/>
-      <c r="BZ9" s="136"/>
-      <c r="CA9" s="136"/>
-      <c r="CB9" s="136"/>
-      <c r="CC9" s="136"/>
-      <c r="CD9" s="136"/>
-      <c r="CE9" s="136"/>
-      <c r="CF9" s="136"/>
-      <c r="CG9" s="136"/>
-      <c r="CH9" s="136"/>
-      <c r="CI9" s="136"/>
-      <c r="CJ9" s="136"/>
-      <c r="CK9" s="136"/>
-      <c r="CL9" s="136"/>
-      <c r="CM9" s="136"/>
-      <c r="CN9" s="136"/>
-      <c r="CO9" s="136"/>
-      <c r="CP9" s="136"/>
-      <c r="CQ9" s="136"/>
-      <c r="CR9" s="136"/>
-      <c r="CS9" s="136"/>
-      <c r="CT9" s="136"/>
-      <c r="CU9" s="136"/>
-      <c r="CV9" s="136"/>
-      <c r="CW9" s="136"/>
+      <c r="BV9" s="160"/>
+      <c r="BW9" s="160"/>
+      <c r="BX9" s="160"/>
+      <c r="BY9" s="160"/>
+      <c r="BZ9" s="160"/>
+      <c r="CA9" s="160"/>
+      <c r="CB9" s="160"/>
+      <c r="CC9" s="160"/>
+      <c r="CD9" s="160"/>
+      <c r="CE9" s="160"/>
+      <c r="CF9" s="160"/>
+      <c r="CG9" s="160"/>
+      <c r="CH9" s="160"/>
+      <c r="CI9" s="160"/>
+      <c r="CJ9" s="160"/>
+      <c r="CK9" s="160"/>
+      <c r="CL9" s="160"/>
+      <c r="CM9" s="160"/>
+      <c r="CN9" s="160"/>
+      <c r="CO9" s="160"/>
+      <c r="CP9" s="160"/>
+      <c r="CQ9" s="160"/>
+      <c r="CR9" s="160"/>
+      <c r="CS9" s="160"/>
+      <c r="CT9" s="160"/>
+      <c r="CU9" s="160"/>
+      <c r="CV9" s="160"/>
+      <c r="CW9" s="160"/>
     </row>
     <row r="10">
       <c r="A10" t="s" s="172">
@@ -15225,9 +15225,9 @@
       <c r="E10" t="s" s="172">
         <v>52</v>
       </c>
-      <c r="F10" s="136"/>
-      <c r="G10" s="136"/>
-      <c r="H10" s="136"/>
+      <c r="F10" s="160"/>
+      <c r="G10" s="160"/>
+      <c r="H10" s="160"/>
       <c r="I10" s="747"/>
       <c r="J10" s="748"/>
       <c r="K10" s="391"/>
@@ -15293,34 +15293,34 @@
       <c r="BS10" s="767"/>
       <c r="BT10" s="768"/>
       <c r="BU10" s="769"/>
-      <c r="BV10" s="136"/>
-      <c r="BW10" s="136"/>
-      <c r="BX10" s="136"/>
-      <c r="BY10" s="136"/>
-      <c r="BZ10" s="136"/>
-      <c r="CA10" s="136"/>
-      <c r="CB10" s="136"/>
-      <c r="CC10" s="136"/>
-      <c r="CD10" s="136"/>
-      <c r="CE10" s="136"/>
-      <c r="CF10" s="136"/>
-      <c r="CG10" s="136"/>
-      <c r="CH10" s="136"/>
-      <c r="CI10" s="136"/>
-      <c r="CJ10" s="136"/>
-      <c r="CK10" s="136"/>
-      <c r="CL10" s="136"/>
-      <c r="CM10" s="136"/>
-      <c r="CN10" s="136"/>
-      <c r="CO10" s="136"/>
-      <c r="CP10" s="136"/>
-      <c r="CQ10" s="136"/>
-      <c r="CR10" s="136"/>
-      <c r="CS10" s="136"/>
-      <c r="CT10" s="136"/>
-      <c r="CU10" s="136"/>
-      <c r="CV10" s="136"/>
-      <c r="CW10" s="136"/>
+      <c r="BV10" s="160"/>
+      <c r="BW10" s="160"/>
+      <c r="BX10" s="160"/>
+      <c r="BY10" s="160"/>
+      <c r="BZ10" s="160"/>
+      <c r="CA10" s="160"/>
+      <c r="CB10" s="160"/>
+      <c r="CC10" s="160"/>
+      <c r="CD10" s="160"/>
+      <c r="CE10" s="160"/>
+      <c r="CF10" s="160"/>
+      <c r="CG10" s="160"/>
+      <c r="CH10" s="160"/>
+      <c r="CI10" s="160"/>
+      <c r="CJ10" s="160"/>
+      <c r="CK10" s="160"/>
+      <c r="CL10" s="160"/>
+      <c r="CM10" s="160"/>
+      <c r="CN10" s="160"/>
+      <c r="CO10" s="160"/>
+      <c r="CP10" s="160"/>
+      <c r="CQ10" s="160"/>
+      <c r="CR10" s="160"/>
+      <c r="CS10" s="160"/>
+      <c r="CT10" s="160"/>
+      <c r="CU10" s="160"/>
+      <c r="CV10" s="160"/>
+      <c r="CW10" s="160"/>
     </row>
     <row r="11">
       <c r="A11" t="s" s="172">
@@ -15338,16 +15338,16 @@
       <c r="E11" t="s" s="172">
         <v>53</v>
       </c>
-      <c r="F11" s="136"/>
-      <c r="G11" s="136"/>
-      <c r="H11" s="136"/>
-      <c r="I11" s="136"/>
-      <c r="J11" s="136"/>
-      <c r="K11" s="136"/>
-      <c r="L11" s="136"/>
-      <c r="M11" s="136"/>
-      <c r="N11" s="136"/>
-      <c r="O11" s="136"/>
+      <c r="F11" s="160"/>
+      <c r="G11" s="160"/>
+      <c r="H11" s="160"/>
+      <c r="I11" s="160"/>
+      <c r="J11" s="160"/>
+      <c r="K11" s="160"/>
+      <c r="L11" s="160"/>
+      <c r="M11" s="160"/>
+      <c r="N11" s="160"/>
+      <c r="O11" s="160"/>
       <c r="P11" s="438"/>
       <c r="Q11" s="439"/>
       <c r="R11" s="440"/>
@@ -15406,34 +15406,34 @@
       <c r="BS11" s="788"/>
       <c r="BT11" s="789"/>
       <c r="BU11" s="790"/>
-      <c r="BV11" s="136"/>
-      <c r="BW11" s="136"/>
-      <c r="BX11" s="136"/>
-      <c r="BY11" s="136"/>
-      <c r="BZ11" s="136"/>
-      <c r="CA11" s="136"/>
-      <c r="CB11" s="136"/>
-      <c r="CC11" s="136"/>
-      <c r="CD11" s="136"/>
-      <c r="CE11" s="136"/>
-      <c r="CF11" s="136"/>
-      <c r="CG11" s="136"/>
-      <c r="CH11" s="136"/>
-      <c r="CI11" s="136"/>
-      <c r="CJ11" s="136"/>
-      <c r="CK11" s="136"/>
-      <c r="CL11" s="136"/>
-      <c r="CM11" s="136"/>
-      <c r="CN11" s="136"/>
-      <c r="CO11" s="136"/>
-      <c r="CP11" s="136"/>
-      <c r="CQ11" s="136"/>
-      <c r="CR11" s="136"/>
-      <c r="CS11" s="136"/>
-      <c r="CT11" s="136"/>
-      <c r="CU11" s="136"/>
-      <c r="CV11" s="136"/>
-      <c r="CW11" s="136"/>
+      <c r="BV11" s="160"/>
+      <c r="BW11" s="160"/>
+      <c r="BX11" s="160"/>
+      <c r="BY11" s="160"/>
+      <c r="BZ11" s="160"/>
+      <c r="CA11" s="160"/>
+      <c r="CB11" s="160"/>
+      <c r="CC11" s="160"/>
+      <c r="CD11" s="160"/>
+      <c r="CE11" s="160"/>
+      <c r="CF11" s="160"/>
+      <c r="CG11" s="160"/>
+      <c r="CH11" s="160"/>
+      <c r="CI11" s="160"/>
+      <c r="CJ11" s="160"/>
+      <c r="CK11" s="160"/>
+      <c r="CL11" s="160"/>
+      <c r="CM11" s="160"/>
+      <c r="CN11" s="160"/>
+      <c r="CO11" s="160"/>
+      <c r="CP11" s="160"/>
+      <c r="CQ11" s="160"/>
+      <c r="CR11" s="160"/>
+      <c r="CS11" s="160"/>
+      <c r="CT11" s="160"/>
+      <c r="CU11" s="160"/>
+      <c r="CV11" s="160"/>
+      <c r="CW11" s="160"/>
     </row>
     <row r="12">
       <c r="A12" t="s" s="172">
@@ -15451,8 +15451,8 @@
       <c r="E12" t="s" s="172">
         <v>54</v>
       </c>
-      <c r="F12" s="136"/>
-      <c r="G12" s="136"/>
+      <c r="F12" s="160"/>
+      <c r="G12" s="160"/>
       <c r="H12" s="791"/>
       <c r="I12" s="792"/>
       <c r="J12" s="793"/>
@@ -15489,7 +15489,7 @@
       <c r="AO12" s="507"/>
       <c r="AP12" s="508"/>
       <c r="AQ12" s="509"/>
-      <c r="AR12" s="136"/>
+      <c r="AR12" s="160"/>
       <c r="AS12" s="804"/>
       <c r="AT12" s="805"/>
       <c r="AU12" s="806"/>
@@ -15519,34 +15519,34 @@
       <c r="BS12" s="830"/>
       <c r="BT12" s="831"/>
       <c r="BU12" s="832"/>
-      <c r="BV12" s="136"/>
-      <c r="BW12" s="136"/>
-      <c r="BX12" s="136"/>
-      <c r="BY12" s="136"/>
-      <c r="BZ12" s="136"/>
-      <c r="CA12" s="136"/>
-      <c r="CB12" s="136"/>
-      <c r="CC12" s="136"/>
-      <c r="CD12" s="136"/>
-      <c r="CE12" s="136"/>
-      <c r="CF12" s="136"/>
-      <c r="CG12" s="136"/>
-      <c r="CH12" s="136"/>
-      <c r="CI12" s="136"/>
-      <c r="CJ12" s="136"/>
-      <c r="CK12" s="136"/>
-      <c r="CL12" s="136"/>
-      <c r="CM12" s="136"/>
-      <c r="CN12" s="136"/>
-      <c r="CO12" s="136"/>
-      <c r="CP12" s="136"/>
-      <c r="CQ12" s="136"/>
-      <c r="CR12" s="136"/>
-      <c r="CS12" s="136"/>
-      <c r="CT12" s="136"/>
-      <c r="CU12" s="136"/>
-      <c r="CV12" s="136"/>
-      <c r="CW12" s="136"/>
+      <c r="BV12" s="160"/>
+      <c r="BW12" s="160"/>
+      <c r="BX12" s="160"/>
+      <c r="BY12" s="160"/>
+      <c r="BZ12" s="160"/>
+      <c r="CA12" s="160"/>
+      <c r="CB12" s="160"/>
+      <c r="CC12" s="160"/>
+      <c r="CD12" s="160"/>
+      <c r="CE12" s="160"/>
+      <c r="CF12" s="160"/>
+      <c r="CG12" s="160"/>
+      <c r="CH12" s="160"/>
+      <c r="CI12" s="160"/>
+      <c r="CJ12" s="160"/>
+      <c r="CK12" s="160"/>
+      <c r="CL12" s="160"/>
+      <c r="CM12" s="160"/>
+      <c r="CN12" s="160"/>
+      <c r="CO12" s="160"/>
+      <c r="CP12" s="160"/>
+      <c r="CQ12" s="160"/>
+      <c r="CR12" s="160"/>
+      <c r="CS12" s="160"/>
+      <c r="CT12" s="160"/>
+      <c r="CU12" s="160"/>
+      <c r="CV12" s="160"/>
+      <c r="CW12" s="160"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="172">
@@ -15564,18 +15564,18 @@
       <c r="E13" t="s" s="172">
         <v>86</v>
       </c>
-      <c r="F13" s="136"/>
-      <c r="G13" s="136"/>
+      <c r="F13" s="160"/>
+      <c r="G13" s="160"/>
       <c r="H13" s="833"/>
       <c r="I13" s="834"/>
       <c r="J13" s="835"/>
       <c r="K13" s="836"/>
-      <c r="L13" s="136"/>
-      <c r="M13" s="136"/>
-      <c r="N13" s="136"/>
-      <c r="O13" s="136"/>
-      <c r="P13" s="136"/>
-      <c r="Q13" s="136"/>
+      <c r="L13" s="160"/>
+      <c r="M13" s="160"/>
+      <c r="N13" s="160"/>
+      <c r="O13" s="160"/>
+      <c r="P13" s="160"/>
+      <c r="Q13" s="160"/>
       <c r="R13" s="510"/>
       <c r="S13" s="511"/>
       <c r="T13" s="512"/>
@@ -15632,34 +15632,34 @@
       <c r="BS13" s="858"/>
       <c r="BT13" s="859"/>
       <c r="BU13" s="860"/>
-      <c r="BV13" s="136"/>
-      <c r="BW13" s="136"/>
-      <c r="BX13" s="136"/>
-      <c r="BY13" s="136"/>
-      <c r="BZ13" s="136"/>
-      <c r="CA13" s="136"/>
-      <c r="CB13" s="136"/>
-      <c r="CC13" s="136"/>
-      <c r="CD13" s="136"/>
-      <c r="CE13" s="136"/>
-      <c r="CF13" s="136"/>
-      <c r="CG13" s="136"/>
-      <c r="CH13" s="136"/>
-      <c r="CI13" s="136"/>
-      <c r="CJ13" s="136"/>
-      <c r="CK13" s="136"/>
-      <c r="CL13" s="136"/>
-      <c r="CM13" s="136"/>
-      <c r="CN13" s="136"/>
-      <c r="CO13" s="136"/>
-      <c r="CP13" s="136"/>
-      <c r="CQ13" s="136"/>
-      <c r="CR13" s="136"/>
-      <c r="CS13" s="136"/>
-      <c r="CT13" s="136"/>
-      <c r="CU13" s="136"/>
-      <c r="CV13" s="136"/>
-      <c r="CW13" s="136"/>
+      <c r="BV13" s="160"/>
+      <c r="BW13" s="160"/>
+      <c r="BX13" s="160"/>
+      <c r="BY13" s="160"/>
+      <c r="BZ13" s="160"/>
+      <c r="CA13" s="160"/>
+      <c r="CB13" s="160"/>
+      <c r="CC13" s="160"/>
+      <c r="CD13" s="160"/>
+      <c r="CE13" s="160"/>
+      <c r="CF13" s="160"/>
+      <c r="CG13" s="160"/>
+      <c r="CH13" s="160"/>
+      <c r="CI13" s="160"/>
+      <c r="CJ13" s="160"/>
+      <c r="CK13" s="160"/>
+      <c r="CL13" s="160"/>
+      <c r="CM13" s="160"/>
+      <c r="CN13" s="160"/>
+      <c r="CO13" s="160"/>
+      <c r="CP13" s="160"/>
+      <c r="CQ13" s="160"/>
+      <c r="CR13" s="160"/>
+      <c r="CS13" s="160"/>
+      <c r="CT13" s="160"/>
+      <c r="CU13" s="160"/>
+      <c r="CV13" s="160"/>
+      <c r="CW13" s="160"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="172">
@@ -15678,101 +15678,101 @@
         <v>55</v>
       </c>
       <c r="F14" s="549"/>
-      <c r="G14" s="136"/>
-      <c r="H14" s="136"/>
-      <c r="I14" s="136"/>
-      <c r="J14" s="136"/>
-      <c r="K14" s="136"/>
-      <c r="L14" s="136"/>
-      <c r="M14" s="136"/>
-      <c r="N14" s="136"/>
-      <c r="O14" s="136"/>
-      <c r="P14" s="136"/>
-      <c r="Q14" s="136"/>
-      <c r="R14" s="136"/>
-      <c r="S14" s="136"/>
-      <c r="T14" s="136"/>
-      <c r="U14" s="136"/>
-      <c r="V14" s="136"/>
-      <c r="W14" s="136"/>
-      <c r="X14" s="136"/>
-      <c r="Y14" s="136"/>
-      <c r="Z14" s="136"/>
-      <c r="AA14" s="136"/>
-      <c r="AB14" s="136"/>
-      <c r="AC14" s="136"/>
-      <c r="AD14" s="136"/>
-      <c r="AE14" s="136"/>
-      <c r="AF14" s="136"/>
-      <c r="AG14" s="136"/>
-      <c r="AH14" s="136"/>
-      <c r="AI14" s="136"/>
-      <c r="AJ14" s="136"/>
-      <c r="AK14" s="136"/>
-      <c r="AL14" s="136"/>
-      <c r="AM14" s="136"/>
-      <c r="AN14" s="136"/>
-      <c r="AO14" s="136"/>
-      <c r="AP14" s="136"/>
-      <c r="AQ14" s="136"/>
-      <c r="AR14" s="136"/>
-      <c r="AS14" s="136"/>
-      <c r="AT14" s="136"/>
-      <c r="AU14" s="136"/>
-      <c r="AV14" s="136"/>
-      <c r="AW14" s="136"/>
-      <c r="AX14" s="136"/>
-      <c r="AY14" s="136"/>
-      <c r="AZ14" s="136"/>
-      <c r="BA14" s="136"/>
-      <c r="BB14" s="136"/>
-      <c r="BC14" s="136"/>
-      <c r="BD14" s="136"/>
-      <c r="BE14" s="136"/>
-      <c r="BF14" s="136"/>
-      <c r="BG14" s="136"/>
-      <c r="BH14" s="136"/>
-      <c r="BI14" s="136"/>
-      <c r="BJ14" s="136"/>
-      <c r="BK14" s="136"/>
-      <c r="BL14" s="136"/>
-      <c r="BM14" s="136"/>
-      <c r="BN14" s="136"/>
-      <c r="BO14" s="136"/>
-      <c r="BP14" s="136"/>
-      <c r="BQ14" s="136"/>
-      <c r="BR14" s="136"/>
-      <c r="BS14" s="136"/>
-      <c r="BT14" s="136"/>
-      <c r="BU14" s="136"/>
-      <c r="BV14" s="136"/>
-      <c r="BW14" s="136"/>
-      <c r="BX14" s="136"/>
-      <c r="BY14" s="136"/>
-      <c r="BZ14" s="136"/>
-      <c r="CA14" s="136"/>
-      <c r="CB14" s="136"/>
-      <c r="CC14" s="136"/>
-      <c r="CD14" s="136"/>
-      <c r="CE14" s="136"/>
-      <c r="CF14" s="136"/>
-      <c r="CG14" s="136"/>
-      <c r="CH14" s="136"/>
-      <c r="CI14" s="136"/>
-      <c r="CJ14" s="136"/>
-      <c r="CK14" s="136"/>
-      <c r="CL14" s="136"/>
-      <c r="CM14" s="136"/>
-      <c r="CN14" s="136"/>
-      <c r="CO14" s="136"/>
-      <c r="CP14" s="136"/>
-      <c r="CQ14" s="136"/>
-      <c r="CR14" s="136"/>
-      <c r="CS14" s="136"/>
-      <c r="CT14" s="136"/>
-      <c r="CU14" s="136"/>
-      <c r="CV14" s="136"/>
-      <c r="CW14" s="136"/>
+      <c r="G14" s="160"/>
+      <c r="H14" s="160"/>
+      <c r="I14" s="160"/>
+      <c r="J14" s="160"/>
+      <c r="K14" s="160"/>
+      <c r="L14" s="160"/>
+      <c r="M14" s="160"/>
+      <c r="N14" s="160"/>
+      <c r="O14" s="160"/>
+      <c r="P14" s="160"/>
+      <c r="Q14" s="160"/>
+      <c r="R14" s="160"/>
+      <c r="S14" s="160"/>
+      <c r="T14" s="160"/>
+      <c r="U14" s="160"/>
+      <c r="V14" s="160"/>
+      <c r="W14" s="160"/>
+      <c r="X14" s="160"/>
+      <c r="Y14" s="160"/>
+      <c r="Z14" s="160"/>
+      <c r="AA14" s="160"/>
+      <c r="AB14" s="160"/>
+      <c r="AC14" s="160"/>
+      <c r="AD14" s="160"/>
+      <c r="AE14" s="160"/>
+      <c r="AF14" s="160"/>
+      <c r="AG14" s="160"/>
+      <c r="AH14" s="160"/>
+      <c r="AI14" s="160"/>
+      <c r="AJ14" s="160"/>
+      <c r="AK14" s="160"/>
+      <c r="AL14" s="160"/>
+      <c r="AM14" s="160"/>
+      <c r="AN14" s="160"/>
+      <c r="AO14" s="160"/>
+      <c r="AP14" s="160"/>
+      <c r="AQ14" s="160"/>
+      <c r="AR14" s="160"/>
+      <c r="AS14" s="160"/>
+      <c r="AT14" s="160"/>
+      <c r="AU14" s="160"/>
+      <c r="AV14" s="160"/>
+      <c r="AW14" s="160"/>
+      <c r="AX14" s="160"/>
+      <c r="AY14" s="160"/>
+      <c r="AZ14" s="160"/>
+      <c r="BA14" s="160"/>
+      <c r="BB14" s="160"/>
+      <c r="BC14" s="160"/>
+      <c r="BD14" s="160"/>
+      <c r="BE14" s="160"/>
+      <c r="BF14" s="160"/>
+      <c r="BG14" s="160"/>
+      <c r="BH14" s="160"/>
+      <c r="BI14" s="160"/>
+      <c r="BJ14" s="160"/>
+      <c r="BK14" s="160"/>
+      <c r="BL14" s="160"/>
+      <c r="BM14" s="160"/>
+      <c r="BN14" s="160"/>
+      <c r="BO14" s="160"/>
+      <c r="BP14" s="160"/>
+      <c r="BQ14" s="160"/>
+      <c r="BR14" s="160"/>
+      <c r="BS14" s="160"/>
+      <c r="BT14" s="160"/>
+      <c r="BU14" s="160"/>
+      <c r="BV14" s="160"/>
+      <c r="BW14" s="160"/>
+      <c r="BX14" s="160"/>
+      <c r="BY14" s="160"/>
+      <c r="BZ14" s="160"/>
+      <c r="CA14" s="160"/>
+      <c r="CB14" s="160"/>
+      <c r="CC14" s="160"/>
+      <c r="CD14" s="160"/>
+      <c r="CE14" s="160"/>
+      <c r="CF14" s="160"/>
+      <c r="CG14" s="160"/>
+      <c r="CH14" s="160"/>
+      <c r="CI14" s="160"/>
+      <c r="CJ14" s="160"/>
+      <c r="CK14" s="160"/>
+      <c r="CL14" s="160"/>
+      <c r="CM14" s="160"/>
+      <c r="CN14" s="160"/>
+      <c r="CO14" s="160"/>
+      <c r="CP14" s="160"/>
+      <c r="CQ14" s="160"/>
+      <c r="CR14" s="160"/>
+      <c r="CS14" s="160"/>
+      <c r="CT14" s="160"/>
+      <c r="CU14" s="160"/>
+      <c r="CV14" s="160"/>
+      <c r="CW14" s="160"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="172">
@@ -15790,9 +15790,9 @@
       <c r="E15" t="s" s="172">
         <v>56</v>
       </c>
-      <c r="F15" s="136"/>
-      <c r="G15" s="136"/>
-      <c r="H15" s="136"/>
+      <c r="F15" s="160"/>
+      <c r="G15" s="160"/>
+      <c r="H15" s="160"/>
       <c r="I15" s="861"/>
       <c r="J15" s="862"/>
       <c r="K15" s="863"/>
@@ -15842,50 +15842,50 @@
       <c r="BC15" s="593"/>
       <c r="BD15" s="594"/>
       <c r="BE15" s="595"/>
-      <c r="BF15" s="136"/>
-      <c r="BG15" s="136"/>
-      <c r="BH15" s="136"/>
-      <c r="BI15" s="136"/>
-      <c r="BJ15" s="136"/>
-      <c r="BK15" s="136"/>
-      <c r="BL15" s="136"/>
-      <c r="BM15" s="136"/>
-      <c r="BN15" s="136"/>
-      <c r="BO15" s="136"/>
-      <c r="BP15" s="136"/>
-      <c r="BQ15" s="136"/>
-      <c r="BR15" s="136"/>
-      <c r="BS15" s="136"/>
-      <c r="BT15" s="136"/>
-      <c r="BU15" s="136"/>
-      <c r="BV15" s="136"/>
-      <c r="BW15" s="136"/>
-      <c r="BX15" s="136"/>
-      <c r="BY15" s="136"/>
-      <c r="BZ15" s="136"/>
-      <c r="CA15" s="136"/>
-      <c r="CB15" s="136"/>
-      <c r="CC15" s="136"/>
-      <c r="CD15" s="136"/>
-      <c r="CE15" s="136"/>
-      <c r="CF15" s="136"/>
-      <c r="CG15" s="136"/>
-      <c r="CH15" s="136"/>
-      <c r="CI15" s="136"/>
-      <c r="CJ15" s="136"/>
-      <c r="CK15" s="136"/>
-      <c r="CL15" s="136"/>
-      <c r="CM15" s="136"/>
-      <c r="CN15" s="136"/>
-      <c r="CO15" s="136"/>
-      <c r="CP15" s="136"/>
-      <c r="CQ15" s="136"/>
-      <c r="CR15" s="136"/>
-      <c r="CS15" s="136"/>
-      <c r="CT15" s="136"/>
-      <c r="CU15" s="136"/>
-      <c r="CV15" s="136"/>
-      <c r="CW15" s="136"/>
+      <c r="BF15" s="160"/>
+      <c r="BG15" s="160"/>
+      <c r="BH15" s="160"/>
+      <c r="BI15" s="160"/>
+      <c r="BJ15" s="160"/>
+      <c r="BK15" s="160"/>
+      <c r="BL15" s="160"/>
+      <c r="BM15" s="160"/>
+      <c r="BN15" s="160"/>
+      <c r="BO15" s="160"/>
+      <c r="BP15" s="160"/>
+      <c r="BQ15" s="160"/>
+      <c r="BR15" s="160"/>
+      <c r="BS15" s="160"/>
+      <c r="BT15" s="160"/>
+      <c r="BU15" s="160"/>
+      <c r="BV15" s="160"/>
+      <c r="BW15" s="160"/>
+      <c r="BX15" s="160"/>
+      <c r="BY15" s="160"/>
+      <c r="BZ15" s="160"/>
+      <c r="CA15" s="160"/>
+      <c r="CB15" s="160"/>
+      <c r="CC15" s="160"/>
+      <c r="CD15" s="160"/>
+      <c r="CE15" s="160"/>
+      <c r="CF15" s="160"/>
+      <c r="CG15" s="160"/>
+      <c r="CH15" s="160"/>
+      <c r="CI15" s="160"/>
+      <c r="CJ15" s="160"/>
+      <c r="CK15" s="160"/>
+      <c r="CL15" s="160"/>
+      <c r="CM15" s="160"/>
+      <c r="CN15" s="160"/>
+      <c r="CO15" s="160"/>
+      <c r="CP15" s="160"/>
+      <c r="CQ15" s="160"/>
+      <c r="CR15" s="160"/>
+      <c r="CS15" s="160"/>
+      <c r="CT15" s="160"/>
+      <c r="CU15" s="160"/>
+      <c r="CV15" s="160"/>
+      <c r="CW15" s="160"/>
     </row>
   </sheetData>
   <mergeCells>

</xml_diff>